<commit_message>
Fund update as of january 07 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2018001\OneDrive - Banco Central de la Republica Dominicana\Desktop\Proyectos\goat_app\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Desktop/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="502" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{07BFC868-C1A4-4265-A7EA-76F456466191}"/>
+  <xr:revisionPtr revIDLastSave="536" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DB058DB-06CD-8049-8B7D-087A6DE66EAD}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="495" windowWidth="24720" windowHeight="17505" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="4" r:id="rId1"/>
@@ -18,25 +18,37 @@
     <sheet name="Ingreso" sheetId="1" r:id="rId3"/>
     <sheet name="Gastos" sheetId="2" r:id="rId4"/>
     <sheet name="Cuentas por cobrar" sheetId="6" r:id="rId5"/>
-    <sheet name="Otros depositos" sheetId="3" r:id="rId6"/>
+    <sheet name="Histórico de tecnicas" sheetId="7" r:id="rId6"/>
+    <sheet name="Otros depositos" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Ingreso!$A$1:$C$1</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="84">
   <si>
     <t>Row Labels</t>
   </si>
@@ -285,6 +297,9 @@
   </si>
   <si>
     <t>Sin detalle</t>
+  </si>
+  <si>
+    <t>Wilkin</t>
   </si>
 </sst>
 </file>
@@ -2928,16 +2943,16 @@
       <selection activeCell="P50" sqref="D50:P50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -3005,7 +3020,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -3045,7 +3060,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3073,7 +3088,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3122,7 +3137,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3150,7 +3165,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3165,7 +3180,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3195,7 +3210,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3212,7 +3227,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
@@ -3240,7 +3255,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
@@ -3267,7 +3282,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
@@ -3281,7 +3296,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
@@ -3309,7 +3324,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
@@ -3340,7 +3355,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
@@ -3392,7 +3407,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
@@ -3428,7 +3443,7 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
@@ -3474,7 +3489,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
@@ -3499,7 +3514,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
@@ -3513,7 +3528,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
@@ -3539,7 +3554,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
@@ -3561,7 +3576,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
@@ -3592,7 +3607,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
@@ -3606,7 +3621,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
@@ -3660,7 +3675,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
@@ -3688,7 +3703,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
@@ -3726,7 +3741,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
@@ -3768,7 +3783,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
@@ -3778,7 +3793,7 @@
       <c r="G29" s="3"/>
       <c r="W29" s="3"/>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
@@ -3793,7 +3808,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
@@ -3808,7 +3823,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
@@ -3823,7 +3838,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>30</v>
       </c>
@@ -3844,7 +3859,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>31</v>
       </c>
@@ -3859,7 +3874,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>32</v>
       </c>
@@ -3883,7 +3898,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>33</v>
       </c>
@@ -3898,7 +3913,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>34</v>
       </c>
@@ -3922,7 +3937,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>35</v>
       </c>
@@ -3943,7 +3958,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>36</v>
       </c>
@@ -3961,7 +3976,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>37</v>
       </c>
@@ -3976,7 +3991,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>38</v>
       </c>
@@ -3997,7 +4012,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>39</v>
       </c>
@@ -4015,7 +4030,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>40</v>
       </c>
@@ -4030,7 +4045,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>41</v>
       </c>
@@ -4048,7 +4063,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>42</v>
       </c>
@@ -4063,7 +4078,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>48</v>
       </c>
@@ -4078,7 +4093,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B47" s="7" t="s">
         <v>43</v>
       </c>
@@ -4144,7 +4159,7 @@
         <v>12055</v>
       </c>
     </row>
-    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B50" s="8" t="s">
         <v>44</v>
       </c>
@@ -4193,7 +4208,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B51" s="10" t="s">
         <v>45</v>
       </c>
@@ -4260,24 +4275,24 @@
       <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="5.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>46</v>
       </c>
@@ -4299,7 +4314,7 @@
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -4367,7 +4382,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -4405,7 +4420,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -4431,7 +4446,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -4478,7 +4493,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -4505,7 +4520,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -4517,7 +4532,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -4544,7 +4559,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -4559,7 +4574,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -4586,7 +4601,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -4613,7 +4628,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -4626,7 +4641,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -4653,7 +4668,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -4683,7 +4698,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -4734,7 +4749,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -4770,7 +4785,7 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -4815,7 +4830,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -4840,7 +4855,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -4853,7 +4868,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -4878,7 +4893,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -4899,7 +4914,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -4929,7 +4944,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -4942,7 +4957,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -4996,7 +5011,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -5024,7 +5039,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -5059,7 +5074,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -5102,7 +5117,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
@@ -5110,7 +5125,7 @@
       <c r="H30"/>
       <c r="V30" s="3"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -5123,7 +5138,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
@@ -5136,7 +5151,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
@@ -5149,7 +5164,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>30</v>
       </c>
@@ -5168,7 +5183,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -5181,7 +5196,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>32</v>
       </c>
@@ -5203,7 +5218,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>33</v>
       </c>
@@ -5216,7 +5231,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>34</v>
       </c>
@@ -5238,7 +5253,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -5257,7 +5272,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
@@ -5273,7 +5288,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
@@ -5286,7 +5301,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>38</v>
       </c>
@@ -5305,7 +5320,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>39</v>
       </c>
@@ -5321,7 +5336,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>40</v>
       </c>
@@ -5334,7 +5349,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
@@ -5350,7 +5365,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>42</v>
       </c>
@@ -5363,7 +5378,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -5376,7 +5391,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>43</v>
       </c>
@@ -5441,7 +5456,7 @@
         <v>12055</v>
       </c>
     </row>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -5450,20 +5465,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C202"/>
+  <dimension ref="A1:D226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="B186" sqref="B186"/>
+    <sheetView topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="A204" sqref="A204"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
@@ -5473,8 +5488,11 @@
       <c r="C1" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44710</v>
       </c>
@@ -5484,8 +5502,11 @@
       <c r="C2" s="3">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44724</v>
       </c>
@@ -5495,8 +5516,11 @@
       <c r="C3" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44724</v>
       </c>
@@ -5506,8 +5530,11 @@
       <c r="C4" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44724</v>
       </c>
@@ -5517,8 +5544,11 @@
       <c r="C5" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44724</v>
       </c>
@@ -5528,8 +5558,11 @@
       <c r="C6" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44724</v>
       </c>
@@ -5539,8 +5572,11 @@
       <c r="C7" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44724</v>
       </c>
@@ -5550,8 +5586,11 @@
       <c r="C8" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44724</v>
       </c>
@@ -5561,8 +5600,11 @@
       <c r="C9" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44724</v>
       </c>
@@ -5572,8 +5614,11 @@
       <c r="C10" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44724</v>
       </c>
@@ -5583,8 +5628,11 @@
       <c r="C11" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44724</v>
       </c>
@@ -5594,8 +5642,11 @@
       <c r="C12" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44724</v>
       </c>
@@ -5605,8 +5656,11 @@
       <c r="C13" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44724</v>
       </c>
@@ -5616,8 +5670,11 @@
       <c r="C14" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44724</v>
       </c>
@@ -5627,8 +5684,11 @@
       <c r="C15" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44724</v>
       </c>
@@ -5638,8 +5698,11 @@
       <c r="C16" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44724</v>
       </c>
@@ -5649,8 +5712,11 @@
       <c r="C17" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44731</v>
       </c>
@@ -5660,8 +5726,11 @@
       <c r="C18" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44731</v>
       </c>
@@ -5671,8 +5740,11 @@
       <c r="C19" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44731</v>
       </c>
@@ -5682,8 +5754,11 @@
       <c r="C20" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>44731</v>
       </c>
@@ -5693,8 +5768,11 @@
       <c r="C21" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>44731</v>
       </c>
@@ -5704,8 +5782,11 @@
       <c r="C22" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44731</v>
       </c>
@@ -5715,8 +5796,11 @@
       <c r="C23" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44731</v>
       </c>
@@ -5726,8 +5810,11 @@
       <c r="C24" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>44731</v>
       </c>
@@ -5737,8 +5824,11 @@
       <c r="C25" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44731</v>
       </c>
@@ -5748,8 +5838,11 @@
       <c r="C26" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>44731</v>
       </c>
@@ -5759,8 +5852,11 @@
       <c r="C27" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>44731</v>
       </c>
@@ -5770,8 +5866,11 @@
       <c r="C28" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>44731</v>
       </c>
@@ -5781,8 +5880,11 @@
       <c r="C29" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>44731</v>
       </c>
@@ -5792,8 +5894,11 @@
       <c r="C30" s="3">
         <v>65</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44738</v>
       </c>
@@ -5803,8 +5908,11 @@
       <c r="C31" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>44738</v>
       </c>
@@ -5814,8 +5922,11 @@
       <c r="C32" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>44738</v>
       </c>
@@ -5825,8 +5936,11 @@
       <c r="C33" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>44738</v>
       </c>
@@ -5836,8 +5950,11 @@
       <c r="C34" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>44738</v>
       </c>
@@ -5847,8 +5964,11 @@
       <c r="C35" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44738</v>
       </c>
@@ -5858,8 +5978,11 @@
       <c r="C36" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>44738</v>
       </c>
@@ -5869,8 +5992,11 @@
       <c r="C37" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>44738</v>
       </c>
@@ -5880,8 +6006,11 @@
       <c r="C38" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>44738</v>
       </c>
@@ -5891,8 +6020,11 @@
       <c r="C39" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44738</v>
       </c>
@@ -5902,8 +6034,11 @@
       <c r="C40" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>44738</v>
       </c>
@@ -5913,8 +6048,11 @@
       <c r="C41" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>44738</v>
       </c>
@@ -5924,8 +6062,11 @@
       <c r="C42" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>44738</v>
       </c>
@@ -5935,8 +6076,11 @@
       <c r="C43" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>44738</v>
       </c>
@@ -5946,8 +6090,11 @@
       <c r="C44" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44738</v>
       </c>
@@ -5957,8 +6104,11 @@
       <c r="C45" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>44752</v>
       </c>
@@ -5968,8 +6118,11 @@
       <c r="C46" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>44752</v>
       </c>
@@ -5979,8 +6132,11 @@
       <c r="C47" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>44752</v>
       </c>
@@ -5990,8 +6146,11 @@
       <c r="C48" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>44752</v>
       </c>
@@ -6001,8 +6160,11 @@
       <c r="C49" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>44752</v>
       </c>
@@ -6012,8 +6174,11 @@
       <c r="C50" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>44752</v>
       </c>
@@ -6023,8 +6188,11 @@
       <c r="C51" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>44752</v>
       </c>
@@ -6034,8 +6202,11 @@
       <c r="C52" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>44752</v>
       </c>
@@ -6045,8 +6216,11 @@
       <c r="C53" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>44752</v>
       </c>
@@ -6056,8 +6230,11 @@
       <c r="C54" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>44752</v>
       </c>
@@ -6067,8 +6244,11 @@
       <c r="C55" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>44752</v>
       </c>
@@ -6078,8 +6258,11 @@
       <c r="C56" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>44752</v>
       </c>
@@ -6089,8 +6272,11 @@
       <c r="C57" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>44752</v>
       </c>
@@ -6100,8 +6286,11 @@
       <c r="C58" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>44766</v>
       </c>
@@ -6111,8 +6300,11 @@
       <c r="C59" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>44766</v>
       </c>
@@ -6122,8 +6314,11 @@
       <c r="C60" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>44766</v>
       </c>
@@ -6133,8 +6328,11 @@
       <c r="C61" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>44766</v>
       </c>
@@ -6144,8 +6342,11 @@
       <c r="C62" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>44766</v>
       </c>
@@ -6155,8 +6356,11 @@
       <c r="C63" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>44766</v>
       </c>
@@ -6166,8 +6370,11 @@
       <c r="C64" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>44766</v>
       </c>
@@ -6177,8 +6384,11 @@
       <c r="C65" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>44766</v>
       </c>
@@ -6188,8 +6398,11 @@
       <c r="C66" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>44766</v>
       </c>
@@ -6199,8 +6412,11 @@
       <c r="C67" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>44787</v>
       </c>
@@ -6210,8 +6426,11 @@
       <c r="C68" s="3">
         <v>150</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>44795</v>
       </c>
@@ -6221,8 +6440,11 @@
       <c r="C69" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>44795</v>
       </c>
@@ -6232,8 +6454,11 @@
       <c r="C70" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>44795</v>
       </c>
@@ -6243,8 +6468,11 @@
       <c r="C71" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>44795</v>
       </c>
@@ -6254,8 +6482,11 @@
       <c r="C72" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>44795</v>
       </c>
@@ -6265,8 +6496,11 @@
       <c r="C73" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>44795</v>
       </c>
@@ -6276,8 +6510,11 @@
       <c r="C74" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>44815</v>
       </c>
@@ -6287,8 +6524,11 @@
       <c r="C75" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>44815</v>
       </c>
@@ -6298,8 +6538,11 @@
       <c r="C76" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>44815</v>
       </c>
@@ -6309,8 +6552,11 @@
       <c r="C77" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>44815</v>
       </c>
@@ -6320,8 +6566,11 @@
       <c r="C78" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>44815</v>
       </c>
@@ -6331,8 +6580,11 @@
       <c r="C79" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>44815</v>
       </c>
@@ -6342,8 +6594,11 @@
       <c r="C80" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>44815</v>
       </c>
@@ -6353,8 +6608,11 @@
       <c r="C81" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>44815</v>
       </c>
@@ -6364,8 +6622,11 @@
       <c r="C82" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>44815</v>
       </c>
@@ -6375,8 +6636,11 @@
       <c r="C83" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>44815</v>
       </c>
@@ -6386,8 +6650,11 @@
       <c r="C84" s="3">
         <v>35</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>44843</v>
       </c>
@@ -6397,8 +6664,11 @@
       <c r="C85" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>44843</v>
       </c>
@@ -6408,8 +6678,11 @@
       <c r="C86" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>44843</v>
       </c>
@@ -6419,8 +6692,11 @@
       <c r="C87" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>44843</v>
       </c>
@@ -6430,8 +6706,11 @@
       <c r="C88" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>44843</v>
       </c>
@@ -6441,8 +6720,11 @@
       <c r="C89" s="3">
         <v>35</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>44843</v>
       </c>
@@ -6452,8 +6734,11 @@
       <c r="C90" s="3">
         <v>45</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>44843</v>
       </c>
@@ -6463,8 +6748,11 @@
       <c r="C91" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>44843</v>
       </c>
@@ -6474,8 +6762,11 @@
       <c r="C92" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>44843</v>
       </c>
@@ -6485,8 +6776,11 @@
       <c r="C93" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>44843</v>
       </c>
@@ -6496,8 +6790,11 @@
       <c r="C94" s="3">
         <v>550</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>44843</v>
       </c>
@@ -6507,8 +6804,11 @@
       <c r="C95" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>44843</v>
       </c>
@@ -6518,8 +6818,11 @@
       <c r="C96" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>44843</v>
       </c>
@@ -6529,8 +6832,11 @@
       <c r="C97" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>44843</v>
       </c>
@@ -6540,8 +6846,11 @@
       <c r="C98" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>44843</v>
       </c>
@@ -6551,8 +6860,11 @@
       <c r="C99" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>44843</v>
       </c>
@@ -6562,8 +6874,11 @@
       <c r="C100" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>44843</v>
       </c>
@@ -6573,8 +6888,11 @@
       <c r="C101" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>44850</v>
       </c>
@@ -6584,8 +6902,11 @@
       <c r="C102" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>44850</v>
       </c>
@@ -6595,8 +6916,11 @@
       <c r="C103" s="3">
         <v>75</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>44850</v>
       </c>
@@ -6606,8 +6930,11 @@
       <c r="C104" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>44850</v>
       </c>
@@ -6617,8 +6944,11 @@
       <c r="C105" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>44850</v>
       </c>
@@ -6628,8 +6958,11 @@
       <c r="C106" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>44850</v>
       </c>
@@ -6639,8 +6972,11 @@
       <c r="C107" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>44850</v>
       </c>
@@ -6650,8 +6986,11 @@
       <c r="C108" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>44857</v>
       </c>
@@ -6661,8 +7000,11 @@
       <c r="C109" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>44857</v>
       </c>
@@ -6672,8 +7014,11 @@
       <c r="C110" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>44857</v>
       </c>
@@ -6683,8 +7028,11 @@
       <c r="C111" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>44857</v>
       </c>
@@ -6694,8 +7042,11 @@
       <c r="C112" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>44857</v>
       </c>
@@ -6705,8 +7056,11 @@
       <c r="C113" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>44857</v>
       </c>
@@ -6716,8 +7070,11 @@
       <c r="C114" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>44857</v>
       </c>
@@ -6727,8 +7084,11 @@
       <c r="C115" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>44857</v>
       </c>
@@ -6738,8 +7098,11 @@
       <c r="C116" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>44857</v>
       </c>
@@ -6749,8 +7112,11 @@
       <c r="C117" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>44857</v>
       </c>
@@ -6760,8 +7126,11 @@
       <c r="C118" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D118" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>44857</v>
       </c>
@@ -6771,8 +7140,11 @@
       <c r="C119" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>44864</v>
       </c>
@@ -6782,8 +7154,11 @@
       <c r="C120" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D120" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>44864</v>
       </c>
@@ -6793,8 +7168,11 @@
       <c r="C121" s="3">
         <v>45</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D121" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>44864</v>
       </c>
@@ -6804,8 +7182,11 @@
       <c r="C122" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D122" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>44864</v>
       </c>
@@ -6815,8 +7196,11 @@
       <c r="C123" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>44864</v>
       </c>
@@ -6826,8 +7210,11 @@
       <c r="C124" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D124" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>44864</v>
       </c>
@@ -6837,8 +7224,11 @@
       <c r="C125" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D125" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>44864</v>
       </c>
@@ -6848,8 +7238,11 @@
       <c r="C126" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D126" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>44871</v>
       </c>
@@ -6859,8 +7252,11 @@
       <c r="C127" s="3">
         <v>40</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D127" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>44871</v>
       </c>
@@ -6870,8 +7266,11 @@
       <c r="C128" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D128" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>44871</v>
       </c>
@@ -6881,8 +7280,11 @@
       <c r="C129" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D129" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>44871</v>
       </c>
@@ -6892,8 +7294,11 @@
       <c r="C130" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D130" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>44871</v>
       </c>
@@ -6903,8 +7308,11 @@
       <c r="C131" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D131" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>44871</v>
       </c>
@@ -6914,8 +7322,11 @@
       <c r="C132" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D132" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>44871</v>
       </c>
@@ -6925,8 +7336,11 @@
       <c r="C133" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D133" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>44871</v>
       </c>
@@ -6936,8 +7350,11 @@
       <c r="C134" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D134" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>44871</v>
       </c>
@@ -6947,8 +7364,11 @@
       <c r="C135" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D135" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>44871</v>
       </c>
@@ -6958,8 +7378,11 @@
       <c r="C136" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D136" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
         <v>44871</v>
       </c>
@@ -6969,8 +7392,11 @@
       <c r="C137" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D137" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>44871</v>
       </c>
@@ -6980,8 +7406,11 @@
       <c r="C138" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D138" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
         <v>44871</v>
       </c>
@@ -6991,8 +7420,11 @@
       <c r="C139" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D139" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>44871</v>
       </c>
@@ -7002,8 +7434,11 @@
       <c r="C140" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D140" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
         <v>44878</v>
       </c>
@@ -7013,8 +7448,11 @@
       <c r="C141" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D141" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
         <v>44878</v>
       </c>
@@ -7024,8 +7462,11 @@
       <c r="C142" s="3">
         <v>35</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D142" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
         <v>44878</v>
       </c>
@@ -7035,8 +7476,11 @@
       <c r="C143" s="3">
         <v>35</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D143" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
         <v>44878</v>
       </c>
@@ -7046,8 +7490,11 @@
       <c r="C144" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D144" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <v>44878</v>
       </c>
@@ -7057,8 +7504,11 @@
       <c r="C145" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D145" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>44878</v>
       </c>
@@ -7068,8 +7518,11 @@
       <c r="C146" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D146" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
         <v>44878</v>
       </c>
@@ -7079,8 +7532,11 @@
       <c r="C147" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D147" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
         <v>44878</v>
       </c>
@@ -7090,8 +7546,11 @@
       <c r="C148" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D148" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
         <v>44878</v>
       </c>
@@ -7101,8 +7560,11 @@
       <c r="C149" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D149" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <v>44878</v>
       </c>
@@ -7112,8 +7574,11 @@
       <c r="C150" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D150" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
         <v>44878</v>
       </c>
@@ -7123,8 +7588,11 @@
       <c r="C151" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D151" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
         <v>44892</v>
       </c>
@@ -7134,8 +7602,11 @@
       <c r="C152" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D152" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
         <v>44892</v>
       </c>
@@ -7145,8 +7616,11 @@
       <c r="C153" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D153" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <v>44892</v>
       </c>
@@ -7156,8 +7630,11 @@
       <c r="C154" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D154" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
         <v>44892</v>
       </c>
@@ -7167,8 +7644,11 @@
       <c r="C155" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D155" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
         <v>44892</v>
       </c>
@@ -7178,8 +7658,11 @@
       <c r="C156" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D156" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
         <v>44899</v>
       </c>
@@ -7189,8 +7672,11 @@
       <c r="C157" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D157" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
         <v>44899</v>
       </c>
@@ -7200,8 +7686,11 @@
       <c r="C158" s="3">
         <v>35</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D158" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
         <v>44899</v>
       </c>
@@ -7211,8 +7700,11 @@
       <c r="C159" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D159" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
         <v>44899</v>
       </c>
@@ -7222,8 +7714,11 @@
       <c r="C160" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D160" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
         <v>44899</v>
       </c>
@@ -7233,8 +7728,11 @@
       <c r="C161" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D161" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
         <v>44899</v>
       </c>
@@ -7244,8 +7742,11 @@
       <c r="C162" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D162" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
         <v>44899</v>
       </c>
@@ -7255,8 +7756,11 @@
       <c r="C163" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D163" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
         <v>44899</v>
       </c>
@@ -7266,8 +7770,11 @@
       <c r="C164" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D164" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
         <v>44899</v>
       </c>
@@ -7277,8 +7784,11 @@
       <c r="C165" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D165" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
         <v>44899</v>
       </c>
@@ -7288,8 +7798,11 @@
       <c r="C166" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D166" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="2">
         <v>44899</v>
       </c>
@@ -7299,8 +7812,11 @@
       <c r="C167" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D167" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
         <v>44899</v>
       </c>
@@ -7310,8 +7826,11 @@
       <c r="C168" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D168" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" s="2">
         <v>44899</v>
       </c>
@@ -7321,8 +7840,11 @@
       <c r="C169" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D169" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
         <v>44906</v>
       </c>
@@ -7332,8 +7854,11 @@
       <c r="C170" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D170" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="2">
         <v>44906</v>
       </c>
@@ -7343,8 +7868,11 @@
       <c r="C171" s="3">
         <v>200</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D171" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
         <v>44906</v>
       </c>
@@ -7354,8 +7882,11 @@
       <c r="C172" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D172" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="2">
         <v>44906</v>
       </c>
@@ -7365,8 +7896,11 @@
       <c r="C173" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D173" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
         <v>44906</v>
       </c>
@@ -7376,8 +7910,11 @@
       <c r="C174" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D174" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" s="2">
         <v>44906</v>
       </c>
@@ -7387,8 +7924,11 @@
       <c r="C175" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D175" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
         <v>44906</v>
       </c>
@@ -7398,8 +7938,11 @@
       <c r="C176" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D176" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" s="2">
         <v>44906</v>
       </c>
@@ -7409,8 +7952,11 @@
       <c r="C177" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D177" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" s="2">
         <v>44906</v>
       </c>
@@ -7420,8 +7966,11 @@
       <c r="C178" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D178" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
         <v>44906</v>
       </c>
@@ -7431,8 +7980,11 @@
       <c r="C179" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D179" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" s="2">
         <v>44906</v>
       </c>
@@ -7442,8 +7994,11 @@
       <c r="C180" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D180" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="2">
         <v>44906</v>
       </c>
@@ -7453,8 +8008,11 @@
       <c r="C181" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D181" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
         <v>44906</v>
       </c>
@@ -7464,8 +8022,11 @@
       <c r="C182" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D182" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" s="2">
         <v>44906</v>
       </c>
@@ -7475,8 +8036,11 @@
       <c r="C183" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D183" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
         <v>44906</v>
       </c>
@@ -7486,8 +8050,11 @@
       <c r="C184" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D184" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="2">
         <v>44906</v>
       </c>
@@ -7497,8 +8064,11 @@
       <c r="C185" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D185" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
         <v>44906</v>
       </c>
@@ -7508,8 +8078,11 @@
       <c r="C186" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D186" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="2">
         <v>44913</v>
       </c>
@@ -7519,8 +8092,11 @@
       <c r="C187" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D187" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
         <v>44913</v>
       </c>
@@ -7530,8 +8106,11 @@
       <c r="C188" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D188" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="2">
         <v>44913</v>
       </c>
@@ -7541,8 +8120,11 @@
       <c r="C189" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D189" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" s="2">
         <v>44913</v>
       </c>
@@ -7552,8 +8134,11 @@
       <c r="C190" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D190" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" s="2">
         <v>44913</v>
       </c>
@@ -7563,8 +8148,11 @@
       <c r="C191" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D191" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" s="2">
         <v>44913</v>
       </c>
@@ -7574,8 +8162,11 @@
       <c r="C192" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D192" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" s="2">
         <v>44913</v>
       </c>
@@ -7585,8 +8176,11 @@
       <c r="C193" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D193" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
         <v>44913</v>
       </c>
@@ -7596,8 +8190,11 @@
       <c r="C194" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D194" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="2">
         <v>44913</v>
       </c>
@@ -7607,8 +8204,11 @@
       <c r="C195" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D195" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="2">
         <v>44913</v>
       </c>
@@ -7618,8 +8218,11 @@
       <c r="C196" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D196" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" s="2">
         <v>44913</v>
       </c>
@@ -7629,8 +8232,11 @@
       <c r="C197" s="3">
         <v>35</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D197" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="2">
         <v>44913</v>
       </c>
@@ -7640,8 +8246,11 @@
       <c r="C198" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D198" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" s="2">
         <v>44913</v>
       </c>
@@ -7651,8 +8260,11 @@
       <c r="C199" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D199" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="2">
         <v>44913</v>
       </c>
@@ -7662,8 +8274,11 @@
       <c r="C200" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D200" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" s="2">
         <v>44913</v>
       </c>
@@ -7673,8 +8288,11 @@
       <c r="C201" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D201" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" s="2">
         <v>44913</v>
       </c>
@@ -7684,13 +8302,347 @@
       <c r="C202" s="3">
         <v>150</v>
       </c>
+      <c r="D202" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B203" t="s">
+        <v>38</v>
+      </c>
+      <c r="C203">
+        <v>50</v>
+      </c>
+      <c r="D203" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B204" t="s">
+        <v>3</v>
+      </c>
+      <c r="C204">
+        <v>200</v>
+      </c>
+      <c r="D204" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B205" t="s">
+        <v>4</v>
+      </c>
+      <c r="C205">
+        <v>0</v>
+      </c>
+      <c r="D205" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B206" t="s">
+        <v>13</v>
+      </c>
+      <c r="C206">
+        <v>50</v>
+      </c>
+      <c r="D206" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B207" t="s">
+        <v>16</v>
+      </c>
+      <c r="C207">
+        <v>50</v>
+      </c>
+      <c r="D207" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B208" t="s">
+        <v>1</v>
+      </c>
+      <c r="C208">
+        <v>100</v>
+      </c>
+      <c r="D208" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A209" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B209" t="s">
+        <v>83</v>
+      </c>
+      <c r="C209">
+        <v>50</v>
+      </c>
+      <c r="D209" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A210" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B210" t="s">
+        <v>15</v>
+      </c>
+      <c r="C210">
+        <v>100</v>
+      </c>
+      <c r="D210" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A211" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B211" t="s">
+        <v>22</v>
+      </c>
+      <c r="C211">
+        <v>50</v>
+      </c>
+      <c r="D211" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A212" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B212" t="s">
+        <v>24</v>
+      </c>
+      <c r="C212">
+        <v>100</v>
+      </c>
+      <c r="D212" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A213" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B213" t="s">
+        <v>20</v>
+      </c>
+      <c r="C213">
+        <v>50</v>
+      </c>
+      <c r="D213" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A214" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B214" t="s">
+        <v>2</v>
+      </c>
+      <c r="C214">
+        <v>100</v>
+      </c>
+      <c r="D214" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B215" t="s">
+        <v>28</v>
+      </c>
+      <c r="C215">
+        <v>50</v>
+      </c>
+      <c r="D215" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A216" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B216" t="s">
+        <v>14</v>
+      </c>
+      <c r="C216">
+        <v>100</v>
+      </c>
+      <c r="D216" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A217" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B217" t="s">
+        <v>35</v>
+      </c>
+      <c r="C217">
+        <v>50</v>
+      </c>
+      <c r="D217" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A218" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B218" t="s">
+        <v>25</v>
+      </c>
+      <c r="C218">
+        <v>100</v>
+      </c>
+      <c r="D218" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A219" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B219" t="s">
+        <v>34</v>
+      </c>
+      <c r="C219">
+        <v>0</v>
+      </c>
+      <c r="D219" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A220" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B220" t="s">
+        <v>12</v>
+      </c>
+      <c r="C220">
+        <v>50</v>
+      </c>
+      <c r="D220" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A221" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B221" t="s">
+        <v>29</v>
+      </c>
+      <c r="C221">
+        <v>15</v>
+      </c>
+      <c r="D221" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A222" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B222" t="s">
+        <v>41</v>
+      </c>
+      <c r="C222">
+        <v>100</v>
+      </c>
+      <c r="D222" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A223" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B223" t="s">
+        <v>16</v>
+      </c>
+      <c r="C223">
+        <v>200</v>
+      </c>
+      <c r="D223" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A224" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B224" t="s">
+        <v>30</v>
+      </c>
+      <c r="C224">
+        <v>100</v>
+      </c>
+      <c r="D224" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A225" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B225" t="s">
+        <v>11</v>
+      </c>
+      <c r="C225">
+        <v>100</v>
+      </c>
+      <c r="D225" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A226" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B226" t="s">
+        <v>20</v>
+      </c>
+      <c r="C226" s="3">
+        <v>100</v>
+      </c>
+      <c r="D226" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState ref="A2:C202">
-      <sortCondition ref="A1:A202"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -7698,19 +8650,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
@@ -7721,7 +8673,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44710</v>
       </c>
@@ -7732,7 +8684,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44724</v>
       </c>
@@ -7743,7 +8695,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44731</v>
       </c>
@@ -7754,7 +8706,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44738</v>
       </c>
@@ -7765,7 +8717,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44752</v>
       </c>
@@ -7776,7 +8728,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44766</v>
       </c>
@@ -7787,7 +8739,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44795</v>
       </c>
@@ -7798,7 +8750,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44815</v>
       </c>
@@ -7809,7 +8761,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44843</v>
       </c>
@@ -7820,7 +8772,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44857</v>
       </c>
@@ -7831,7 +8783,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44857</v>
       </c>
@@ -7842,7 +8794,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44899</v>
       </c>
@@ -7853,7 +8805,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44892</v>
       </c>
@@ -7864,7 +8816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44878</v>
       </c>
@@ -7875,7 +8827,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44906</v>
       </c>
@@ -7886,7 +8838,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44913</v>
       </c>
@@ -7897,7 +8849,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44911</v>
       </c>
@@ -7906,6 +8858,17 @@
       </c>
       <c r="C18">
         <v>1500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19">
+        <v>940</v>
       </c>
     </row>
   </sheetData>
@@ -7919,15 +8882,15 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -7944,33 +8907,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>44906</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>44913</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="12"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7978,6 +8919,89 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE771D5-AE0E-9C4B-B862-1B8092D29603}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="12">
+        <v>44906</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="12">
+        <v>44913</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="12">
+        <v>44933</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2D107B-4260-4C0E-BE4E-10DAADFBD61E}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -7985,9 +9009,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update 15 jan 2022
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Desktop/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="536" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DB058DB-06CD-8049-8B7D-087A6DE66EAD}"/>
+  <xr:revisionPtr revIDLastSave="555" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A354207E-86B2-4142-BC1B-DC92A75A1B0D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8400" yWindow="1960" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="84">
   <si>
     <t>Row Labels</t>
   </si>
@@ -429,7 +429,17 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="right"/>
     </dxf>
@@ -1969,7 +1979,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C69D9E15-FF2B-403E-8037-8C1EF734B27A}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C69D9E15-FF2B-403E-8037-8C1EF734B27A}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:V48" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisCol" showAll="0">
@@ -2626,7 +2636,7 @@
     <dataField name="Sum of Aporte" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="4">
+    <format dxfId="5">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="5" selected="0">
@@ -2639,13 +2649,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="4">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="3">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="5">
@@ -2658,7 +2668,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -5465,10 +5475,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D226"/>
+  <dimension ref="A1:D244"/>
   <sheetViews>
-    <sheetView topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="A204" sqref="A204"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6169,7 +6179,7 @@
         <v>44752</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C50" s="3">
         <v>25</v>
@@ -7079,7 +7089,7 @@
         <v>44857</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C115" s="3">
         <v>25</v>
@@ -7835,7 +7845,7 @@
         <v>44899</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C169" s="3">
         <v>100</v>
@@ -7947,7 +7957,7 @@
         <v>44906</v>
       </c>
       <c r="B177" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="C177" s="3">
         <v>100</v>
@@ -8642,7 +8652,262 @@
         <v>61</v>
       </c>
     </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B227" t="s">
+        <v>20</v>
+      </c>
+      <c r="C227">
+        <v>50</v>
+      </c>
+      <c r="D227" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A228" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B228" t="s">
+        <v>15</v>
+      </c>
+      <c r="C228">
+        <v>200</v>
+      </c>
+      <c r="D228" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A229" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B229" t="s">
+        <v>1</v>
+      </c>
+      <c r="C229">
+        <v>100</v>
+      </c>
+      <c r="D229" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A230" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B230" t="s">
+        <v>9</v>
+      </c>
+      <c r="C230">
+        <v>100</v>
+      </c>
+      <c r="D230" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A231" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B231" t="s">
+        <v>13</v>
+      </c>
+      <c r="C231">
+        <v>50</v>
+      </c>
+      <c r="D231" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B232" t="s">
+        <v>14</v>
+      </c>
+      <c r="C232">
+        <v>100</v>
+      </c>
+      <c r="D232" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A233" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B233" t="s">
+        <v>35</v>
+      </c>
+      <c r="C233">
+        <v>50</v>
+      </c>
+      <c r="D233" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B234" t="s">
+        <v>24</v>
+      </c>
+      <c r="C234">
+        <v>50</v>
+      </c>
+      <c r="D234" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B235" t="s">
+        <v>34</v>
+      </c>
+      <c r="C235">
+        <v>50</v>
+      </c>
+      <c r="D235" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A236" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B236" t="s">
+        <v>4</v>
+      </c>
+      <c r="C236">
+        <v>300</v>
+      </c>
+      <c r="D236" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A237" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B237" t="s">
+        <v>40</v>
+      </c>
+      <c r="C237">
+        <v>50</v>
+      </c>
+      <c r="D237" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A238" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B238" t="s">
+        <v>36</v>
+      </c>
+      <c r="C238">
+        <v>50</v>
+      </c>
+      <c r="D238" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A239" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B239" t="s">
+        <v>12</v>
+      </c>
+      <c r="C239">
+        <v>50</v>
+      </c>
+      <c r="D239" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A240" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B240" t="s">
+        <v>22</v>
+      </c>
+      <c r="C240">
+        <v>50</v>
+      </c>
+      <c r="D240" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A241" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B241" t="s">
+        <v>16</v>
+      </c>
+      <c r="C241">
+        <v>50</v>
+      </c>
+      <c r="D241" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A242" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B242" t="s">
+        <v>83</v>
+      </c>
+      <c r="C242">
+        <v>100</v>
+      </c>
+      <c r="D242" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A243" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B243" t="s">
+        <v>32</v>
+      </c>
+      <c r="C243">
+        <v>40</v>
+      </c>
+      <c r="D243" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A244" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B244" t="s">
+        <v>25</v>
+      </c>
+      <c r="C244">
+        <v>50</v>
+      </c>
+      <c r="D244" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -8650,10 +8915,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8869,6 +9134,17 @@
       </c>
       <c r="C19">
         <v>940</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20">
+        <v>950</v>
       </c>
     </row>
   </sheetData>
@@ -8922,7 +9198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE771D5-AE0E-9C4B-B862-1B8092D29603}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ajuste aportes del chamo
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Desktop/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="597" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B9F5DEE-3C89-8144-A44E-189D46146E32}"/>
+  <xr:revisionPtr revIDLastSave="598" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3903127B-6CB4-D64B-B932-39509BCA243F}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5488,8 +5488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
+      <selection activeCell="C237" sqref="C237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8797,7 +8797,7 @@
         <v>4</v>
       </c>
       <c r="C236">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="D236" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
Update 05 Feb 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Desktop/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="598" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3903127B-6CB4-D64B-B932-39509BCA243F}"/>
+  <xr:revisionPtr revIDLastSave="615" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57F32451-E7D1-CA4F-8909-58F35EE82BFE}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="86">
   <si>
     <t>Row Labels</t>
   </si>
@@ -316,7 +316,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -431,10 +431,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -5486,10 +5486,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D276"/>
+  <dimension ref="A1:D291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
-      <selection activeCell="C237" sqref="C237"/>
+    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
+      <selection activeCell="G287" sqref="G287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9363,9 +9363,219 @@
         <v>51</v>
       </c>
     </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A277" s="2">
+        <v>44948</v>
+      </c>
+      <c r="B277" t="s">
+        <v>16</v>
+      </c>
+      <c r="C277" s="3">
+        <v>300</v>
+      </c>
+      <c r="D277" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A278" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B278" t="s">
+        <v>32</v>
+      </c>
+      <c r="C278">
+        <v>50</v>
+      </c>
+      <c r="D278" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A279" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B279" t="s">
+        <v>18</v>
+      </c>
+      <c r="C279">
+        <v>100</v>
+      </c>
+      <c r="D279" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A280" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B280" t="s">
+        <v>1</v>
+      </c>
+      <c r="C280">
+        <v>45</v>
+      </c>
+      <c r="D280" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A281" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B281" t="s">
+        <v>2</v>
+      </c>
+      <c r="C281">
+        <v>100</v>
+      </c>
+      <c r="D281" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A282" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B282" t="s">
+        <v>12</v>
+      </c>
+      <c r="C282">
+        <v>300</v>
+      </c>
+      <c r="D282" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A283" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B283" t="s">
+        <v>20</v>
+      </c>
+      <c r="C283">
+        <v>100</v>
+      </c>
+      <c r="D283" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A284" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B284" t="s">
+        <v>14</v>
+      </c>
+      <c r="C284">
+        <v>300</v>
+      </c>
+      <c r="D284" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A285" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B285" t="s">
+        <v>23</v>
+      </c>
+      <c r="C285">
+        <v>100</v>
+      </c>
+      <c r="D285" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A286" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B286" t="s">
+        <v>9</v>
+      </c>
+      <c r="C286">
+        <v>100</v>
+      </c>
+      <c r="D286" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A287" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B287" t="s">
+        <v>22</v>
+      </c>
+      <c r="C287">
+        <v>50</v>
+      </c>
+      <c r="D287" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A288" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B288" t="s">
+        <v>11</v>
+      </c>
+      <c r="C288">
+        <v>50</v>
+      </c>
+      <c r="D288" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A289" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B289" t="s">
+        <v>3</v>
+      </c>
+      <c r="C289">
+        <v>100</v>
+      </c>
+      <c r="D289" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A290" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B290" t="s">
+        <v>15</v>
+      </c>
+      <c r="C290">
+        <v>300</v>
+      </c>
+      <c r="D290" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A291" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B291" t="s">
+        <v>16</v>
+      </c>
+      <c r="C291">
+        <v>300</v>
+      </c>
+      <c r="D291" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9374,10 +9584,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9627,6 +9837,17 @@
       </c>
       <c r="C22" s="16">
         <v>3775</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="16">
+        <v>940</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mes actual y anterior
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Desktop/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="615" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57F32451-E7D1-CA4F-8909-58F35EE82BFE}"/>
+  <xr:revisionPtr revIDLastSave="616" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7C3C499-598F-7B40-8757-9F582ECA458D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="86">
   <si>
     <t>Row Labels</t>
   </si>
@@ -1990,7 +1990,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C69D9E15-FF2B-403E-8037-8C1EF734B27A}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C69D9E15-FF2B-403E-8037-8C1EF734B27A}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:V48" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisCol" showAll="0">
@@ -5488,8 +5488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
-      <selection activeCell="G287" sqref="G287"/>
+    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
+      <selection activeCell="A278" sqref="A278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9560,18 +9560,7 @@
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A291" s="2">
-        <v>44962</v>
-      </c>
-      <c r="B291" t="s">
-        <v>16</v>
-      </c>
-      <c r="C291">
-        <v>300</v>
-      </c>
-      <c r="D291" t="s">
-        <v>51</v>
-      </c>
+      <c r="C291"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
Aporte al 12 de febrero 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Desktop/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="621" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D7BF224-EE26-554E-A915-8006C98DF232}"/>
+  <xr:revisionPtr revIDLastSave="656" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2AEA503-6F9A-4541-B95E-F860A7CF8F88}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="10000" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="87">
   <si>
     <t>Row Labels</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>Pelota, Mallas y bomba</t>
+  </si>
+  <si>
+    <t>julio</t>
   </si>
 </sst>
 </file>
@@ -1990,7 +1993,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C69D9E15-FF2B-403E-8037-8C1EF734B27A}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C69D9E15-FF2B-403E-8037-8C1EF734B27A}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:V48" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisCol" showAll="0">
@@ -5486,10 +5489,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D292"/>
+  <dimension ref="A1:D304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="A264" sqref="A264"/>
+    <sheetView topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="A294" sqref="A294:A304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9183,13 +9186,13 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" s="2">
-        <v>44948</v>
+        <v>44956</v>
       </c>
       <c r="B264" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C264">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="D264" t="s">
         <v>51</v>
@@ -9200,7 +9203,7 @@
         <v>44948</v>
       </c>
       <c r="B265" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C265">
         <v>50</v>
@@ -9214,10 +9217,10 @@
         <v>44948</v>
       </c>
       <c r="B266" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C266">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D266" t="s">
         <v>51</v>
@@ -9228,10 +9231,10 @@
         <v>44948</v>
       </c>
       <c r="B267" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C267">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D267" t="s">
         <v>51</v>
@@ -9242,10 +9245,10 @@
         <v>44948</v>
       </c>
       <c r="B268" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C268">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D268" t="s">
         <v>51</v>
@@ -9256,10 +9259,10 @@
         <v>44948</v>
       </c>
       <c r="B269" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C269">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D269" t="s">
         <v>51</v>
@@ -9270,7 +9273,7 @@
         <v>44948</v>
       </c>
       <c r="B270" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C270">
         <v>50</v>
@@ -9284,10 +9287,10 @@
         <v>44948</v>
       </c>
       <c r="B271" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C271">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D271" t="s">
         <v>51</v>
@@ -9298,7 +9301,7 @@
         <v>44948</v>
       </c>
       <c r="B272" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C272">
         <v>0</v>
@@ -9312,7 +9315,7 @@
         <v>44948</v>
       </c>
       <c r="B273" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C273">
         <v>0</v>
@@ -9326,10 +9329,10 @@
         <v>44948</v>
       </c>
       <c r="B274" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C274">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D274" t="s">
         <v>51</v>
@@ -9340,7 +9343,7 @@
         <v>44948</v>
       </c>
       <c r="B275" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C275">
         <v>50</v>
@@ -9354,7 +9357,7 @@
         <v>44948</v>
       </c>
       <c r="B276" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C276">
         <v>50</v>
@@ -9368,10 +9371,10 @@
         <v>44948</v>
       </c>
       <c r="B277" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C277">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D277" t="s">
         <v>51</v>
@@ -9382,10 +9385,10 @@
         <v>44948</v>
       </c>
       <c r="B278" t="s">
-        <v>16</v>
-      </c>
-      <c r="C278" s="3">
-        <v>300</v>
+        <v>11</v>
+      </c>
+      <c r="C278">
+        <v>100</v>
       </c>
       <c r="D278" t="s">
         <v>51</v>
@@ -9393,13 +9396,13 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" s="2">
-        <v>44962</v>
+        <v>44948</v>
       </c>
       <c r="B279" t="s">
-        <v>32</v>
-      </c>
-      <c r="C279">
-        <v>50</v>
+        <v>16</v>
+      </c>
+      <c r="C279" s="3">
+        <v>300</v>
       </c>
       <c r="D279" t="s">
         <v>51</v>
@@ -9410,10 +9413,10 @@
         <v>44962</v>
       </c>
       <c r="B280" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C280">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D280" t="s">
         <v>51</v>
@@ -9424,10 +9427,10 @@
         <v>44962</v>
       </c>
       <c r="B281" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C281">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="D281" t="s">
         <v>51</v>
@@ -9438,10 +9441,10 @@
         <v>44962</v>
       </c>
       <c r="B282" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C282">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="D282" t="s">
         <v>51</v>
@@ -9452,10 +9455,10 @@
         <v>44962</v>
       </c>
       <c r="B283" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C283">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D283" t="s">
         <v>51</v>
@@ -9466,10 +9469,10 @@
         <v>44962</v>
       </c>
       <c r="B284" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C284">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D284" t="s">
         <v>51</v>
@@ -9480,10 +9483,10 @@
         <v>44962</v>
       </c>
       <c r="B285" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C285">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D285" t="s">
         <v>51</v>
@@ -9494,10 +9497,10 @@
         <v>44962</v>
       </c>
       <c r="B286" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C286">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D286" t="s">
         <v>51</v>
@@ -9508,7 +9511,7 @@
         <v>44962</v>
       </c>
       <c r="B287" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C287">
         <v>100</v>
@@ -9522,10 +9525,10 @@
         <v>44962</v>
       </c>
       <c r="B288" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C288">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D288" t="s">
         <v>51</v>
@@ -9536,7 +9539,7 @@
         <v>44962</v>
       </c>
       <c r="B289" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C289">
         <v>50</v>
@@ -9550,10 +9553,10 @@
         <v>44962</v>
       </c>
       <c r="B290" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C290">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D290" t="s">
         <v>51</v>
@@ -9564,17 +9567,196 @@
         <v>44962</v>
       </c>
       <c r="B291" t="s">
+        <v>3</v>
+      </c>
+      <c r="C291">
+        <v>100</v>
+      </c>
+      <c r="D291" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A292" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B292" t="s">
         <v>15</v>
       </c>
-      <c r="C291">
+      <c r="C292">
         <v>300</v>
       </c>
-      <c r="D291" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C292"/>
+      <c r="D292" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A293" s="2">
+        <v>44969</v>
+      </c>
+      <c r="B293" t="s">
+        <v>3</v>
+      </c>
+      <c r="C293">
+        <v>200</v>
+      </c>
+      <c r="D293" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A294" s="2">
+        <v>44969</v>
+      </c>
+      <c r="B294" t="s">
+        <v>22</v>
+      </c>
+      <c r="C294" s="3">
+        <v>100</v>
+      </c>
+      <c r="D294" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A295" s="2">
+        <v>44969</v>
+      </c>
+      <c r="B295" t="s">
+        <v>15</v>
+      </c>
+      <c r="C295" s="3">
+        <v>50</v>
+      </c>
+      <c r="D295" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A296" s="2">
+        <v>44969</v>
+      </c>
+      <c r="B296" t="s">
+        <v>24</v>
+      </c>
+      <c r="C296" s="3">
+        <v>0</v>
+      </c>
+      <c r="D296" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A297" s="2">
+        <v>44969</v>
+      </c>
+      <c r="B297" t="s">
+        <v>4</v>
+      </c>
+      <c r="C297" s="3">
+        <v>200</v>
+      </c>
+      <c r="D297" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A298" s="2">
+        <v>44969</v>
+      </c>
+      <c r="B298" t="s">
+        <v>12</v>
+      </c>
+      <c r="C298" s="3">
+        <v>0</v>
+      </c>
+      <c r="D298" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A299" s="2">
+        <v>44969</v>
+      </c>
+      <c r="B299" t="s">
+        <v>20</v>
+      </c>
+      <c r="C299" s="3">
+        <v>100</v>
+      </c>
+      <c r="D299" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A300" s="2">
+        <v>44969</v>
+      </c>
+      <c r="B300" t="s">
+        <v>9</v>
+      </c>
+      <c r="C300" s="3">
+        <v>50</v>
+      </c>
+      <c r="D300" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A301" s="2">
+        <v>44969</v>
+      </c>
+      <c r="B301" t="s">
+        <v>41</v>
+      </c>
+      <c r="C301" s="3">
+        <v>50</v>
+      </c>
+      <c r="D301" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A302" s="2">
+        <v>44969</v>
+      </c>
+      <c r="B302" t="s">
+        <v>13</v>
+      </c>
+      <c r="C302" s="3">
+        <v>100</v>
+      </c>
+      <c r="D302" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A303" s="2">
+        <v>44969</v>
+      </c>
+      <c r="B303" t="s">
+        <v>32</v>
+      </c>
+      <c r="C303" s="3">
+        <v>100</v>
+      </c>
+      <c r="D303" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A304" s="2">
+        <v>44969</v>
+      </c>
+      <c r="B304" t="s">
+        <v>86</v>
+      </c>
+      <c r="C304" s="3">
+        <v>200</v>
+      </c>
+      <c r="D304" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
@@ -9587,10 +9769,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9851,6 +10033,17 @@
       </c>
       <c r="C23" s="16">
         <v>940</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>44969</v>
+      </c>
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="16">
+        <v>950</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update al 26 feb 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Desktop/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="673" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8843D653-3955-BA49-A41C-5CCF165E81D8}"/>
+  <xr:revisionPtr revIDLastSave="695" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B5FADD2-1306-7141-8ABF-55E641AC2C58}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14700" windowHeight="17500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="91">
   <si>
     <t>Row Labels</t>
   </si>
@@ -309,6 +309,18 @@
   </si>
   <si>
     <t>julio</t>
+  </si>
+  <si>
+    <t>Comentario</t>
+  </si>
+  <si>
+    <t>Dijo "Diablo, pero que mmg son estos tipos"</t>
+  </si>
+  <si>
+    <t>Mac Daniel</t>
+  </si>
+  <si>
+    <t>Nada</t>
   </si>
 </sst>
 </file>
@@ -5489,10 +5501,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D306"/>
+  <dimension ref="A1:D330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="I300" sqref="I300"/>
+    <sheetView tabSelected="1" topLeftCell="A294" workbookViewId="0">
+      <selection activeCell="G318" sqref="G318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9786,6 +9798,342 @@
         <v>51</v>
       </c>
     </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A307" s="2">
+        <v>44976</v>
+      </c>
+      <c r="B307" t="s">
+        <v>4</v>
+      </c>
+      <c r="C307">
+        <v>150</v>
+      </c>
+      <c r="D307" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A308" s="2">
+        <v>44976</v>
+      </c>
+      <c r="B308" t="s">
+        <v>89</v>
+      </c>
+      <c r="C308">
+        <v>300</v>
+      </c>
+      <c r="D308" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A309" s="2">
+        <v>44976</v>
+      </c>
+      <c r="B309" t="s">
+        <v>13</v>
+      </c>
+      <c r="C309">
+        <v>100</v>
+      </c>
+      <c r="D309" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A310" s="2">
+        <v>44976</v>
+      </c>
+      <c r="B310" t="s">
+        <v>3</v>
+      </c>
+      <c r="C310">
+        <v>100</v>
+      </c>
+      <c r="D310" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A311" s="2">
+        <v>44976</v>
+      </c>
+      <c r="B311" t="s">
+        <v>25</v>
+      </c>
+      <c r="C311">
+        <v>50</v>
+      </c>
+      <c r="D311" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A312" s="2">
+        <v>44976</v>
+      </c>
+      <c r="B312" t="s">
+        <v>9</v>
+      </c>
+      <c r="C312">
+        <v>50</v>
+      </c>
+      <c r="D312" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A313" s="2">
+        <v>44976</v>
+      </c>
+      <c r="B313" t="s">
+        <v>11</v>
+      </c>
+      <c r="C313">
+        <v>150</v>
+      </c>
+      <c r="D313" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A314" s="2">
+        <v>44976</v>
+      </c>
+      <c r="B314" t="s">
+        <v>20</v>
+      </c>
+      <c r="C314">
+        <v>50</v>
+      </c>
+      <c r="D314" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A315" s="2">
+        <v>44976</v>
+      </c>
+      <c r="B315" t="s">
+        <v>2</v>
+      </c>
+      <c r="C315">
+        <v>250</v>
+      </c>
+      <c r="D315" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A316" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B316" t="s">
+        <v>2</v>
+      </c>
+      <c r="C316">
+        <v>50</v>
+      </c>
+      <c r="D316" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A317" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B317" t="s">
+        <v>22</v>
+      </c>
+      <c r="C317">
+        <v>100</v>
+      </c>
+      <c r="D317" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A318" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B318" t="s">
+        <v>35</v>
+      </c>
+      <c r="C318">
+        <v>100</v>
+      </c>
+      <c r="D318" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A319" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B319" t="s">
+        <v>4</v>
+      </c>
+      <c r="C319">
+        <v>100</v>
+      </c>
+      <c r="D319" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A320" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B320" t="s">
+        <v>34</v>
+      </c>
+      <c r="C320">
+        <v>0</v>
+      </c>
+      <c r="D320" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A321" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B321" t="s">
+        <v>15</v>
+      </c>
+      <c r="C321">
+        <v>0</v>
+      </c>
+      <c r="D321" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A322" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B322" t="s">
+        <v>24</v>
+      </c>
+      <c r="C322">
+        <v>0</v>
+      </c>
+      <c r="D322" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A323" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B323" t="s">
+        <v>13</v>
+      </c>
+      <c r="C323">
+        <v>0</v>
+      </c>
+      <c r="D323" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A324" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B324" t="s">
+        <v>30</v>
+      </c>
+      <c r="C324">
+        <v>50</v>
+      </c>
+      <c r="D324" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A325" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B325" t="s">
+        <v>83</v>
+      </c>
+      <c r="C325">
+        <v>200</v>
+      </c>
+      <c r="D325" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A326" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B326" t="s">
+        <v>25</v>
+      </c>
+      <c r="C326">
+        <v>50</v>
+      </c>
+      <c r="D326" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A327" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B327" t="s">
+        <v>20</v>
+      </c>
+      <c r="C327">
+        <v>50</v>
+      </c>
+      <c r="D327" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A328" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B328" t="s">
+        <v>11</v>
+      </c>
+      <c r="C328">
+        <v>100</v>
+      </c>
+      <c r="D328" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A329" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B329" t="s">
+        <v>14</v>
+      </c>
+      <c r="C329">
+        <v>50</v>
+      </c>
+      <c r="D329" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A330" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B330" t="s">
+        <v>16</v>
+      </c>
+      <c r="C330">
+        <v>300</v>
+      </c>
+      <c r="D330" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
@@ -9797,10 +10145,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:C25"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10074,6 +10422,28 @@
         <v>950</v>
       </c>
     </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>44976</v>
+      </c>
+      <c r="B25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="16">
+        <v>940</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10082,10 +10452,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCA2D2E-DEE9-4BB9-9EC2-45DF3BC6F5C1}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10093,7 +10463,7 @@
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -10109,8 +10479,11 @@
       <c r="E1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
         <v>44948</v>
       </c>
@@ -10124,7 +10497,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>44969</v>
       </c>
@@ -10136,6 +10509,23 @@
       </c>
       <c r="D3">
         <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="12">
+        <v>44983</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Primer actualizacion marzo 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Desktop/proyectos_r/1-personales/goat/website/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2018001\OneDrive - Banco Central de la Republica Dominicana\Desktop\Proyectos\goat_website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="695" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B5FADD2-1306-7141-8ABF-55E641AC2C58}"/>
+  <xr:revisionPtr revIDLastSave="711" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{58603BCF-227F-4006-BF8D-BF859B0CA15B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14700" windowHeight="17500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="14700" windowHeight="17505" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="4" r:id="rId1"/>
@@ -32,23 +32,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="91">
   <si>
     <t>Row Labels</t>
   </si>
@@ -2979,16 +2968,16 @@
       <selection activeCell="P50" sqref="D50:P50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -3056,7 +3045,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -3096,7 +3085,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -3124,7 +3113,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3173,7 +3162,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3201,7 +3190,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3216,7 +3205,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3246,7 +3235,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3263,7 +3252,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
@@ -3291,7 +3280,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
@@ -3318,7 +3307,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
@@ -3332,7 +3321,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
@@ -3360,7 +3349,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
@@ -3391,7 +3380,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
@@ -3443,7 +3432,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
@@ -3479,7 +3468,7 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
@@ -3525,7 +3514,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
@@ -3550,7 +3539,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
@@ -3564,7 +3553,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
@@ -3590,7 +3579,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
@@ -3612,7 +3601,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
@@ -3643,7 +3632,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
@@ -3657,7 +3646,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
@@ -3711,7 +3700,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
@@ -3739,7 +3728,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
@@ -3777,7 +3766,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
@@ -3819,7 +3808,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
@@ -3829,7 +3818,7 @@
       <c r="G29" s="3"/>
       <c r="W29" s="3"/>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
@@ -3844,7 +3833,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
@@ -3859,7 +3848,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
@@ -3874,7 +3863,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>30</v>
       </c>
@@ -3895,7 +3884,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>31</v>
       </c>
@@ -3910,7 +3899,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>32</v>
       </c>
@@ -3934,7 +3923,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>33</v>
       </c>
@@ -3949,7 +3938,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>34</v>
       </c>
@@ -3973,7 +3962,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>35</v>
       </c>
@@ -3994,7 +3983,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>36</v>
       </c>
@@ -4012,7 +4001,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>37</v>
       </c>
@@ -4027,7 +4016,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>38</v>
       </c>
@@ -4048,7 +4037,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>39</v>
       </c>
@@ -4066,7 +4055,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>40</v>
       </c>
@@ -4081,7 +4070,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>41</v>
       </c>
@@ -4099,7 +4088,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>42</v>
       </c>
@@ -4114,7 +4103,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>48</v>
       </c>
@@ -4129,7 +4118,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
         <v>43</v>
       </c>
@@ -4195,7 +4184,7 @@
         <v>12055</v>
       </c>
     </row>
-    <row r="50" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
         <v>44</v>
       </c>
@@ -4244,7 +4233,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="51" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B51" s="10" t="s">
         <v>45</v>
       </c>
@@ -4311,24 +4300,24 @@
       <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="5.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>46</v>
       </c>
@@ -4350,7 +4339,7 @@
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -4418,7 +4407,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -4456,7 +4445,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -4482,7 +4471,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -4529,7 +4518,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -4556,7 +4545,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -4568,7 +4557,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -4595,7 +4584,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -4610,7 +4599,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -4637,7 +4626,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -4664,7 +4653,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -4677,7 +4666,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -4704,7 +4693,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -4734,7 +4723,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -4785,7 +4774,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -4821,7 +4810,7 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -4866,7 +4855,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -4891,7 +4880,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -4904,7 +4893,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -4929,7 +4918,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -4950,7 +4939,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -4980,7 +4969,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -4993,7 +4982,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -5047,7 +5036,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -5075,7 +5064,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -5110,7 +5099,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -5153,7 +5142,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
@@ -5161,7 +5150,7 @@
       <c r="H30"/>
       <c r="V30" s="3"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -5174,7 +5163,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
@@ -5187,7 +5176,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
@@ -5200,7 +5189,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>30</v>
       </c>
@@ -5219,7 +5208,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -5232,7 +5221,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>32</v>
       </c>
@@ -5254,7 +5243,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>33</v>
       </c>
@@ -5267,7 +5256,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>34</v>
       </c>
@@ -5289,7 +5278,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -5308,7 +5297,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
@@ -5324,7 +5313,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
@@ -5337,7 +5326,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>38</v>
       </c>
@@ -5356,7 +5345,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>39</v>
       </c>
@@ -5372,7 +5361,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>40</v>
       </c>
@@ -5385,7 +5374,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
@@ -5401,7 +5390,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>42</v>
       </c>
@@ -5414,7 +5403,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -5427,7 +5416,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>43</v>
       </c>
@@ -5492,7 +5481,7 @@
         <v>12055</v>
       </c>
     </row>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -5501,20 +5490,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D330"/>
+  <dimension ref="A1:D334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A294" workbookViewId="0">
-      <selection activeCell="G318" sqref="G318"/>
+    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
+      <selection activeCell="A332" sqref="A332:A334"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
@@ -5528,7 +5517,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44710</v>
       </c>
@@ -5542,7 +5531,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44724</v>
       </c>
@@ -5556,7 +5545,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44724</v>
       </c>
@@ -5570,7 +5559,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44724</v>
       </c>
@@ -5584,7 +5573,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44724</v>
       </c>
@@ -5598,7 +5587,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44724</v>
       </c>
@@ -5612,7 +5601,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44724</v>
       </c>
@@ -5626,7 +5615,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44724</v>
       </c>
@@ -5640,7 +5629,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44724</v>
       </c>
@@ -5654,7 +5643,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44724</v>
       </c>
@@ -5668,7 +5657,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44724</v>
       </c>
@@ -5682,7 +5671,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44724</v>
       </c>
@@ -5696,7 +5685,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44724</v>
       </c>
@@ -5710,7 +5699,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44724</v>
       </c>
@@ -5724,7 +5713,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44724</v>
       </c>
@@ -5738,7 +5727,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44724</v>
       </c>
@@ -5752,7 +5741,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44731</v>
       </c>
@@ -5766,7 +5755,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44731</v>
       </c>
@@ -5780,7 +5769,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44731</v>
       </c>
@@ -5794,7 +5783,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44731</v>
       </c>
@@ -5808,7 +5797,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44731</v>
       </c>
@@ -5822,7 +5811,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44731</v>
       </c>
@@ -5836,7 +5825,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44731</v>
       </c>
@@ -5850,7 +5839,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44731</v>
       </c>
@@ -5864,7 +5853,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44731</v>
       </c>
@@ -5878,7 +5867,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44731</v>
       </c>
@@ -5892,7 +5881,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44731</v>
       </c>
@@ -5906,7 +5895,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44731</v>
       </c>
@@ -5920,7 +5909,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44731</v>
       </c>
@@ -5934,7 +5923,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44738</v>
       </c>
@@ -5948,7 +5937,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>44738</v>
       </c>
@@ -5962,7 +5951,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44738</v>
       </c>
@@ -5976,7 +5965,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>44738</v>
       </c>
@@ -5990,7 +5979,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>44738</v>
       </c>
@@ -6004,7 +5993,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>44738</v>
       </c>
@@ -6018,7 +6007,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>44738</v>
       </c>
@@ -6032,7 +6021,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>44738</v>
       </c>
@@ -6046,7 +6035,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>44738</v>
       </c>
@@ -6060,7 +6049,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>44738</v>
       </c>
@@ -6074,7 +6063,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>44738</v>
       </c>
@@ -6088,7 +6077,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>44738</v>
       </c>
@@ -6102,7 +6091,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>44738</v>
       </c>
@@ -6116,7 +6105,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>44738</v>
       </c>
@@ -6130,7 +6119,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44738</v>
       </c>
@@ -6144,7 +6133,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>44752</v>
       </c>
@@ -6158,7 +6147,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44752</v>
       </c>
@@ -6172,7 +6161,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>44752</v>
       </c>
@@ -6186,7 +6175,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>44752</v>
       </c>
@@ -6200,7 +6189,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>44752</v>
       </c>
@@ -6214,7 +6203,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>44752</v>
       </c>
@@ -6228,7 +6217,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>44752</v>
       </c>
@@ -6242,7 +6231,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>44752</v>
       </c>
@@ -6256,7 +6245,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>44752</v>
       </c>
@@ -6270,7 +6259,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>44752</v>
       </c>
@@ -6284,7 +6273,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>44752</v>
       </c>
@@ -6298,7 +6287,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>44752</v>
       </c>
@@ -6312,7 +6301,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>44752</v>
       </c>
@@ -6326,7 +6315,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>44766</v>
       </c>
@@ -6340,7 +6329,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>44766</v>
       </c>
@@ -6354,7 +6343,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>44766</v>
       </c>
@@ -6368,7 +6357,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>44766</v>
       </c>
@@ -6382,7 +6371,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>44766</v>
       </c>
@@ -6396,7 +6385,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>44766</v>
       </c>
@@ -6410,7 +6399,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>44766</v>
       </c>
@@ -6424,7 +6413,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>44766</v>
       </c>
@@ -6438,7 +6427,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>44766</v>
       </c>
@@ -6452,7 +6441,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>44787</v>
       </c>
@@ -6466,7 +6455,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>44795</v>
       </c>
@@ -6480,7 +6469,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>44795</v>
       </c>
@@ -6494,7 +6483,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>44795</v>
       </c>
@@ -6508,7 +6497,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>44795</v>
       </c>
@@ -6522,7 +6511,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>44795</v>
       </c>
@@ -6536,7 +6525,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>44795</v>
       </c>
@@ -6550,7 +6539,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>44815</v>
       </c>
@@ -6564,7 +6553,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>44815</v>
       </c>
@@ -6578,7 +6567,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>44815</v>
       </c>
@@ -6592,7 +6581,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>44815</v>
       </c>
@@ -6606,7 +6595,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>44815</v>
       </c>
@@ -6620,7 +6609,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>44815</v>
       </c>
@@ -6634,7 +6623,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>44815</v>
       </c>
@@ -6648,7 +6637,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>44815</v>
       </c>
@@ -6662,7 +6651,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>44815</v>
       </c>
@@ -6676,7 +6665,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>44815</v>
       </c>
@@ -6690,7 +6679,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>44843</v>
       </c>
@@ -6704,7 +6693,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>44843</v>
       </c>
@@ -6718,7 +6707,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>44843</v>
       </c>
@@ -6732,7 +6721,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>44843</v>
       </c>
@@ -6746,7 +6735,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>44843</v>
       </c>
@@ -6760,7 +6749,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>44843</v>
       </c>
@@ -6774,7 +6763,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>44843</v>
       </c>
@@ -6788,7 +6777,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>44843</v>
       </c>
@@ -6802,7 +6791,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>44843</v>
       </c>
@@ -6816,7 +6805,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>44843</v>
       </c>
@@ -6830,7 +6819,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>44843</v>
       </c>
@@ -6844,7 +6833,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>44843</v>
       </c>
@@ -6858,7 +6847,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>44843</v>
       </c>
@@ -6872,7 +6861,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>44843</v>
       </c>
@@ -6886,7 +6875,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>44843</v>
       </c>
@@ -6900,7 +6889,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>44843</v>
       </c>
@@ -6914,7 +6903,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>44843</v>
       </c>
@@ -6928,7 +6917,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>44850</v>
       </c>
@@ -6942,7 +6931,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>44850</v>
       </c>
@@ -6956,7 +6945,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>44850</v>
       </c>
@@ -6970,7 +6959,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>44850</v>
       </c>
@@ -6984,7 +6973,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>44850</v>
       </c>
@@ -6998,7 +6987,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>44850</v>
       </c>
@@ -7012,7 +7001,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>44850</v>
       </c>
@@ -7026,7 +7015,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>44857</v>
       </c>
@@ -7040,7 +7029,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>44857</v>
       </c>
@@ -7054,7 +7043,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>44857</v>
       </c>
@@ -7068,7 +7057,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>44857</v>
       </c>
@@ -7082,7 +7071,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>44857</v>
       </c>
@@ -7096,7 +7085,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>44857</v>
       </c>
@@ -7110,7 +7099,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>44857</v>
       </c>
@@ -7124,7 +7113,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>44857</v>
       </c>
@@ -7138,7 +7127,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>44857</v>
       </c>
@@ -7152,7 +7141,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>44857</v>
       </c>
@@ -7166,7 +7155,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>44857</v>
       </c>
@@ -7180,7 +7169,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>44864</v>
       </c>
@@ -7194,7 +7183,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>44864</v>
       </c>
@@ -7208,7 +7197,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>44864</v>
       </c>
@@ -7222,7 +7211,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>44864</v>
       </c>
@@ -7236,7 +7225,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>44864</v>
       </c>
@@ -7250,7 +7239,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>44864</v>
       </c>
@@ -7264,7 +7253,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>44864</v>
       </c>
@@ -7278,7 +7267,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>44871</v>
       </c>
@@ -7292,7 +7281,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>44871</v>
       </c>
@@ -7306,7 +7295,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>44871</v>
       </c>
@@ -7320,7 +7309,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>44871</v>
       </c>
@@ -7334,7 +7323,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>44871</v>
       </c>
@@ -7348,7 +7337,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>44871</v>
       </c>
@@ -7362,7 +7351,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>44871</v>
       </c>
@@ -7376,7 +7365,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>44871</v>
       </c>
@@ -7390,7 +7379,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>44871</v>
       </c>
@@ -7404,7 +7393,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>44871</v>
       </c>
@@ -7418,7 +7407,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>44871</v>
       </c>
@@ -7432,7 +7421,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>44871</v>
       </c>
@@ -7446,7 +7435,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>44871</v>
       </c>
@@ -7460,7 +7449,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>44871</v>
       </c>
@@ -7474,7 +7463,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>44878</v>
       </c>
@@ -7488,7 +7477,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>44878</v>
       </c>
@@ -7502,7 +7491,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>44878</v>
       </c>
@@ -7516,7 +7505,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>44878</v>
       </c>
@@ -7530,7 +7519,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>44878</v>
       </c>
@@ -7544,7 +7533,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>44878</v>
       </c>
@@ -7558,7 +7547,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>44878</v>
       </c>
@@ -7572,7 +7561,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>44878</v>
       </c>
@@ -7586,7 +7575,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>44878</v>
       </c>
@@ -7600,7 +7589,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>44878</v>
       </c>
@@ -7614,7 +7603,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>44878</v>
       </c>
@@ -7628,7 +7617,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>44892</v>
       </c>
@@ -7642,7 +7631,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>44892</v>
       </c>
@@ -7656,7 +7645,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>44892</v>
       </c>
@@ -7670,7 +7659,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>44892</v>
       </c>
@@ -7684,7 +7673,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>44892</v>
       </c>
@@ -7698,7 +7687,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>44899</v>
       </c>
@@ -7712,7 +7701,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>44899</v>
       </c>
@@ -7726,7 +7715,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>44899</v>
       </c>
@@ -7740,7 +7729,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>44899</v>
       </c>
@@ -7754,7 +7743,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>44899</v>
       </c>
@@ -7768,7 +7757,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>44899</v>
       </c>
@@ -7782,7 +7771,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>44899</v>
       </c>
@@ -7796,7 +7785,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>44899</v>
       </c>
@@ -7810,7 +7799,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>44899</v>
       </c>
@@ -7824,7 +7813,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>44899</v>
       </c>
@@ -7838,7 +7827,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>44899</v>
       </c>
@@ -7852,7 +7841,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>44899</v>
       </c>
@@ -7866,7 +7855,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>44899</v>
       </c>
@@ -7880,7 +7869,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>44906</v>
       </c>
@@ -7894,7 +7883,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>44906</v>
       </c>
@@ -7908,7 +7897,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>44906</v>
       </c>
@@ -7922,7 +7911,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>44906</v>
       </c>
@@ -7936,7 +7925,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>44906</v>
       </c>
@@ -7950,7 +7939,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>44906</v>
       </c>
@@ -7964,7 +7953,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>44906</v>
       </c>
@@ -7978,7 +7967,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>44906</v>
       </c>
@@ -7992,7 +7981,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>44906</v>
       </c>
@@ -8006,7 +7995,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>44906</v>
       </c>
@@ -8020,7 +8009,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>44906</v>
       </c>
@@ -8034,7 +8023,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>44906</v>
       </c>
@@ -8048,7 +8037,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>44906</v>
       </c>
@@ -8062,7 +8051,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>44906</v>
       </c>
@@ -8076,7 +8065,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>44906</v>
       </c>
@@ -8090,7 +8079,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>44906</v>
       </c>
@@ -8104,7 +8093,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>44906</v>
       </c>
@@ -8118,7 +8107,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>44913</v>
       </c>
@@ -8132,7 +8121,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>44913</v>
       </c>
@@ -8146,7 +8135,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>44913</v>
       </c>
@@ -8160,7 +8149,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>44913</v>
       </c>
@@ -8174,7 +8163,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>44913</v>
       </c>
@@ -8188,7 +8177,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>44913</v>
       </c>
@@ -8202,7 +8191,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>44913</v>
       </c>
@@ -8216,7 +8205,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>44913</v>
       </c>
@@ -8230,7 +8219,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>44913</v>
       </c>
@@ -8244,7 +8233,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>44913</v>
       </c>
@@ -8258,7 +8247,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>44913</v>
       </c>
@@ -8272,7 +8261,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>44913</v>
       </c>
@@ -8286,7 +8275,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>44913</v>
       </c>
@@ -8300,7 +8289,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>44913</v>
       </c>
@@ -8314,7 +8303,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>44913</v>
       </c>
@@ -8328,7 +8317,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>44913</v>
       </c>
@@ -8342,7 +8331,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>44933</v>
       </c>
@@ -8356,7 +8345,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>44933</v>
       </c>
@@ -8370,7 +8359,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>44933</v>
       </c>
@@ -8384,7 +8373,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>44933</v>
       </c>
@@ -8398,7 +8387,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>44933</v>
       </c>
@@ -8412,7 +8401,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>44933</v>
       </c>
@@ -8426,7 +8415,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>44933</v>
       </c>
@@ -8440,7 +8429,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>44933</v>
       </c>
@@ -8454,7 +8443,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>44933</v>
       </c>
@@ -8468,7 +8457,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>44933</v>
       </c>
@@ -8482,7 +8471,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>44933</v>
       </c>
@@ -8496,7 +8485,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>44933</v>
       </c>
@@ -8510,7 +8499,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>44933</v>
       </c>
@@ -8524,7 +8513,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>44933</v>
       </c>
@@ -8538,7 +8527,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>44933</v>
       </c>
@@ -8552,7 +8541,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>44933</v>
       </c>
@@ -8566,7 +8555,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>44933</v>
       </c>
@@ -8580,7 +8569,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>44933</v>
       </c>
@@ -8594,7 +8583,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>44933</v>
       </c>
@@ -8608,7 +8597,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>44933</v>
       </c>
@@ -8622,7 +8611,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>44933</v>
       </c>
@@ -8636,7 +8625,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>44933</v>
       </c>
@@ -8650,7 +8639,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>44933</v>
       </c>
@@ -8664,7 +8653,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>44933</v>
       </c>
@@ -8678,7 +8667,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <v>44941</v>
       </c>
@@ -8692,7 +8681,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <v>44941</v>
       </c>
@@ -8706,7 +8695,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>44941</v>
       </c>
@@ -8720,7 +8709,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
         <v>44941</v>
       </c>
@@ -8734,7 +8723,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
         <v>44941</v>
       </c>
@@ -8748,7 +8737,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
         <v>44941</v>
       </c>
@@ -8762,7 +8751,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
         <v>44941</v>
       </c>
@@ -8776,7 +8765,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
         <v>44941</v>
       </c>
@@ -8790,7 +8779,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
         <v>44941</v>
       </c>
@@ -8804,7 +8793,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
         <v>44941</v>
       </c>
@@ -8818,7 +8807,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
         <v>44941</v>
       </c>
@@ -8832,7 +8821,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
         <v>44941</v>
       </c>
@@ -8846,7 +8835,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
         <v>44941</v>
       </c>
@@ -8860,7 +8849,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
         <v>44941</v>
       </c>
@@ -8874,7 +8863,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
         <v>44941</v>
       </c>
@@ -8888,7 +8877,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
         <v>44941</v>
       </c>
@@ -8902,7 +8891,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
         <v>44941</v>
       </c>
@@ -8916,7 +8905,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
         <v>44941</v>
       </c>
@@ -8930,7 +8919,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
         <v>44941</v>
       </c>
@@ -8944,7 +8933,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
         <v>44941</v>
       </c>
@@ -8958,7 +8947,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
         <v>44955</v>
       </c>
@@ -8972,7 +8961,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
         <v>44956</v>
       </c>
@@ -8986,7 +8975,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" s="2">
         <v>44956</v>
       </c>
@@ -9000,7 +8989,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
         <v>44956</v>
       </c>
@@ -9014,7 +9003,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="2">
         <v>44956</v>
       </c>
@@ -9028,7 +9017,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="2">
         <v>44956</v>
       </c>
@@ -9042,7 +9031,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="2">
         <v>44956</v>
       </c>
@@ -9056,7 +9045,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" s="2">
         <v>44956</v>
       </c>
@@ -9070,7 +9059,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
         <v>44956</v>
       </c>
@@ -9084,7 +9073,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" s="2">
         <v>44956</v>
       </c>
@@ -9098,7 +9087,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" s="2">
         <v>44956</v>
       </c>
@@ -9112,7 +9101,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="2">
         <v>44956</v>
       </c>
@@ -9126,7 +9115,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="2">
         <v>44956</v>
       </c>
@@ -9140,7 +9129,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="2">
         <v>44956</v>
       </c>
@@ -9154,7 +9143,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="2">
         <v>44956</v>
       </c>
@@ -9168,7 +9157,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="2">
         <v>44956</v>
       </c>
@@ -9182,7 +9171,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="2">
         <v>44956</v>
       </c>
@@ -9196,7 +9185,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="2">
         <v>44956</v>
       </c>
@@ -9210,7 +9199,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" s="2">
         <v>44948</v>
       </c>
@@ -9224,7 +9213,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="2">
         <v>44948</v>
       </c>
@@ -9238,7 +9227,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" s="2">
         <v>44948</v>
       </c>
@@ -9252,7 +9241,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" s="2">
         <v>44948</v>
       </c>
@@ -9266,7 +9255,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="2">
         <v>44948</v>
       </c>
@@ -9280,7 +9269,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="2">
         <v>44948</v>
       </c>
@@ -9294,7 +9283,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" s="2">
         <v>44948</v>
       </c>
@@ -9308,7 +9297,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" s="2">
         <v>44948</v>
       </c>
@@ -9322,7 +9311,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" s="2">
         <v>44948</v>
       </c>
@@ -9336,7 +9325,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" s="2">
         <v>44948</v>
       </c>
@@ -9350,7 +9339,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" s="2">
         <v>44948</v>
       </c>
@@ -9364,7 +9353,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" s="2">
         <v>44948</v>
       </c>
@@ -9378,7 +9367,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" s="2">
         <v>44948</v>
       </c>
@@ -9392,7 +9381,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" s="2">
         <v>44948</v>
       </c>
@@ -9406,7 +9395,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" s="2">
         <v>44948</v>
       </c>
@@ -9420,7 +9409,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" s="2">
         <v>44962</v>
       </c>
@@ -9434,7 +9423,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" s="2">
         <v>44962</v>
       </c>
@@ -9448,7 +9437,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" s="2">
         <v>44962</v>
       </c>
@@ -9462,7 +9451,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" s="2">
         <v>44962</v>
       </c>
@@ -9476,7 +9465,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" s="2">
         <v>44962</v>
       </c>
@@ -9490,7 +9479,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" s="2">
         <v>44962</v>
       </c>
@@ -9504,7 +9493,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" s="2">
         <v>44962</v>
       </c>
@@ -9518,7 +9507,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" s="2">
         <v>44962</v>
       </c>
@@ -9532,7 +9521,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" s="2">
         <v>44962</v>
       </c>
@@ -9546,7 +9535,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="2">
         <v>44962</v>
       </c>
@@ -9560,7 +9549,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" s="2">
         <v>44962</v>
       </c>
@@ -9574,7 +9563,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" s="2">
         <v>44962</v>
       </c>
@@ -9588,7 +9577,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" s="2">
         <v>44962</v>
       </c>
@@ -9602,7 +9591,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" s="2">
         <v>44969</v>
       </c>
@@ -9616,7 +9605,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" s="2">
         <v>44957</v>
       </c>
@@ -9630,7 +9619,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" s="2">
         <v>44969</v>
       </c>
@@ -9644,7 +9633,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="2">
         <v>44969</v>
       </c>
@@ -9658,7 +9647,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" s="2">
         <v>44969</v>
       </c>
@@ -9672,7 +9661,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" s="2">
         <v>44969</v>
       </c>
@@ -9686,7 +9675,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" s="2">
         <v>44969</v>
       </c>
@@ -9700,7 +9689,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" s="2">
         <v>44969</v>
       </c>
@@ -9714,7 +9703,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" s="2">
         <v>44969</v>
       </c>
@@ -9728,7 +9717,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" s="2">
         <v>44969</v>
       </c>
@@ -9742,7 +9731,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" s="2">
         <v>44969</v>
       </c>
@@ -9756,7 +9745,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" s="2">
         <v>44969</v>
       </c>
@@ -9770,7 +9759,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" s="2">
         <v>44956</v>
       </c>
@@ -9784,7 +9773,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" s="2">
         <v>44969</v>
       </c>
@@ -9798,7 +9787,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" s="2">
         <v>44976</v>
       </c>
@@ -9812,7 +9801,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" s="2">
         <v>44976</v>
       </c>
@@ -9826,7 +9815,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" s="2">
         <v>44976</v>
       </c>
@@ -9840,7 +9829,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" s="2">
         <v>44976</v>
       </c>
@@ -9854,7 +9843,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" s="2">
         <v>44976</v>
       </c>
@@ -9868,7 +9857,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" s="2">
         <v>44976</v>
       </c>
@@ -9882,7 +9871,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" s="2">
         <v>44976</v>
       </c>
@@ -9896,7 +9885,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" s="2">
         <v>44976</v>
       </c>
@@ -9910,7 +9899,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" s="2">
         <v>44976</v>
       </c>
@@ -9924,7 +9913,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" s="2">
         <v>44983</v>
       </c>
@@ -9938,7 +9927,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" s="2">
         <v>44983</v>
       </c>
@@ -9952,7 +9941,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" s="2">
         <v>44983</v>
       </c>
@@ -9966,7 +9955,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" s="2">
         <v>44983</v>
       </c>
@@ -9980,7 +9969,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" s="2">
         <v>44983</v>
       </c>
@@ -9994,7 +9983,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" s="2">
         <v>44983</v>
       </c>
@@ -10008,7 +9997,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" s="2">
         <v>44983</v>
       </c>
@@ -10022,7 +10011,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" s="2">
         <v>44983</v>
       </c>
@@ -10036,7 +10025,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" s="2">
         <v>44983</v>
       </c>
@@ -10050,7 +10039,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" s="2">
         <v>44983</v>
       </c>
@@ -10064,7 +10053,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" s="2">
         <v>44983</v>
       </c>
@@ -10078,7 +10067,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" s="2">
         <v>44983</v>
       </c>
@@ -10092,7 +10081,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" s="2">
         <v>44983</v>
       </c>
@@ -10106,7 +10095,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" s="2">
         <v>44983</v>
       </c>
@@ -10120,7 +10109,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330" s="2">
         <v>44983</v>
       </c>
@@ -10131,6 +10120,62 @@
         <v>300</v>
       </c>
       <c r="D330" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A331" s="2">
+        <v>44986</v>
+      </c>
+      <c r="B331" t="s">
+        <v>14</v>
+      </c>
+      <c r="C331" s="3">
+        <v>300</v>
+      </c>
+      <c r="D331" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A332" s="2">
+        <v>44986</v>
+      </c>
+      <c r="B332" t="s">
+        <v>15</v>
+      </c>
+      <c r="C332" s="3">
+        <v>300</v>
+      </c>
+      <c r="D332" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A333" s="2">
+        <v>44986</v>
+      </c>
+      <c r="B333" t="s">
+        <v>24</v>
+      </c>
+      <c r="C333" s="3">
+        <v>300</v>
+      </c>
+      <c r="D333" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A334" s="2">
+        <v>44986</v>
+      </c>
+      <c r="B334" t="s">
+        <v>9</v>
+      </c>
+      <c r="C334" s="3">
+        <v>400</v>
+      </c>
+      <c r="D334" t="s">
         <v>51</v>
       </c>
     </row>
@@ -10151,14 +10196,14 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
@@ -10169,7 +10214,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44710</v>
       </c>
@@ -10180,7 +10225,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44724</v>
       </c>
@@ -10191,7 +10236,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44731</v>
       </c>
@@ -10202,7 +10247,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44738</v>
       </c>
@@ -10213,7 +10258,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44752</v>
       </c>
@@ -10224,7 +10269,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44766</v>
       </c>
@@ -10235,7 +10280,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44795</v>
       </c>
@@ -10246,7 +10291,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44815</v>
       </c>
@@ -10257,7 +10302,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44843</v>
       </c>
@@ -10268,7 +10313,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44857</v>
       </c>
@@ -10279,7 +10324,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44857</v>
       </c>
@@ -10290,7 +10335,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44899</v>
       </c>
@@ -10301,7 +10346,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44892</v>
       </c>
@@ -10312,7 +10357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44878</v>
       </c>
@@ -10323,7 +10368,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44906</v>
       </c>
@@ -10334,7 +10379,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44913</v>
       </c>
@@ -10345,7 +10390,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44911</v>
       </c>
@@ -10356,7 +10401,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44933</v>
       </c>
@@ -10367,7 +10412,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44941</v>
       </c>
@@ -10378,7 +10423,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44948</v>
       </c>
@@ -10389,7 +10434,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44955</v>
       </c>
@@ -10400,7 +10445,7 @@
         <v>3775</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44962</v>
       </c>
@@ -10411,7 +10456,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44969</v>
       </c>
@@ -10422,7 +10467,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44976</v>
       </c>
@@ -10433,7 +10478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44983</v>
       </c>
@@ -10458,12 +10503,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -10483,7 +10528,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>44948</v>
       </c>
@@ -10497,7 +10542,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>44969</v>
       </c>
@@ -10511,7 +10556,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>44983</v>
       </c>
@@ -10541,9 +10586,9 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -10560,7 +10605,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>44906</v>
       </c>
@@ -10577,7 +10622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>44913</v>
       </c>
@@ -10594,7 +10639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>44933</v>
       </c>
@@ -10624,9 +10669,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Aportes robert y jeicol marzo 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2018001\OneDrive - Banco Central de la Republica Dominicana\Desktop\Proyectos\goat_website\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bancentralrd-my.sharepoint.com/personal/j_rosa_bancentral_gov_do/Documents/Desktop/Proyectos/goat_website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="711" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{58603BCF-227F-4006-BF8D-BF859B0CA15B}"/>
+  <xr:revisionPtr revIDLastSave="719" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{B94DF280-7F38-40D2-9BB1-7BD2C716FE9D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="14700" windowHeight="17505" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="91">
   <si>
     <t>Row Labels</t>
   </si>
@@ -1994,7 +1994,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C69D9E15-FF2B-403E-8037-8C1EF734B27A}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C69D9E15-FF2B-403E-8037-8C1EF734B27A}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:V48" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisCol" showAll="0">
@@ -5490,10 +5490,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D334"/>
+  <dimension ref="A1:D336"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
-      <selection activeCell="A332" sqref="A332:A334"/>
+      <selection activeCell="B337" sqref="B337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10176,6 +10176,34 @@
         <v>400</v>
       </c>
       <c r="D334" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A335" s="2">
+        <v>44986</v>
+      </c>
+      <c r="B335" t="s">
+        <v>35</v>
+      </c>
+      <c r="C335" s="3">
+        <v>300</v>
+      </c>
+      <c r="D335" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A336" s="2">
+        <v>44986</v>
+      </c>
+      <c r="B336" t="s">
+        <v>23</v>
+      </c>
+      <c r="C336" s="3">
+        <v>500</v>
+      </c>
+      <c r="D336" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización al 05 marzo 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Desktop/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="742" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEF9EB6C-43A0-0744-A557-59EC42BAC911}"/>
+  <xr:revisionPtr revIDLastSave="792" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA19808D-246D-0B4E-891D-6F7D13CC9E9C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="95">
   <si>
     <t>Row Labels</t>
   </si>
@@ -326,7 +326,13 @@
     <t>Mesa</t>
   </si>
   <si>
-    <t>Chaqueta</t>
+    <t>Discutiendo con el chamo y diciendo improperios</t>
+  </si>
+  <si>
+    <t>Caja chica</t>
+  </si>
+  <si>
+    <t>Aporte arreglar puerta</t>
   </si>
 </sst>
 </file>
@@ -339,7 +345,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,6 +380,13 @@
       <b/>
       <sz val="11"/>
       <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -430,7 +443,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -469,12 +482,33 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2024,7 +2058,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C69D9E15-FF2B-403E-8037-8C1EF734B27A}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C69D9E15-FF2B-403E-8037-8C1EF734B27A}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:V48" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisCol" showAll="0">
@@ -2681,7 +2715,7 @@
     <dataField name="Sum of Aporte" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="5">
+    <format dxfId="7">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="5" selected="0">
@@ -2694,13 +2728,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="6">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="5">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="5">
@@ -2713,7 +2747,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -5520,10 +5554,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D338"/>
+  <dimension ref="A1:D351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
-      <selection activeCell="E338" sqref="E338"/>
+    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
+      <selection activeCell="G349" sqref="G349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10253,21 +10287,203 @@
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A338" s="2">
-        <v>44986</v>
-      </c>
-      <c r="B338" t="s">
-        <v>89</v>
-      </c>
-      <c r="C338" s="3">
+        <v>44990</v>
+      </c>
+      <c r="B338" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C338" s="20">
+        <v>150</v>
+      </c>
+      <c r="D338" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A339" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B339" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C339" s="20">
+        <v>200</v>
+      </c>
+      <c r="D339" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A340" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B340" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C340" s="20">
+        <v>150</v>
+      </c>
+      <c r="D340" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A341" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B341" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C341" s="20">
+        <v>500</v>
+      </c>
+      <c r="D341" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A342" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B342" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C342" s="20">
+        <v>100</v>
+      </c>
+      <c r="D342" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A343" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B343" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C343" s="20">
+        <v>100</v>
+      </c>
+      <c r="D343" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A344" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B344" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C344" s="20">
+        <v>150</v>
+      </c>
+      <c r="D344" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A345" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B345" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C345" s="20">
+        <v>50</v>
+      </c>
+      <c r="D345" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A346" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B346" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C346" s="20">
+        <v>50</v>
+      </c>
+      <c r="D346" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A347" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B347" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C347" s="20">
+        <v>200</v>
+      </c>
+      <c r="D347" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A348" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B348" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C348" s="20">
+        <v>100</v>
+      </c>
+      <c r="D348" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A349" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B349" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C349" s="20">
+        <v>50</v>
+      </c>
+      <c r="D349" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A350" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B350" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C350" s="20">
         <v>300</v>
       </c>
-      <c r="D338" t="s">
+      <c r="D350" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A351" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B351" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C351" s="3">
+        <v>150</v>
+      </c>
+      <c r="D351" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10276,10 +10492,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10586,6 +10802,40 @@
         <v>3200</v>
       </c>
     </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28">
+        <f>800+150</f>
+        <v>950</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="16">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="16">
+        <v>300</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10594,10 +10844,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCA2D2E-DEE9-4BB9-9EC2-45DF3BC6F5C1}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10627,10 +10877,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
-        <v>44948</v>
+        <v>44983</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>61</v>
@@ -10638,35 +10888,7 @@
       <c r="D2">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="12">
-        <v>44969</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="12">
-        <v>44983</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4">
-        <v>100</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="F2" t="s">
         <v>88</v>
       </c>
     </row>
@@ -10677,15 +10899,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE771D5-AE0E-9C4B-B862-1B8092D29603}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -10701,8 +10923,11 @@
       <c r="E1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
         <v>44906</v>
       </c>
@@ -10719,7 +10944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>44913</v>
       </c>
@@ -10736,7 +10961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>44933</v>
       </c>
@@ -10751,6 +10976,60 @@
       </c>
       <c r="E4" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="12">
+        <v>44948</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="12">
+        <v>44969</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="12">
+        <v>44990</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -10763,7 +11042,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10785,15 +11064,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="17">
-        <v>1200</v>
-      </c>
-      <c r="C2" t="s">
-        <v>92</v>
-      </c>
+      <c r="B2" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update al 11 mar 2023, fix this year table
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Desktop/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="792" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA19808D-246D-0B4E-891D-6F7D13CC9E9C}"/>
+  <xr:revisionPtr revIDLastSave="796" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9709060-82AC-D542-8FB6-7C53D77B849B}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="95">
   <si>
     <t>Row Labels</t>
   </si>
@@ -488,27 +488,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2715,7 +2695,7 @@
     <dataField name="Sum of Aporte" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="7">
+    <format dxfId="5">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="5" selected="0">
@@ -2728,13 +2708,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="4">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="3">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="5">
@@ -2747,7 +2727,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -5554,10 +5534,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D351"/>
+  <dimension ref="A1:D352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
-      <selection activeCell="G349" sqref="G349"/>
+    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
+      <selection activeCell="A353" sqref="A353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10478,6 +10458,20 @@
         <v>150</v>
       </c>
       <c r="D351" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A352" s="2">
+        <v>44996</v>
+      </c>
+      <c r="B352" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C352" s="3">
+        <v>200</v>
+      </c>
+      <c r="D352" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pago kivelo y Javier marzo
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Desktop/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1012" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38C2C7CC-21BD-7549-9E83-61A2F90B7B58}"/>
+  <xr:revisionPtr revIDLastSave="1020" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B51EDC3-C1B1-9447-A5B6-2A11E2C2E146}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="4" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="96">
   <si>
     <t>Row Labels</t>
   </si>
@@ -5519,10 +5519,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D365"/>
+  <dimension ref="A1:D367"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A314" workbookViewId="0">
-      <selection activeCell="A366" sqref="A366"/>
+    <sheetView tabSelected="1" topLeftCell="A347" workbookViewId="0">
+      <selection activeCell="B368" sqref="B368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10639,6 +10639,34 @@
         <v>300</v>
       </c>
       <c r="D365" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A366" s="2">
+        <v>45000</v>
+      </c>
+      <c r="B366" t="s">
+        <v>33</v>
+      </c>
+      <c r="C366" s="3">
+        <v>300</v>
+      </c>
+      <c r="D366" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A367" s="2">
+        <v>45000</v>
+      </c>
+      <c r="B367" t="s">
+        <v>37</v>
+      </c>
+      <c r="C367" s="3">
+        <v>400</v>
+      </c>
+      <c r="D367" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pago arbitro domingo 19 de marzo
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Desktop/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1020" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B51EDC3-C1B1-9447-A5B6-2A11E2C2E146}"/>
+  <xr:revisionPtr revIDLastSave="1023" documentId="13_ncr:1_{A5B72EDE-4AFF-4FA1-84AB-8EF4FBC89CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F12355D7-E883-084A-B577-F75AB71EF96D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="4" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="96">
   <si>
     <t>Row Labels</t>
   </si>
@@ -5521,7 +5521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D367"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A347" workbookViewId="0">
+    <sheetView topLeftCell="A347" workbookViewId="0">
       <selection activeCell="B368" sqref="B368"/>
     </sheetView>
   </sheetViews>
@@ -10681,10 +10681,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11033,6 +11033,17 @@
         <v>84</v>
       </c>
       <c r="C31" s="16">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>45004</v>
+      </c>
+      <c r="B32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="16">
         <v>800</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización al 2 de abril y reglas
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Library/CloudStorage/OneDrive-Personal/Desktop/proyectos_r/1-personales/goat/website/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Desktop/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4D9C3A-336C-664A-B64F-4A547AC2498E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{FA4D9C3A-336C-664A-B64F-4A547AC2498E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7B9DB18-E64D-7946-AABD-71F312F7EC89}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="3" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="99">
   <si>
     <t>Row Labels</t>
   </si>
@@ -335,6 +335,15 @@
   </si>
   <si>
     <t>Hizo un pique y rebotó el balón inapropiadamente</t>
+  </si>
+  <si>
+    <t>Pelota</t>
+  </si>
+  <si>
+    <t>Tecnica</t>
+  </si>
+  <si>
+    <t>Discutió con el Arbito y le dijo algo</t>
   </si>
 </sst>
 </file>
@@ -2023,7 +2032,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C69D9E15-FF2B-403E-8037-8C1EF734B27A}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C69D9E15-FF2B-403E-8037-8C1EF734B27A}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:V48" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisCol" showAll="0">
@@ -2993,7 +3002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9F77B7-C594-4E55-848A-11E6F2163B93}">
   <dimension ref="B3:W51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="W47" sqref="W47"/>
     </sheetView>
   </sheetViews>
@@ -5519,10 +5528,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D368"/>
+  <dimension ref="A1:D383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A347" workbookViewId="0">
-      <selection activeCell="A369" sqref="A369"/>
+    <sheetView topLeftCell="A349" workbookViewId="0">
+      <selection activeCell="B383" sqref="B383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10684,6 +10693,216 @@
         <v>70</v>
       </c>
     </row>
+    <row r="369" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A369" s="2">
+        <v>45011</v>
+      </c>
+      <c r="B369" t="s">
+        <v>43</v>
+      </c>
+      <c r="C369">
+        <v>100</v>
+      </c>
+      <c r="D369" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A370" s="2">
+        <v>45011</v>
+      </c>
+      <c r="B370" t="s">
+        <v>55</v>
+      </c>
+      <c r="C370">
+        <v>100</v>
+      </c>
+      <c r="D370" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="371" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A371" s="2">
+        <v>45011</v>
+      </c>
+      <c r="B371" t="s">
+        <v>23</v>
+      </c>
+      <c r="C371">
+        <v>100</v>
+      </c>
+      <c r="D371" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="372" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A372" s="2">
+        <v>45011</v>
+      </c>
+      <c r="B372" t="s">
+        <v>49</v>
+      </c>
+      <c r="C372">
+        <v>200</v>
+      </c>
+      <c r="D372" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A373" s="2">
+        <v>45011</v>
+      </c>
+      <c r="B373" t="s">
+        <v>22</v>
+      </c>
+      <c r="C373">
+        <v>200</v>
+      </c>
+      <c r="D373" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A374" s="2">
+        <v>45011</v>
+      </c>
+      <c r="B374" t="s">
+        <v>25</v>
+      </c>
+      <c r="C374" s="3">
+        <v>200</v>
+      </c>
+      <c r="D374" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A375" s="2">
+        <v>45018</v>
+      </c>
+      <c r="B375" t="s">
+        <v>24</v>
+      </c>
+      <c r="C375">
+        <v>250</v>
+      </c>
+      <c r="D375" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A376" s="2">
+        <v>45018</v>
+      </c>
+      <c r="B376" t="s">
+        <v>23</v>
+      </c>
+      <c r="C376">
+        <v>100</v>
+      </c>
+      <c r="D376" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A377" s="2">
+        <v>45018</v>
+      </c>
+      <c r="B377" t="s">
+        <v>40</v>
+      </c>
+      <c r="C377">
+        <v>500</v>
+      </c>
+      <c r="D377" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A378" s="2">
+        <v>45018</v>
+      </c>
+      <c r="B378" t="s">
+        <v>54</v>
+      </c>
+      <c r="C378">
+        <v>50</v>
+      </c>
+      <c r="D378" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A379" s="2">
+        <v>45018</v>
+      </c>
+      <c r="B379" t="s">
+        <v>73</v>
+      </c>
+      <c r="C379">
+        <v>200</v>
+      </c>
+      <c r="D379" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A380" s="2">
+        <v>45018</v>
+      </c>
+      <c r="B380" t="s">
+        <v>73</v>
+      </c>
+      <c r="C380">
+        <v>100</v>
+      </c>
+      <c r="D380" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A381" s="2">
+        <v>45018</v>
+      </c>
+      <c r="B381" t="s">
+        <v>41</v>
+      </c>
+      <c r="C381">
+        <v>100</v>
+      </c>
+      <c r="D381" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A382" s="2">
+        <v>45018</v>
+      </c>
+      <c r="B382" t="s">
+        <v>43</v>
+      </c>
+      <c r="C382">
+        <v>100</v>
+      </c>
+      <c r="D382" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A383" s="2">
+        <v>45018</v>
+      </c>
+      <c r="B383" t="s">
+        <v>35</v>
+      </c>
+      <c r="C383">
+        <v>300</v>
+      </c>
+      <c r="D383" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
@@ -10695,10 +10914,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11061,6 +11280,39 @@
         <v>800</v>
       </c>
     </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>45011</v>
+      </c>
+      <c r="B33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="16">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>45018</v>
+      </c>
+      <c r="B34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="16">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>45018</v>
+      </c>
+      <c r="B35" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="16">
+        <v>940</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11069,10 +11321,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCA2D2E-DEE9-4BB9-9EC2-45DF3BC6F5C1}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11103,10 +11355,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
-        <v>44983</v>
+        <v>44997</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>74</v>
@@ -11115,23 +11367,6 @@
         <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="12">
-        <v>44997</v>
-      </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-      <c r="F3" t="s">
         <v>95</v>
       </c>
     </row>
@@ -11142,10 +11377,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE771D5-AE0E-9C4B-B862-1B8092D29603}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11278,6 +11513,46 @@
         <v>94</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="12">
+        <v>44983</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="12">
+        <v>45018</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9">
+        <v>100</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Aportes al 16 de abril 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Desktop/proyectos_r/1-personales/goat/website/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Backup/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{FA4D9C3A-336C-664A-B64F-4A547AC2498E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7B9DB18-E64D-7946-AABD-71F312F7EC89}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{FA4D9C3A-336C-664A-B64F-4A547AC2498E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56F0D6F0-554B-EC4C-9B29-6C4666693F19}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="99">
   <si>
     <t>Row Labels</t>
   </si>
@@ -2032,7 +2032,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C69D9E15-FF2B-403E-8037-8C1EF734B27A}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C69D9E15-FF2B-403E-8037-8C1EF734B27A}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:V48" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisCol" showAll="0">
@@ -5528,10 +5528,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D383"/>
+  <dimension ref="A1:D392"/>
   <sheetViews>
-    <sheetView topLeftCell="A349" workbookViewId="0">
-      <selection activeCell="B383" sqref="B383"/>
+    <sheetView tabSelected="1" topLeftCell="A359" workbookViewId="0">
+      <selection activeCell="C392" sqref="C392"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10903,6 +10903,132 @@
         <v>70</v>
       </c>
     </row>
+    <row r="384" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A384" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B384" t="s">
+        <v>37</v>
+      </c>
+      <c r="C384" s="3">
+        <v>100</v>
+      </c>
+      <c r="D384" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A385" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B385" t="s">
+        <v>40</v>
+      </c>
+      <c r="C385" s="3">
+        <v>300</v>
+      </c>
+      <c r="D385" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A386" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B386" t="s">
+        <v>50</v>
+      </c>
+      <c r="C386" s="3">
+        <v>250</v>
+      </c>
+      <c r="D386" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="387" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A387" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B387" t="s">
+        <v>44</v>
+      </c>
+      <c r="C387" s="3">
+        <v>250</v>
+      </c>
+      <c r="D387" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A388" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B388" t="s">
+        <v>55</v>
+      </c>
+      <c r="C388" s="3">
+        <v>300</v>
+      </c>
+      <c r="D388" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A389" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B389" t="s">
+        <v>36</v>
+      </c>
+      <c r="C389" s="3">
+        <v>250</v>
+      </c>
+      <c r="D389" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A390" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B390" t="s">
+        <v>34</v>
+      </c>
+      <c r="C390" s="3">
+        <v>200</v>
+      </c>
+      <c r="D390" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A391" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B391" t="s">
+        <v>37</v>
+      </c>
+      <c r="C391" s="3">
+        <v>300</v>
+      </c>
+      <c r="D391" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A392" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B392" t="s">
+        <v>32</v>
+      </c>
+      <c r="C392" s="3">
+        <v>100</v>
+      </c>
+      <c r="D392" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
@@ -10914,10 +11040,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11313,6 +11439,17 @@
         <v>940</v>
       </c>
     </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="16">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11321,10 +11458,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCA2D2E-DEE9-4BB9-9EC2-45DF3BC6F5C1}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11353,23 +11490,6 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="12">
-        <v>44997</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-      <c r="F2" t="s">
-        <v>95</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11377,10 +11497,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE771D5-AE0E-9C4B-B862-1B8092D29603}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11553,6 +11673,26 @@
         <v>98</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="12">
+        <v>44997</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización al 7 mayo de 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Library/CloudStorage/OneDrive-Personal/Backup/proyectos_r/1-personales/goat/website/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Backup/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBF4DC7-46AB-CD4C-8342-9A9041627525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{5FBF4DC7-46AB-CD4C-8342-9A9041627525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A8216FB-B781-2348-A689-5237F444EADF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ingreso" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="64">
   <si>
     <t>Alfredo</t>
   </si>
@@ -230,10 +230,10 @@
     <t>Pelota</t>
   </si>
   <si>
-    <t>Tecnica</t>
+    <t>Discutió con el Arbito y le dijo algo</t>
   </si>
   <si>
-    <t>Discutió con el Arbito y le dijo algo</t>
+    <t>Agua</t>
   </si>
 </sst>
 </file>
@@ -243,7 +243,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -289,7 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -298,10 +298,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -595,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D403"/>
+  <dimension ref="A1:D416"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A364" workbookViewId="0">
-      <selection activeCell="G397" sqref="G397"/>
+    <sheetView topLeftCell="A380" workbookViewId="0">
+      <selection activeCell="B417" sqref="B417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5330,10 +5327,10 @@
       <c r="A338" s="1">
         <v>44990</v>
       </c>
-      <c r="B338" s="6" t="s">
+      <c r="B338" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C338" s="6">
+      <c r="C338" s="5">
         <v>150</v>
       </c>
       <c r="D338" t="s">
@@ -5344,10 +5341,10 @@
       <c r="A339" s="1">
         <v>44990</v>
       </c>
-      <c r="B339" s="6" t="s">
+      <c r="B339" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C339" s="6">
+      <c r="C339" s="5">
         <v>200</v>
       </c>
       <c r="D339" t="s">
@@ -5358,10 +5355,10 @@
       <c r="A340" s="1">
         <v>44990</v>
       </c>
-      <c r="B340" s="6" t="s">
+      <c r="B340" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C340" s="6">
+      <c r="C340" s="5">
         <v>150</v>
       </c>
       <c r="D340" t="s">
@@ -5372,10 +5369,10 @@
       <c r="A341" s="1">
         <v>44990</v>
       </c>
-      <c r="B341" s="6" t="s">
+      <c r="B341" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C341" s="6">
+      <c r="C341" s="5">
         <v>500</v>
       </c>
       <c r="D341" t="s">
@@ -5386,10 +5383,10 @@
       <c r="A342" s="1">
         <v>44990</v>
       </c>
-      <c r="B342" s="6" t="s">
+      <c r="B342" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C342" s="6">
+      <c r="C342" s="5">
         <v>100</v>
       </c>
       <c r="D342" t="s">
@@ -5400,10 +5397,10 @@
       <c r="A343" s="1">
         <v>44990</v>
       </c>
-      <c r="B343" s="6" t="s">
+      <c r="B343" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C343" s="6">
+      <c r="C343" s="5">
         <v>100</v>
       </c>
       <c r="D343" t="s">
@@ -5414,10 +5411,10 @@
       <c r="A344" s="1">
         <v>44990</v>
       </c>
-      <c r="B344" s="6" t="s">
+      <c r="B344" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C344" s="6">
+      <c r="C344" s="5">
         <v>150</v>
       </c>
       <c r="D344" t="s">
@@ -5428,10 +5425,10 @@
       <c r="A345" s="1">
         <v>44990</v>
       </c>
-      <c r="B345" s="6" t="s">
+      <c r="B345" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C345" s="6">
+      <c r="C345" s="5">
         <v>50</v>
       </c>
       <c r="D345" t="s">
@@ -5442,10 +5439,10 @@
       <c r="A346" s="1">
         <v>44990</v>
       </c>
-      <c r="B346" s="6" t="s">
+      <c r="B346" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C346" s="6">
+      <c r="C346" s="5">
         <v>50</v>
       </c>
       <c r="D346" t="s">
@@ -5456,10 +5453,10 @@
       <c r="A347" s="1">
         <v>44990</v>
       </c>
-      <c r="B347" s="6" t="s">
+      <c r="B347" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C347" s="6">
+      <c r="C347" s="5">
         <v>200</v>
       </c>
       <c r="D347" t="s">
@@ -5470,10 +5467,10 @@
       <c r="A348" s="1">
         <v>44990</v>
       </c>
-      <c r="B348" s="6" t="s">
+      <c r="B348" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C348" s="6">
+      <c r="C348" s="5">
         <v>100</v>
       </c>
       <c r="D348" t="s">
@@ -5484,10 +5481,10 @@
       <c r="A349" s="1">
         <v>44990</v>
       </c>
-      <c r="B349" s="6" t="s">
+      <c r="B349" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C349" s="6">
+      <c r="C349" s="5">
         <v>50</v>
       </c>
       <c r="D349" t="s">
@@ -5498,10 +5495,10 @@
       <c r="A350" s="1">
         <v>44990</v>
       </c>
-      <c r="B350" s="6" t="s">
+      <c r="B350" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C350" s="6">
+      <c r="C350" s="5">
         <v>300</v>
       </c>
       <c r="D350" t="s">
@@ -5512,7 +5509,7 @@
       <c r="A351" s="1">
         <v>44990</v>
       </c>
-      <c r="B351" s="6" t="s">
+      <c r="B351" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C351" s="2">
@@ -5526,7 +5523,7 @@
       <c r="A352" s="1">
         <v>44996</v>
       </c>
-      <c r="B352" s="6" t="s">
+      <c r="B352" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C352" s="2">
@@ -5925,7 +5922,7 @@
         <v>100</v>
       </c>
       <c r="D380" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.2">
@@ -6250,9 +6247,191 @@
         <v>35</v>
       </c>
     </row>
+    <row r="404" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A404" s="1">
+        <v>45046</v>
+      </c>
+      <c r="B404" t="s">
+        <v>38</v>
+      </c>
+      <c r="C404" s="2">
+        <v>100</v>
+      </c>
+      <c r="D404" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A405" s="1">
+        <v>45046</v>
+      </c>
+      <c r="B405" t="s">
+        <v>1</v>
+      </c>
+      <c r="C405" s="2">
+        <v>100</v>
+      </c>
+      <c r="D405" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A406" s="1">
+        <v>45046</v>
+      </c>
+      <c r="B406" t="s">
+        <v>3</v>
+      </c>
+      <c r="C406" s="2">
+        <v>300</v>
+      </c>
+      <c r="D406" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A407" s="1">
+        <v>45046</v>
+      </c>
+      <c r="B407" t="s">
+        <v>0</v>
+      </c>
+      <c r="C407" s="2">
+        <v>200</v>
+      </c>
+      <c r="D407" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A408" s="1">
+        <v>45046</v>
+      </c>
+      <c r="B408" t="s">
+        <v>19</v>
+      </c>
+      <c r="C408" s="2">
+        <v>300</v>
+      </c>
+      <c r="D408" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="409" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A409" s="1">
+        <v>45046</v>
+      </c>
+      <c r="B409" t="s">
+        <v>7</v>
+      </c>
+      <c r="C409" s="2">
+        <v>200</v>
+      </c>
+      <c r="D409" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A410" s="1">
+        <v>45046</v>
+      </c>
+      <c r="B410" t="s">
+        <v>11</v>
+      </c>
+      <c r="C410" s="2">
+        <v>100</v>
+      </c>
+      <c r="D410" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A411" s="1">
+        <v>45053</v>
+      </c>
+      <c r="B411" t="s">
+        <v>1</v>
+      </c>
+      <c r="C411" s="2">
+        <v>100</v>
+      </c>
+      <c r="D411" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A412" s="1">
+        <v>45053</v>
+      </c>
+      <c r="B412" t="s">
+        <v>19</v>
+      </c>
+      <c r="C412" s="2">
+        <v>100</v>
+      </c>
+      <c r="D412" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A413" s="1">
+        <v>45053</v>
+      </c>
+      <c r="B413" t="s">
+        <v>21</v>
+      </c>
+      <c r="C413" s="2">
+        <v>300</v>
+      </c>
+      <c r="D413" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A414" s="1">
+        <v>45053</v>
+      </c>
+      <c r="B414" t="s">
+        <v>7</v>
+      </c>
+      <c r="C414" s="2">
+        <v>50</v>
+      </c>
+      <c r="D414" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A415" s="1">
+        <v>45053</v>
+      </c>
+      <c r="B415" t="s">
+        <v>17</v>
+      </c>
+      <c r="C415" s="2">
+        <v>100</v>
+      </c>
+      <c r="D415" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A416" s="1">
+        <v>45053</v>
+      </c>
+      <c r="B416" t="s">
+        <v>9</v>
+      </c>
+      <c r="C416" s="2">
+        <v>600</v>
+      </c>
+      <c r="D416" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="B418:B1048576 B1:B416">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6261,17 +6440,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -6292,7 +6471,7 @@
       <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>180</v>
       </c>
     </row>
@@ -6314,7 +6493,7 @@
       <c r="B4" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>185</v>
       </c>
     </row>
@@ -6325,7 +6504,7 @@
       <c r="B5" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>185</v>
       </c>
     </row>
@@ -6336,7 +6515,7 @@
       <c r="B6" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>250</v>
       </c>
     </row>
@@ -6347,7 +6526,7 @@
       <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>200</v>
       </c>
     </row>
@@ -6358,7 +6537,7 @@
       <c r="B8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>200</v>
       </c>
     </row>
@@ -6369,7 +6548,7 @@
       <c r="B9" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>200</v>
       </c>
     </row>
@@ -6380,7 +6559,7 @@
       <c r="B10" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>150</v>
       </c>
     </row>
@@ -6391,7 +6570,7 @@
       <c r="B11" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>200</v>
       </c>
     </row>
@@ -6402,7 +6581,7 @@
       <c r="B12" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>443</v>
       </c>
     </row>
@@ -6413,7 +6592,7 @@
       <c r="B13" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>150</v>
       </c>
     </row>
@@ -6424,7 +6603,7 @@
       <c r="B14" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6435,7 +6614,7 @@
       <c r="B15" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>200</v>
       </c>
     </row>
@@ -6446,7 +6625,7 @@
       <c r="B16" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>950</v>
       </c>
     </row>
@@ -6457,7 +6636,7 @@
       <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>950</v>
       </c>
     </row>
@@ -6468,7 +6647,7 @@
       <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>1500</v>
       </c>
     </row>
@@ -6479,7 +6658,7 @@
       <c r="B19" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>940</v>
       </c>
     </row>
@@ -6490,7 +6669,7 @@
       <c r="B20" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>950</v>
       </c>
     </row>
@@ -6501,7 +6680,7 @@
       <c r="B21" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>800</v>
       </c>
     </row>
@@ -6512,7 +6691,7 @@
       <c r="B22" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>3775</v>
       </c>
     </row>
@@ -6523,7 +6702,7 @@
       <c r="B23" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>940</v>
       </c>
     </row>
@@ -6534,7 +6713,7 @@
       <c r="B24" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>950</v>
       </c>
     </row>
@@ -6545,7 +6724,7 @@
       <c r="B25" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6556,7 +6735,7 @@
       <c r="B26" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <v>940</v>
       </c>
     </row>
@@ -6567,7 +6746,7 @@
       <c r="B27" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="4">
         <v>3200</v>
       </c>
     </row>
@@ -6578,7 +6757,7 @@
       <c r="B28" t="s">
         <v>47</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="4">
         <f>800+150</f>
         <v>950</v>
       </c>
@@ -6590,7 +6769,7 @@
       <c r="B29" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <v>730</v>
       </c>
     </row>
@@ -6601,7 +6780,7 @@
       <c r="B30" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <v>300</v>
       </c>
     </row>
@@ -6612,7 +6791,7 @@
       <c r="B31" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="4">
         <v>800</v>
       </c>
     </row>
@@ -6623,7 +6802,7 @@
       <c r="B32" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="4">
         <v>800</v>
       </c>
     </row>
@@ -6634,7 +6813,7 @@
       <c r="B33" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="4">
         <v>900</v>
       </c>
     </row>
@@ -6645,7 +6824,7 @@
       <c r="B34" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="4">
         <v>2300</v>
       </c>
     </row>
@@ -6656,7 +6835,7 @@
       <c r="B35" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="4">
         <v>940</v>
       </c>
     </row>
@@ -6667,7 +6846,7 @@
       <c r="B36" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="4">
         <v>1000</v>
       </c>
     </row>
@@ -6678,8 +6857,31 @@
       <c r="B37" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="4">
         <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>45046</v>
+      </c>
+      <c r="B38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>45053</v>
+      </c>
+      <c r="B39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="4">
+        <f>800+150</f>
+        <v>950</v>
       </c>
     </row>
   </sheetData>
@@ -6902,7 +7104,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Actualizar listado de miembros
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Backup/proyectos_r/1-personales/goat/website/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d7fcadea2d58d9a6/Escritorio/GOAT/goat_website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="13_ncr:1_{5FBF4DC7-46AB-CD4C-8342-9A9041627525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA73770E-0CE3-4140-ACC7-693649C7701A}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{5FBF4DC7-46AB-CD4C-8342-9A9041627525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B9DB3FF-3A22-418C-B889-8B567CC0A95E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ingreso" sheetId="1" r:id="rId1"/>
@@ -308,7 +308,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -600,18 +600,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D423"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.68359375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.68359375" customWidth="1"/>
+    <col min="3" max="3" width="10.3125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -625,7 +625,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>44710</v>
       </c>
@@ -639,7 +639,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>44724</v>
       </c>
@@ -653,7 +653,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>44724</v>
       </c>
@@ -667,7 +667,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>44724</v>
       </c>
@@ -681,7 +681,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>44724</v>
       </c>
@@ -695,7 +695,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>44724</v>
       </c>
@@ -709,7 +709,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>44724</v>
       </c>
@@ -723,7 +723,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>44724</v>
       </c>
@@ -737,7 +737,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>44724</v>
       </c>
@@ -751,7 +751,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>44724</v>
       </c>
@@ -765,7 +765,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>44724</v>
       </c>
@@ -779,7 +779,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>44724</v>
       </c>
@@ -793,7 +793,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>44724</v>
       </c>
@@ -807,7 +807,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>44724</v>
       </c>
@@ -821,7 +821,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>44724</v>
       </c>
@@ -835,7 +835,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
         <v>44724</v>
       </c>
@@ -849,7 +849,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1">
         <v>44731</v>
       </c>
@@ -863,7 +863,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1">
         <v>44731</v>
       </c>
@@ -877,7 +877,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1">
         <v>44731</v>
       </c>
@@ -891,7 +891,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1">
         <v>44731</v>
       </c>
@@ -905,7 +905,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1">
         <v>44731</v>
       </c>
@@ -919,7 +919,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1">
         <v>44731</v>
       </c>
@@ -933,7 +933,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1">
         <v>44731</v>
       </c>
@@ -947,7 +947,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1">
         <v>44731</v>
       </c>
@@ -961,7 +961,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1">
         <v>44731</v>
       </c>
@@ -975,7 +975,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1">
         <v>44731</v>
       </c>
@@ -989,7 +989,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1">
         <v>44731</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1">
         <v>44731</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1">
         <v>44731</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1">
         <v>44738</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1">
         <v>44738</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1">
         <v>44738</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1">
         <v>44738</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1">
         <v>44738</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1">
         <v>44738</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1">
         <v>44738</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1">
         <v>44738</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1">
         <v>44738</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1">
         <v>44738</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1">
         <v>44738</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1">
         <v>44738</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1">
         <v>44738</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1">
         <v>44738</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1">
         <v>44738</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1">
         <v>44752</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1">
         <v>44752</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1">
         <v>44752</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1">
         <v>44752</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1">
         <v>44752</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1">
         <v>44752</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1">
         <v>44752</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1">
         <v>44752</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1">
         <v>44752</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1">
         <v>44752</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1">
         <v>44752</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1">
         <v>44752</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1">
         <v>44752</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1">
         <v>44766</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1">
         <v>44766</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1">
         <v>44766</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1">
         <v>44766</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1">
         <v>44766</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1">
         <v>44766</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1">
         <v>44766</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1">
         <v>44766</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1">
         <v>44766</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1">
         <v>44787</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1">
         <v>44795</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1">
         <v>44795</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1">
         <v>44795</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1">
         <v>44795</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1">
         <v>44795</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1">
         <v>44795</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1">
         <v>44815</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1">
         <v>44815</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1">
         <v>44815</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1">
         <v>44815</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1">
         <v>44815</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1">
         <v>44815</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1">
         <v>44815</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1">
         <v>44815</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1">
         <v>44815</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1">
         <v>44815</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1">
         <v>44843</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1">
         <v>44843</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1">
         <v>44843</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1">
         <v>44843</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1">
         <v>44843</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1">
         <v>44843</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1">
         <v>44843</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1">
         <v>44843</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1">
         <v>44843</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1">
         <v>44843</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1">
         <v>44843</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1">
         <v>44843</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="1">
         <v>44843</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="1">
         <v>44843</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1">
         <v>44843</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="1">
         <v>44843</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1">
         <v>44843</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="1">
         <v>44850</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="1">
         <v>44850</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="1">
         <v>44850</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="1">
         <v>44850</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="1">
         <v>44850</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="1">
         <v>44850</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="1">
         <v>44850</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="1">
         <v>44857</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="1">
         <v>44857</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="1">
         <v>44857</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="1">
         <v>44857</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="1">
         <v>44857</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="1">
         <v>44857</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="1">
         <v>44857</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="1">
         <v>44857</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="1">
         <v>44857</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="1">
         <v>44857</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="1">
         <v>44857</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="1">
         <v>44864</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="1">
         <v>44864</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="1">
         <v>44864</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="1">
         <v>44864</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="1">
         <v>44864</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="1">
         <v>44864</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="1">
         <v>44864</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="1">
         <v>44871</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="1">
         <v>44871</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="1">
         <v>44871</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="1">
         <v>44871</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="1">
         <v>44871</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="1">
         <v>44871</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="1">
         <v>44871</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="1">
         <v>44871</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="1">
         <v>44871</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="1">
         <v>44871</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="1">
         <v>44871</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="1">
         <v>44871</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="1">
         <v>44871</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="1">
         <v>44871</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="1">
         <v>44878</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="1">
         <v>44878</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="1">
         <v>44878</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="1">
         <v>44878</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="1">
         <v>44878</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="1">
         <v>44878</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="1">
         <v>44878</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="1">
         <v>44878</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="1">
         <v>44878</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="1">
         <v>44878</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="1">
         <v>44878</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="1">
         <v>44892</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="1">
         <v>44892</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="1">
         <v>44892</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="1">
         <v>44892</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="1">
         <v>44892</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="1">
         <v>44899</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="1">
         <v>44899</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="1">
         <v>44899</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="1">
         <v>44899</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="1">
         <v>44899</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="1">
         <v>44899</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="1">
         <v>44899</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="1">
         <v>44899</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="1">
         <v>44899</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="1">
         <v>44899</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="1">
         <v>44899</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="1">
         <v>44899</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="1">
         <v>44899</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="1">
         <v>44906</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="1">
         <v>44906</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="1">
         <v>44906</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="1">
         <v>44906</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="1">
         <v>44906</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="1">
         <v>44906</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="1">
         <v>44906</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="1">
         <v>44906</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="1">
         <v>44906</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="1">
         <v>44906</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="1">
         <v>44906</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="1">
         <v>44906</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="1">
         <v>44906</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="1">
         <v>44906</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="1">
         <v>44906</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="1">
         <v>44906</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="1">
         <v>44906</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="1">
         <v>44913</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="1">
         <v>44913</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="1">
         <v>44913</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="1">
         <v>44913</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="1">
         <v>44913</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="1">
         <v>44913</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="1">
         <v>44913</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="1">
         <v>44913</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="1">
         <v>44913</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="1">
         <v>44913</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="1">
         <v>44913</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="1">
         <v>44913</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="1">
         <v>44913</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="1">
         <v>44913</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="1">
         <v>44913</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="1">
         <v>44913</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" s="1">
         <v>44933</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="1">
         <v>44933</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" s="1">
         <v>44933</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="1">
         <v>44933</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" s="1">
         <v>44933</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" s="1">
         <v>44933</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="1">
         <v>44933</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" s="1">
         <v>44933</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="1">
         <v>44933</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" s="1">
         <v>44933</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="1">
         <v>44933</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="1">
         <v>44933</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="1">
         <v>44933</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="1">
         <v>44933</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="1">
         <v>44933</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" s="1">
         <v>44933</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="1">
         <v>44933</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="1">
         <v>44933</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" s="1">
         <v>44933</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="1">
         <v>44933</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" s="1">
         <v>44933</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" s="1">
         <v>44933</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="1">
         <v>44933</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="1">
         <v>44933</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" s="1">
         <v>44941</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" s="1">
         <v>44941</v>
       </c>
@@ -3803,7 +3803,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" s="1">
         <v>44941</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" s="1">
         <v>44941</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="1">
         <v>44941</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" s="1">
         <v>44941</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" s="1">
         <v>44941</v>
       </c>
@@ -3873,7 +3873,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" s="1">
         <v>44941</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" s="1">
         <v>44941</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="1">
         <v>44941</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="1">
         <v>44941</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="1">
         <v>44941</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" s="1">
         <v>44941</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="1">
         <v>44941</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="1">
         <v>44941</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="1">
         <v>44941</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="1">
         <v>44941</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" s="1">
         <v>44941</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="1">
         <v>44941</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="1">
         <v>44941</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" s="1">
         <v>44955</v>
       </c>
@@ -4069,7 +4069,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" s="1">
         <v>44956</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A249" s="1">
         <v>44956</v>
       </c>
@@ -4097,7 +4097,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" s="1">
         <v>44956</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" s="1">
         <v>44956</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A252" s="1">
         <v>44956</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" s="1">
         <v>44956</v>
       </c>
@@ -4153,7 +4153,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A254" s="1">
         <v>44956</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" s="1">
         <v>44956</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" s="1">
         <v>44956</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" s="1">
         <v>44956</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" s="1">
         <v>44956</v>
       </c>
@@ -4223,7 +4223,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" s="1">
         <v>44956</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" s="1">
         <v>44956</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" s="1">
         <v>44956</v>
       </c>
@@ -4265,7 +4265,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A262" s="1">
         <v>44956</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" s="1">
         <v>44956</v>
       </c>
@@ -4293,7 +4293,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" s="1">
         <v>44956</v>
       </c>
@@ -4307,7 +4307,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" s="1">
         <v>44948</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" s="1">
         <v>44948</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A267" s="1">
         <v>44948</v>
       </c>
@@ -4349,7 +4349,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A268" s="1">
         <v>44948</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A269" s="1">
         <v>44948</v>
       </c>
@@ -4377,7 +4377,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A270" s="1">
         <v>44948</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A271" s="1">
         <v>44948</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A272" s="1">
         <v>44948</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A273" s="1">
         <v>44948</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A274" s="1">
         <v>44948</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A275" s="1">
         <v>44948</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A276" s="1">
         <v>44948</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A277" s="1">
         <v>44948</v>
       </c>
@@ -4489,7 +4489,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" s="1">
         <v>44948</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A279" s="1">
         <v>44948</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A280" s="1">
         <v>44962</v>
       </c>
@@ -4531,7 +4531,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" s="1">
         <v>44962</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A282" s="1">
         <v>44962</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" s="1">
         <v>44962</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" s="1">
         <v>44962</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" s="1">
         <v>44962</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A286" s="1">
         <v>44962</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" s="1">
         <v>44962</v>
       </c>
@@ -4629,7 +4629,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" s="1">
         <v>44962</v>
       </c>
@@ -4643,7 +4643,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" s="1">
         <v>44962</v>
       </c>
@@ -4657,7 +4657,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A290" s="1">
         <v>44962</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" s="1">
         <v>44962</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A292" s="1">
         <v>44962</v>
       </c>
@@ -4699,7 +4699,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A293" s="1">
         <v>44969</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A294" s="1">
         <v>44957</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A295" s="1">
         <v>44969</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A296" s="1">
         <v>44969</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A297" s="1">
         <v>44969</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" s="1">
         <v>44969</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" s="1">
         <v>44969</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A300" s="1">
         <v>44969</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" s="1">
         <v>44969</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" s="1">
         <v>44969</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" s="1">
         <v>44969</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" s="1">
         <v>44969</v>
       </c>
@@ -4867,7 +4867,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A305" s="1">
         <v>44956</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A306" s="1">
         <v>44969</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A307" s="1">
         <v>44976</v>
       </c>
@@ -4909,7 +4909,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A308" s="1">
         <v>44976</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A309" s="1">
         <v>44976</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A310" s="1">
         <v>44976</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A311" s="1">
         <v>44976</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A312" s="1">
         <v>44976</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A313" s="1">
         <v>44976</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A314" s="1">
         <v>44976</v>
       </c>
@@ -5007,7 +5007,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A315" s="1">
         <v>44976</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A316" s="1">
         <v>44983</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A317" s="1">
         <v>44983</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A318" s="1">
         <v>44983</v>
       </c>
@@ -5063,7 +5063,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A319" s="1">
         <v>44983</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A320" s="1">
         <v>44983</v>
       </c>
@@ -5091,7 +5091,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A321" s="1">
         <v>44983</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A322" s="1">
         <v>44983</v>
       </c>
@@ -5119,7 +5119,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A323" s="1">
         <v>44983</v>
       </c>
@@ -5133,7 +5133,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A324" s="1">
         <v>44983</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A325" s="1">
         <v>44983</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A326" s="1">
         <v>44983</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A327" s="1">
         <v>44983</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" s="1">
         <v>44983</v>
       </c>
@@ -5203,7 +5203,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A329" s="1">
         <v>44983</v>
       </c>
@@ -5217,7 +5217,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A330" s="1">
         <v>44983</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A331" s="1">
         <v>44986</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A332" s="1">
         <v>44986</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A333" s="1">
         <v>44986</v>
       </c>
@@ -5273,7 +5273,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A334" s="1">
         <v>44986</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A335" s="1">
         <v>44986</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A336" s="1">
         <v>44986</v>
       </c>
@@ -5315,7 +5315,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A337" s="1">
         <v>44987</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A338" s="1">
         <v>44990</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A339" s="1">
         <v>44990</v>
       </c>
@@ -5357,7 +5357,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A340" s="1">
         <v>44990</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A341" s="1">
         <v>44990</v>
       </c>
@@ -5385,7 +5385,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A342" s="1">
         <v>44990</v>
       </c>
@@ -5399,7 +5399,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A343" s="1">
         <v>44990</v>
       </c>
@@ -5413,7 +5413,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A344" s="1">
         <v>44990</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A345" s="1">
         <v>44990</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A346" s="1">
         <v>44990</v>
       </c>
@@ -5455,7 +5455,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A347" s="1">
         <v>44990</v>
       </c>
@@ -5469,7 +5469,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A348" s="1">
         <v>44990</v>
       </c>
@@ -5483,7 +5483,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A349" s="1">
         <v>44990</v>
       </c>
@@ -5497,7 +5497,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A350" s="1">
         <v>44990</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="351" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A351" s="1">
         <v>44990</v>
       </c>
@@ -5525,7 +5525,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="352" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A352" s="1">
         <v>44996</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A353" s="1">
         <v>44997</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A354" s="1">
         <v>44997</v>
       </c>
@@ -5567,7 +5567,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A355" s="1">
         <v>44997</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="356" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A356" s="1">
         <v>44997</v>
       </c>
@@ -5595,7 +5595,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="357" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A357" s="1">
         <v>44997</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A358" s="1">
         <v>44997</v>
       </c>
@@ -5623,7 +5623,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A359" s="1">
         <v>44997</v>
       </c>
@@ -5637,7 +5637,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A360" s="1">
         <v>44997</v>
       </c>
@@ -5651,7 +5651,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A361" s="1">
         <v>44997</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A362" s="1">
         <v>44997</v>
       </c>
@@ -5679,7 +5679,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A363" s="1">
         <v>44997</v>
       </c>
@@ -5693,7 +5693,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A364" s="1">
         <v>44997</v>
       </c>
@@ -5707,7 +5707,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A365" s="1">
         <v>44997</v>
       </c>
@@ -5721,7 +5721,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A366" s="1">
         <v>45000</v>
       </c>
@@ -5735,7 +5735,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="367" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A367" s="1">
         <v>45000</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="368" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A368" s="1">
         <v>45010</v>
       </c>
@@ -5763,7 +5763,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="369" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A369" s="1">
         <v>45011</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="370" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A370" s="1">
         <v>45011</v>
       </c>
@@ -5791,7 +5791,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="371" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A371" s="1">
         <v>45011</v>
       </c>
@@ -5805,7 +5805,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="372" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A372" s="1">
         <v>45011</v>
       </c>
@@ -5819,7 +5819,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="373" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A373" s="1">
         <v>45011</v>
       </c>
@@ -5833,7 +5833,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="374" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A374" s="1">
         <v>45011</v>
       </c>
@@ -5847,7 +5847,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="375" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A375" s="1">
         <v>45018</v>
       </c>
@@ -5861,7 +5861,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="376" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A376" s="1">
         <v>45018</v>
       </c>
@@ -5875,7 +5875,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="377" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A377" s="1">
         <v>45018</v>
       </c>
@@ -5889,7 +5889,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="378" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A378" s="1">
         <v>45018</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="379" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A379" s="1">
         <v>45018</v>
       </c>
@@ -5917,7 +5917,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="380" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A380" s="1">
         <v>45018</v>
       </c>
@@ -5931,7 +5931,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="381" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A381" s="1">
         <v>45018</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="382" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A382" s="1">
         <v>45018</v>
       </c>
@@ -5959,7 +5959,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="383" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A383" s="1">
         <v>45018</v>
       </c>
@@ -5973,7 +5973,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="384" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A384" s="1">
         <v>45032</v>
       </c>
@@ -5987,7 +5987,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="385" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A385" s="1">
         <v>45032</v>
       </c>
@@ -6001,7 +6001,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="386" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A386" s="1">
         <v>45032</v>
       </c>
@@ -6015,7 +6015,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="387" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A387" s="1">
         <v>45032</v>
       </c>
@@ -6029,7 +6029,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="388" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A388" s="1">
         <v>45032</v>
       </c>
@@ -6043,7 +6043,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="389" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A389" s="1">
         <v>45032</v>
       </c>
@@ -6057,7 +6057,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="390" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A390" s="1">
         <v>45032</v>
       </c>
@@ -6071,7 +6071,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="391" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A391" s="1">
         <v>45032</v>
       </c>
@@ -6085,7 +6085,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="392" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A392" s="1">
         <v>45032</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="393" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A393" s="1">
         <v>45032</v>
       </c>
@@ -6113,7 +6113,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="394" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A394" s="1">
         <v>45032</v>
       </c>
@@ -6127,7 +6127,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="395" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A395" s="1">
         <v>45032</v>
       </c>
@@ -6141,7 +6141,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="396" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A396" s="1">
         <v>45032</v>
       </c>
@@ -6155,7 +6155,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="397" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A397" s="1">
         <v>45039</v>
       </c>
@@ -6169,7 +6169,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="398" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A398" s="1">
         <v>45039</v>
       </c>
@@ -6183,7 +6183,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="399" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A399" s="1">
         <v>45039</v>
       </c>
@@ -6197,7 +6197,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="400" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A400" s="1">
         <v>45039</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="401" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A401" s="1">
         <v>45039</v>
       </c>
@@ -6225,7 +6225,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="402" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A402" s="1">
         <v>45039</v>
       </c>
@@ -6239,7 +6239,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="403" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A403" s="1">
         <v>45046</v>
       </c>
@@ -6253,7 +6253,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="404" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A404" s="1">
         <v>45046</v>
       </c>
@@ -6267,7 +6267,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="405" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A405" s="1">
         <v>45046</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="406" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A406" s="1">
         <v>45046</v>
       </c>
@@ -6295,7 +6295,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="407" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A407" s="1">
         <v>45046</v>
       </c>
@@ -6309,7 +6309,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="408" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A408" s="1">
         <v>45046</v>
       </c>
@@ -6323,7 +6323,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="409" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A409" s="1">
         <v>45046</v>
       </c>
@@ -6337,7 +6337,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="410" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A410" s="1">
         <v>45046</v>
       </c>
@@ -6351,7 +6351,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="411" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A411" s="1">
         <v>45053</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="412" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A412" s="1">
         <v>45053</v>
       </c>
@@ -6379,7 +6379,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="413" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A413" s="1">
         <v>45053</v>
       </c>
@@ -6393,7 +6393,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="414" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A414" s="1">
         <v>45053</v>
       </c>
@@ -6407,7 +6407,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="415" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A415" s="1">
         <v>45053</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="416" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A416" s="1">
         <v>45053</v>
       </c>
@@ -6435,7 +6435,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="417" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A417" s="1">
         <v>45060</v>
       </c>
@@ -6449,7 +6449,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="418" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A418" s="1">
         <v>45060</v>
       </c>
@@ -6463,7 +6463,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="419" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A419" s="1">
         <v>45060</v>
       </c>
@@ -6477,7 +6477,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="420" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A420" s="1">
         <v>45060</v>
       </c>
@@ -6491,7 +6491,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="421" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A421" s="1">
         <v>45060</v>
       </c>
@@ -6505,7 +6505,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="422" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A422" s="1">
         <v>45060</v>
       </c>
@@ -6519,7 +6519,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="423" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A423" s="1">
         <v>45060</v>
       </c>
@@ -6550,14 +6550,14 @@
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.68359375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.47265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.47265625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>44710</v>
       </c>
@@ -6579,7 +6579,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>44724</v>
       </c>
@@ -6590,7 +6590,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>44731</v>
       </c>
@@ -6601,7 +6601,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>44738</v>
       </c>
@@ -6612,7 +6612,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>44752</v>
       </c>
@@ -6623,7 +6623,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>44766</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>44795</v>
       </c>
@@ -6645,7 +6645,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>44815</v>
       </c>
@@ -6656,7 +6656,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>44843</v>
       </c>
@@ -6667,7 +6667,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>44857</v>
       </c>
@@ -6678,7 +6678,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>44857</v>
       </c>
@@ -6689,7 +6689,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>44899</v>
       </c>
@@ -6700,7 +6700,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>44892</v>
       </c>
@@ -6711,7 +6711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>44878</v>
       </c>
@@ -6722,7 +6722,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>44906</v>
       </c>
@@ -6733,7 +6733,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
         <v>44913</v>
       </c>
@@ -6744,7 +6744,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1">
         <v>44911</v>
       </c>
@@ -6755,7 +6755,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1">
         <v>44933</v>
       </c>
@@ -6766,7 +6766,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1">
         <v>44941</v>
       </c>
@@ -6777,7 +6777,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1">
         <v>44948</v>
       </c>
@@ -6788,7 +6788,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1">
         <v>44955</v>
       </c>
@@ -6799,7 +6799,7 @@
         <v>3775</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1">
         <v>44962</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1">
         <v>44969</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1">
         <v>44976</v>
       </c>
@@ -6832,7 +6832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1">
         <v>44983</v>
       </c>
@@ -6843,7 +6843,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1">
         <v>44986</v>
       </c>
@@ -6854,7 +6854,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1">
         <v>44990</v>
       </c>
@@ -6866,7 +6866,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1">
         <v>44990</v>
       </c>
@@ -6877,7 +6877,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1">
         <v>44990</v>
       </c>
@@ -6888,7 +6888,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1">
         <v>44997</v>
       </c>
@@ -6899,7 +6899,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1">
         <v>45004</v>
       </c>
@@ -6910,7 +6910,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1">
         <v>45011</v>
       </c>
@@ -6921,7 +6921,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1">
         <v>45018</v>
       </c>
@@ -6932,7 +6932,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1">
         <v>45018</v>
       </c>
@@ -6943,7 +6943,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1">
         <v>45032</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1">
         <v>45032</v>
       </c>
@@ -6965,7 +6965,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1">
         <v>45046</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1">
         <v>45053</v>
       </c>
@@ -6988,7 +6988,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1">
         <v>45060</v>
       </c>
@@ -7009,17 +7009,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCA2D2E-DEE9-4BB9-9EC2-45DF3BC6F5C1}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.47265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.47265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -7039,7 +7039,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3">
         <v>45060</v>
       </c>
@@ -7069,12 +7069,12 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.47265625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -7094,7 +7094,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3">
         <v>44906</v>
       </c>
@@ -7111,7 +7111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
         <v>44913</v>
       </c>
@@ -7128,7 +7128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
         <v>44933</v>
       </c>
@@ -7145,7 +7145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>44948</v>
       </c>
@@ -7162,7 +7162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>44969</v>
       </c>
@@ -7179,7 +7179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>44990</v>
       </c>
@@ -7199,7 +7199,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3">
         <v>44983</v>
       </c>
@@ -7219,7 +7219,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3">
         <v>45018</v>
       </c>
@@ -7239,7 +7239,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3">
         <v>44997</v>
       </c>

</xml_diff>

<commit_message>
Actualización al 21 de mayo
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Backup/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{5FBF4DC7-46AB-CD4C-8342-9A9041627525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2DB3F08-E223-C146-823B-A873C31D6F09}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="13_ncr:1_{5FBF4DC7-46AB-CD4C-8342-9A9041627525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{985CD627-1A3C-6048-8E63-66CFF677FCD2}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="69">
   <si>
     <t>Alfredo</t>
   </si>
@@ -240,6 +240,15 @@
   </si>
   <si>
     <t>Gustavo</t>
+  </si>
+  <si>
+    <t>Cogió un pique y picó la pelota muy duro</t>
+  </si>
+  <si>
+    <t>Empanadas</t>
+  </si>
+  <si>
+    <t>Aporte mono (pintar cancha)</t>
   </si>
 </sst>
 </file>
@@ -598,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D424"/>
+  <dimension ref="A1:D431"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A403" workbookViewId="0">
-      <selection activeCell="A425" sqref="A425"/>
+    <sheetView tabSelected="1" topLeftCell="A411" workbookViewId="0">
+      <selection activeCell="C428" sqref="C428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6547,6 +6556,104 @@
         <v>34</v>
       </c>
     </row>
+    <row r="425" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A425" s="1">
+        <v>45067</v>
+      </c>
+      <c r="B425" t="s">
+        <v>2</v>
+      </c>
+      <c r="C425">
+        <v>50</v>
+      </c>
+      <c r="D425" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A426" s="1">
+        <v>45067</v>
+      </c>
+      <c r="B426" t="s">
+        <v>10</v>
+      </c>
+      <c r="C426">
+        <v>100</v>
+      </c>
+      <c r="D426" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A427" s="1">
+        <v>45067</v>
+      </c>
+      <c r="B427" t="s">
+        <v>15</v>
+      </c>
+      <c r="C427">
+        <v>100</v>
+      </c>
+      <c r="D427" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A428" s="1">
+        <v>45067</v>
+      </c>
+      <c r="B428" t="s">
+        <v>18</v>
+      </c>
+      <c r="C428">
+        <v>100</v>
+      </c>
+      <c r="D428" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A429" s="1">
+        <v>45067</v>
+      </c>
+      <c r="B429" t="s">
+        <v>24</v>
+      </c>
+      <c r="C429">
+        <v>100</v>
+      </c>
+      <c r="D429" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A430" s="1">
+        <v>45067</v>
+      </c>
+      <c r="B430" t="s">
+        <v>0</v>
+      </c>
+      <c r="C430">
+        <v>100</v>
+      </c>
+      <c r="D430" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A431" s="1">
+        <v>45067</v>
+      </c>
+      <c r="B431" t="s">
+        <v>1</v>
+      </c>
+      <c r="C431">
+        <v>100</v>
+      </c>
+      <c r="D431" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
@@ -6558,10 +6665,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7013,6 +7120,39 @@
         <v>150</v>
       </c>
     </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>45067</v>
+      </c>
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="4">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>45067</v>
+      </c>
+      <c r="B42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" s="4">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>45067</v>
+      </c>
+      <c r="B43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="4">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7021,10 +7161,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCA2D2E-DEE9-4BB9-9EC2-45DF3BC6F5C1}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7068,6 +7208,23 @@
       </c>
       <c r="F2" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>45067</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización al 10 de junio
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Backup/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="13_ncr:1_{5FBF4DC7-46AB-CD4C-8342-9A9041627525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{985CD627-1A3C-6048-8E63-66CFF677FCD2}"/>
+  <xr:revisionPtr revIDLastSave="153" documentId="13_ncr:1_{5FBF4DC7-46AB-CD4C-8342-9A9041627525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33313545-8B88-0748-90DF-53305AB5208C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="70">
   <si>
     <t>Alfredo</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>Aporte mono (pintar cancha)</t>
+  </si>
+  <si>
+    <t>kukito</t>
   </si>
 </sst>
 </file>
@@ -607,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D431"/>
+  <dimension ref="A1:D443"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A411" workbookViewId="0">
-      <selection activeCell="C428" sqref="C428"/>
+    <sheetView tabSelected="1" topLeftCell="A423" workbookViewId="0">
+      <selection activeCell="A441" sqref="A441:A443"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6654,6 +6657,174 @@
         <v>34</v>
       </c>
     </row>
+    <row r="432" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A432" s="1">
+        <v>45081</v>
+      </c>
+      <c r="B432" t="s">
+        <v>1</v>
+      </c>
+      <c r="C432">
+        <v>100</v>
+      </c>
+      <c r="D432" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A433" s="1">
+        <v>45081</v>
+      </c>
+      <c r="B433" t="s">
+        <v>2</v>
+      </c>
+      <c r="C433">
+        <v>200</v>
+      </c>
+      <c r="D433" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A434" s="1">
+        <v>45081</v>
+      </c>
+      <c r="B434" t="s">
+        <v>18</v>
+      </c>
+      <c r="C434">
+        <v>100</v>
+      </c>
+      <c r="D434" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A435" s="1">
+        <v>45081</v>
+      </c>
+      <c r="B435" t="s">
+        <v>24</v>
+      </c>
+      <c r="C435">
+        <v>100</v>
+      </c>
+      <c r="D435" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A436" s="1">
+        <v>45081</v>
+      </c>
+      <c r="B436" t="s">
+        <v>69</v>
+      </c>
+      <c r="C436">
+        <v>50</v>
+      </c>
+      <c r="D436" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A437" s="1">
+        <v>45081</v>
+      </c>
+      <c r="B437" t="s">
+        <v>16</v>
+      </c>
+      <c r="C437">
+        <v>400</v>
+      </c>
+      <c r="D437" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A438" s="1">
+        <v>45081</v>
+      </c>
+      <c r="B438" t="s">
+        <v>0</v>
+      </c>
+      <c r="C438">
+        <v>100</v>
+      </c>
+      <c r="D438" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A439" s="1">
+        <v>45081</v>
+      </c>
+      <c r="B439" t="s">
+        <v>11</v>
+      </c>
+      <c r="C439" s="2">
+        <v>300</v>
+      </c>
+      <c r="D439" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A440" s="1">
+        <v>45074</v>
+      </c>
+      <c r="B440" t="s">
+        <v>37</v>
+      </c>
+      <c r="C440" s="2">
+        <v>100</v>
+      </c>
+      <c r="D440" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A441" s="1">
+        <v>45074</v>
+      </c>
+      <c r="B441" t="s">
+        <v>14</v>
+      </c>
+      <c r="C441" s="2">
+        <v>100</v>
+      </c>
+      <c r="D441" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A442" s="1">
+        <v>45074</v>
+      </c>
+      <c r="B442" t="s">
+        <v>27</v>
+      </c>
+      <c r="C442" s="2">
+        <v>100</v>
+      </c>
+      <c r="D442" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A443" s="1">
+        <v>45074</v>
+      </c>
+      <c r="B443" t="s">
+        <v>1</v>
+      </c>
+      <c r="C443" s="2">
+        <v>85</v>
+      </c>
+      <c r="D443" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
@@ -6665,10 +6836,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="A30" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7151,6 +7322,17 @@
       </c>
       <c r="C43" s="4">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>45081</v>
+      </c>
+      <c r="B44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="4">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización al 11 de junio de 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Backup/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="13_ncr:1_{5FBF4DC7-46AB-CD4C-8342-9A9041627525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33313545-8B88-0748-90DF-53305AB5208C}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="13_ncr:1_{5FBF4DC7-46AB-CD4C-8342-9A9041627525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B58D567D-81EE-6B44-A849-903C34FCA053}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="71">
   <si>
     <t>Alfredo</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>kukito</t>
+  </si>
+  <si>
+    <t>Neverita</t>
   </si>
 </sst>
 </file>
@@ -610,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D443"/>
+  <dimension ref="A1:D454"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A423" workbookViewId="0">
-      <selection activeCell="A441" sqref="A441:A443"/>
+    <sheetView tabSelected="1" topLeftCell="A440" workbookViewId="0">
+      <selection activeCell="C453" sqref="C453"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6825,6 +6828,160 @@
         <v>34</v>
       </c>
     </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A444" s="1">
+        <v>45088</v>
+      </c>
+      <c r="B444" t="s">
+        <v>18</v>
+      </c>
+      <c r="C444" s="2">
+        <v>100</v>
+      </c>
+      <c r="D444" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A445" s="1">
+        <v>45088</v>
+      </c>
+      <c r="B445" t="s">
+        <v>2</v>
+      </c>
+      <c r="C445" s="2">
+        <v>100</v>
+      </c>
+      <c r="D445" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A446" s="1">
+        <v>45088</v>
+      </c>
+      <c r="B446" t="s">
+        <v>27</v>
+      </c>
+      <c r="C446" s="2">
+        <v>100</v>
+      </c>
+      <c r="D446" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A447" s="1">
+        <v>45088</v>
+      </c>
+      <c r="B447" t="s">
+        <v>1</v>
+      </c>
+      <c r="C447" s="2">
+        <v>100</v>
+      </c>
+      <c r="D447" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A448" s="1">
+        <v>45088</v>
+      </c>
+      <c r="B448" t="s">
+        <v>10</v>
+      </c>
+      <c r="C448" s="2">
+        <v>50</v>
+      </c>
+      <c r="D448" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A449" s="1">
+        <v>45088</v>
+      </c>
+      <c r="B449" t="s">
+        <v>65</v>
+      </c>
+      <c r="C449" s="2">
+        <v>50</v>
+      </c>
+      <c r="D449" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A450" s="1">
+        <v>45088</v>
+      </c>
+      <c r="B450" t="s">
+        <v>14</v>
+      </c>
+      <c r="C450" s="2">
+        <v>100</v>
+      </c>
+      <c r="D450" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A451" s="1">
+        <v>45088</v>
+      </c>
+      <c r="B451" t="s">
+        <v>13</v>
+      </c>
+      <c r="C451" s="2">
+        <v>800</v>
+      </c>
+      <c r="D451" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A452" s="1">
+        <v>45088</v>
+      </c>
+      <c r="B452" t="s">
+        <v>19</v>
+      </c>
+      <c r="C452" s="2">
+        <v>250</v>
+      </c>
+      <c r="D452" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A453" s="1">
+        <v>45088</v>
+      </c>
+      <c r="B453" t="s">
+        <v>15</v>
+      </c>
+      <c r="C453" s="2">
+        <v>500</v>
+      </c>
+      <c r="D453" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A454" s="1">
+        <v>45088</v>
+      </c>
+      <c r="B454" t="s">
+        <v>23</v>
+      </c>
+      <c r="C454" s="2">
+        <v>200</v>
+      </c>
+      <c r="D454" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
@@ -6836,10 +6993,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView topLeftCell="A30" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7333,6 +7490,28 @@
       </c>
       <c r="C44" s="4">
         <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>45088</v>
+      </c>
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>45089</v>
+      </c>
+      <c r="B46" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" s="4">
+        <v>4000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización al 28 de junio 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Backup/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="191" documentId="13_ncr:1_{5FBF4DC7-46AB-CD4C-8342-9A9041627525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B58D567D-81EE-6B44-A849-903C34FCA053}"/>
+  <xr:revisionPtr revIDLastSave="196" documentId="13_ncr:1_{5FBF4DC7-46AB-CD4C-8342-9A9041627525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E624762-CF9A-3246-8E0D-BDECC0109DF0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ingreso" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="71">
   <si>
     <t>Alfredo</t>
   </si>
@@ -615,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D454"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A440" workbookViewId="0">
+    <sheetView topLeftCell="A440" workbookViewId="0">
       <selection activeCell="C453" sqref="C453"/>
     </sheetView>
   </sheetViews>
@@ -6993,10 +6993,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7497,10 +7497,10 @@
         <v>45088</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C45" s="4">
-        <v>150</v>
+        <v>950</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -7512,6 +7512,17 @@
       </c>
       <c r="C46" s="4">
         <v>4000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>45095</v>
+      </c>
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="4">
+        <v>800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización al 25 de junio 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Backup/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="196" documentId="13_ncr:1_{5FBF4DC7-46AB-CD4C-8342-9A9041627525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E624762-CF9A-3246-8E0D-BDECC0109DF0}"/>
+  <xr:revisionPtr revIDLastSave="207" documentId="13_ncr:1_{5FBF4DC7-46AB-CD4C-8342-9A9041627525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D3B92EF-3A3F-3C47-A016-DF5A8D7CB1DD}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ingreso" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="71">
   <si>
     <t>Alfredo</t>
   </si>
@@ -613,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D454"/>
+  <dimension ref="A1:D463"/>
   <sheetViews>
-    <sheetView topLeftCell="A440" workbookViewId="0">
-      <selection activeCell="C453" sqref="C453"/>
+    <sheetView tabSelected="1" topLeftCell="A442" workbookViewId="0">
+      <selection activeCell="C460" sqref="C460"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6982,6 +6982,132 @@
         <v>34</v>
       </c>
     </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A455" s="1">
+        <v>45101</v>
+      </c>
+      <c r="B455" t="s">
+        <v>8</v>
+      </c>
+      <c r="C455" s="2">
+        <v>200</v>
+      </c>
+      <c r="D455" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A456" s="1">
+        <v>45101</v>
+      </c>
+      <c r="B456" t="s">
+        <v>23</v>
+      </c>
+      <c r="C456">
+        <v>100</v>
+      </c>
+      <c r="D456" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A457" s="1">
+        <v>45101</v>
+      </c>
+      <c r="B457" t="s">
+        <v>18</v>
+      </c>
+      <c r="C457">
+        <v>100</v>
+      </c>
+      <c r="D457" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A458" s="1">
+        <v>45101</v>
+      </c>
+      <c r="B458" t="s">
+        <v>1</v>
+      </c>
+      <c r="C458">
+        <v>100</v>
+      </c>
+      <c r="D458" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A459" s="1">
+        <v>45101</v>
+      </c>
+      <c r="B459" t="s">
+        <v>16</v>
+      </c>
+      <c r="C459">
+        <v>250</v>
+      </c>
+      <c r="D459" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A460" s="1">
+        <v>45101</v>
+      </c>
+      <c r="B460" t="s">
+        <v>11</v>
+      </c>
+      <c r="C460">
+        <v>100</v>
+      </c>
+      <c r="D460" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A461" s="1">
+        <v>45101</v>
+      </c>
+      <c r="B461" t="s">
+        <v>27</v>
+      </c>
+      <c r="C461">
+        <v>100</v>
+      </c>
+      <c r="D461" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A462" s="1">
+        <v>45101</v>
+      </c>
+      <c r="B462" t="s">
+        <v>14</v>
+      </c>
+      <c r="C462">
+        <v>100</v>
+      </c>
+      <c r="D462" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A463" s="1">
+        <v>45101</v>
+      </c>
+      <c r="B463" t="s">
+        <v>9</v>
+      </c>
+      <c r="C463">
+        <v>600</v>
+      </c>
+      <c r="D463" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
@@ -6993,10 +7119,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView topLeftCell="A29" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7523,6 +7649,17 @@
       </c>
       <c r="C47" s="4">
         <v>800</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>45101</v>
+      </c>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="4">
+        <v>940</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización al 3 de julio de 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Backup/proyectos_r/1-personales/goat/website/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Desktop/goat_website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="13_ncr:1_{5FBF4DC7-46AB-CD4C-8342-9A9041627525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D3B92EF-3A3F-3C47-A016-DF5A8D7CB1DD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605282FA-01C3-D545-8BA8-828FECE85CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="72">
   <si>
     <t>Alfredo</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>Neverita</t>
+  </si>
+  <si>
+    <t>Le pitaron 3 segundos e hizo un pique</t>
   </si>
 </sst>
 </file>
@@ -613,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D463"/>
+  <dimension ref="A1:D473"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A442" workbookViewId="0">
-      <selection activeCell="C460" sqref="C460"/>
+    <sheetView tabSelected="1" topLeftCell="A451" workbookViewId="0">
+      <selection activeCell="A473" sqref="A473"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7108,6 +7111,146 @@
         <v>34</v>
       </c>
     </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A464" s="1">
+        <v>45109</v>
+      </c>
+      <c r="B464" t="s">
+        <v>37</v>
+      </c>
+      <c r="C464" s="2">
+        <v>100</v>
+      </c>
+      <c r="D464" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A465" s="1">
+        <v>45109</v>
+      </c>
+      <c r="B465" t="s">
+        <v>2</v>
+      </c>
+      <c r="C465" s="2">
+        <v>100</v>
+      </c>
+      <c r="D465" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A466" s="1">
+        <v>45109</v>
+      </c>
+      <c r="B466" t="s">
+        <v>1</v>
+      </c>
+      <c r="C466" s="2">
+        <v>100</v>
+      </c>
+      <c r="D466" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A467" s="1">
+        <v>45109</v>
+      </c>
+      <c r="B467" t="s">
+        <v>7</v>
+      </c>
+      <c r="C467" s="2">
+        <v>500</v>
+      </c>
+      <c r="D467" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A468" s="1">
+        <v>45109</v>
+      </c>
+      <c r="B468" t="s">
+        <v>3</v>
+      </c>
+      <c r="C468" s="2">
+        <v>100</v>
+      </c>
+      <c r="D468" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A469" s="1">
+        <v>45109</v>
+      </c>
+      <c r="B469" t="s">
+        <v>8</v>
+      </c>
+      <c r="C469" s="2">
+        <v>100</v>
+      </c>
+      <c r="D469" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A470" s="1">
+        <v>45109</v>
+      </c>
+      <c r="B470" t="s">
+        <v>26</v>
+      </c>
+      <c r="C470" s="2">
+        <v>50</v>
+      </c>
+      <c r="D470" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A471" s="1">
+        <v>45109</v>
+      </c>
+      <c r="B471" t="s">
+        <v>15</v>
+      </c>
+      <c r="C471" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D471" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A472" s="1">
+        <v>45109</v>
+      </c>
+      <c r="B472" t="s">
+        <v>10</v>
+      </c>
+      <c r="C472" s="2">
+        <v>300</v>
+      </c>
+      <c r="D472" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A473" s="1">
+        <v>45109</v>
+      </c>
+      <c r="B473" t="s">
+        <v>40</v>
+      </c>
+      <c r="C473" s="2">
+        <v>900</v>
+      </c>
+      <c r="D473" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
@@ -7119,10 +7262,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView topLeftCell="A33" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7662,6 +7805,17 @@
         <v>940</v>
       </c>
     </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>45101</v>
+      </c>
+      <c r="B49" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" s="4">
+        <v>940</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7670,10 +7824,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCA2D2E-DEE9-4BB9-9EC2-45DF3BC6F5C1}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7734,6 +7888,23 @@
       </c>
       <c r="F3" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>45109</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización al 8 de julio de 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Desktop/goat_website/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/[5] R projects/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605282FA-01C3-D545-8BA8-828FECE85CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{605282FA-01C3-D545-8BA8-828FECE85CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01A2F23C-A395-C44D-889C-44DB37E74974}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="72">
   <si>
     <t>Alfredo</t>
   </si>
@@ -616,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D473"/>
+  <dimension ref="A1:D482"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A451" workbookViewId="0">
-      <selection activeCell="A473" sqref="A473"/>
+    <sheetView tabSelected="1" topLeftCell="A469" workbookViewId="0">
+      <selection activeCell="A482" sqref="A482"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7251,6 +7251,132 @@
         <v>34</v>
       </c>
     </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A474" s="1">
+        <v>45115</v>
+      </c>
+      <c r="B474" t="s">
+        <v>23</v>
+      </c>
+      <c r="C474" s="2">
+        <v>200</v>
+      </c>
+      <c r="D474" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A475" s="1">
+        <v>45115</v>
+      </c>
+      <c r="B475" t="s">
+        <v>1</v>
+      </c>
+      <c r="C475" s="2">
+        <v>100</v>
+      </c>
+      <c r="D475" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A476" s="1">
+        <v>45115</v>
+      </c>
+      <c r="B476" t="s">
+        <v>40</v>
+      </c>
+      <c r="C476" s="2">
+        <v>80</v>
+      </c>
+      <c r="D476" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A477" s="1">
+        <v>45115</v>
+      </c>
+      <c r="B477" t="s">
+        <v>2</v>
+      </c>
+      <c r="C477" s="2">
+        <v>100</v>
+      </c>
+      <c r="D477" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A478" s="1">
+        <v>45115</v>
+      </c>
+      <c r="B478" t="s">
+        <v>8</v>
+      </c>
+      <c r="C478" s="2">
+        <v>100</v>
+      </c>
+      <c r="D478" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A479" s="1">
+        <v>45115</v>
+      </c>
+      <c r="B479" t="s">
+        <v>3</v>
+      </c>
+      <c r="C479" s="2">
+        <v>200</v>
+      </c>
+      <c r="D479" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A480" s="1">
+        <v>45115</v>
+      </c>
+      <c r="B480" t="s">
+        <v>18</v>
+      </c>
+      <c r="C480" s="2">
+        <v>100</v>
+      </c>
+      <c r="D480" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A481" s="1">
+        <v>45115</v>
+      </c>
+      <c r="B481" t="s">
+        <v>30</v>
+      </c>
+      <c r="C481" s="2">
+        <v>100</v>
+      </c>
+      <c r="D481" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="482" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A482" s="1">
+        <v>45115</v>
+      </c>
+      <c r="B482" t="s">
+        <v>11</v>
+      </c>
+      <c r="C482" s="2">
+        <v>300</v>
+      </c>
+      <c r="D482" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
@@ -7262,7 +7388,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView topLeftCell="A33" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A49" sqref="A49"/>
@@ -7807,13 +7933,24 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>45101</v>
+        <v>45109</v>
       </c>
       <c r="B49" t="s">
         <v>46</v>
       </c>
       <c r="C49" s="4">
         <v>940</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>45115</v>
+      </c>
+      <c r="B50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50" s="4">
+        <v>941</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización al 16 de julio 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/[5] R projects/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{605282FA-01C3-D545-8BA8-828FECE85CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01A2F23C-A395-C44D-889C-44DB37E74974}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{605282FA-01C3-D545-8BA8-828FECE85CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEF14118-3BF4-0840-AB1F-29141708B38E}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="75">
   <si>
     <t>Alfredo</t>
   </si>
@@ -258,6 +258,15 @@
   </si>
   <si>
     <t>Le pitaron 3 segundos e hizo un pique</t>
+  </si>
+  <si>
+    <t>chamo</t>
+  </si>
+  <si>
+    <t>Fernando</t>
+  </si>
+  <si>
+    <t>Arbitro y agua</t>
   </si>
 </sst>
 </file>
@@ -616,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D482"/>
+  <dimension ref="A1:D492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A469" workbookViewId="0">
-      <selection activeCell="A482" sqref="A482"/>
+    <sheetView tabSelected="1" topLeftCell="A472" workbookViewId="0">
+      <selection activeCell="A492" sqref="A492"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7312,7 +7321,7 @@
         <v>45115</v>
       </c>
       <c r="B478" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="C478" s="2">
         <v>100</v>
@@ -7374,6 +7383,146 @@
         <v>300</v>
       </c>
       <c r="D482" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="483" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A483" s="1">
+        <v>45123</v>
+      </c>
+      <c r="B483" t="s">
+        <v>28</v>
+      </c>
+      <c r="C483">
+        <v>100</v>
+      </c>
+      <c r="D483" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="484" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A484" s="1">
+        <v>45123</v>
+      </c>
+      <c r="B484" t="s">
+        <v>18</v>
+      </c>
+      <c r="C484">
+        <v>100</v>
+      </c>
+      <c r="D484" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="485" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A485" s="1">
+        <v>45123</v>
+      </c>
+      <c r="B485" t="s">
+        <v>72</v>
+      </c>
+      <c r="C485">
+        <v>100</v>
+      </c>
+      <c r="D485" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="486" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A486" s="1">
+        <v>45123</v>
+      </c>
+      <c r="B486" t="s">
+        <v>8</v>
+      </c>
+      <c r="C486">
+        <v>300</v>
+      </c>
+      <c r="D486" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A487" s="1">
+        <v>45123</v>
+      </c>
+      <c r="B487" t="s">
+        <v>73</v>
+      </c>
+      <c r="C487">
+        <v>100</v>
+      </c>
+      <c r="D487" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="488" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A488" s="1">
+        <v>45123</v>
+      </c>
+      <c r="B488" t="s">
+        <v>14</v>
+      </c>
+      <c r="C488">
+        <v>100</v>
+      </c>
+      <c r="D488" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="489" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A489" s="1">
+        <v>45123</v>
+      </c>
+      <c r="B489" t="s">
+        <v>1</v>
+      </c>
+      <c r="C489">
+        <v>100</v>
+      </c>
+      <c r="D489" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="490" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A490" s="1">
+        <v>45123</v>
+      </c>
+      <c r="B490" t="s">
+        <v>24</v>
+      </c>
+      <c r="C490">
+        <v>200</v>
+      </c>
+      <c r="D490" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="491" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A491" s="1">
+        <v>45123</v>
+      </c>
+      <c r="B491" t="s">
+        <v>27</v>
+      </c>
+      <c r="C491" s="2">
+        <v>400</v>
+      </c>
+      <c r="D491" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="492" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A492" s="1">
+        <v>45123</v>
+      </c>
+      <c r="B492" t="s">
+        <v>19</v>
+      </c>
+      <c r="C492" s="2">
+        <v>250</v>
+      </c>
+      <c r="D492" t="s">
         <v>34</v>
       </c>
     </row>
@@ -7388,10 +7537,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView topLeftCell="A33" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7951,6 +8100,17 @@
       </c>
       <c r="C50" s="4">
         <v>941</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>45123</v>
+      </c>
+      <c r="B51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="4">
+        <v>1100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización al 29 de julio
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/[5] R projects/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{605282FA-01C3-D545-8BA8-828FECE85CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEF14118-3BF4-0840-AB1F-29141708B38E}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{605282FA-01C3-D545-8BA8-828FECE85CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAE2EF19-BD25-6F44-8A6F-5826C8B87C75}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="76">
   <si>
     <t>Alfredo</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>Arbitro y agua</t>
+  </si>
+  <si>
+    <t>Pizarra</t>
   </si>
 </sst>
 </file>
@@ -625,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D492"/>
+  <dimension ref="A1:D499"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A472" workbookViewId="0">
-      <selection activeCell="A492" sqref="A492"/>
+    <sheetView tabSelected="1" topLeftCell="A480" workbookViewId="0">
+      <selection activeCell="A500" sqref="A500"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7526,6 +7529,104 @@
         <v>34</v>
       </c>
     </row>
+    <row r="493" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A493" s="1">
+        <v>45130</v>
+      </c>
+      <c r="B493" t="s">
+        <v>27</v>
+      </c>
+      <c r="C493" s="2">
+        <v>400</v>
+      </c>
+      <c r="D493" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="494" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A494" s="1">
+        <v>45130</v>
+      </c>
+      <c r="B494" t="s">
+        <v>2</v>
+      </c>
+      <c r="C494">
+        <v>200</v>
+      </c>
+      <c r="D494" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="495" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A495" s="1">
+        <v>45130</v>
+      </c>
+      <c r="B495" t="s">
+        <v>16</v>
+      </c>
+      <c r="C495">
+        <v>190</v>
+      </c>
+      <c r="D495" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="496" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A496" s="1">
+        <v>45130</v>
+      </c>
+      <c r="B496" t="s">
+        <v>14</v>
+      </c>
+      <c r="C496">
+        <v>100</v>
+      </c>
+      <c r="D496" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="497" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A497" s="1">
+        <v>45130</v>
+      </c>
+      <c r="B497" t="s">
+        <v>28</v>
+      </c>
+      <c r="C497">
+        <v>100</v>
+      </c>
+      <c r="D497" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="498" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A498" s="1">
+        <v>45130</v>
+      </c>
+      <c r="B498" t="s">
+        <v>12</v>
+      </c>
+      <c r="C498">
+        <v>1600</v>
+      </c>
+      <c r="D498" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="499" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A499" s="1">
+        <v>45136</v>
+      </c>
+      <c r="B499" t="s">
+        <v>20</v>
+      </c>
+      <c r="C499" s="2">
+        <v>2100</v>
+      </c>
+      <c r="D499" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
@@ -7537,10 +7638,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView topLeftCell="A35" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8111,6 +8212,28 @@
       </c>
       <c r="C51" s="4">
         <v>1100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>45130</v>
+      </c>
+      <c r="B52" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" s="4">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>45130</v>
+      </c>
+      <c r="B53" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="4">
+        <v>1600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update al 02 de octubre 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/[5] R projects/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{10E3C71A-65FA-4015-8215-5D860CBA10CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37BC86FE-8C36-E044-9C9B-5E3B5804517A}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{10E3C71A-65FA-4015-8215-5D860CBA10CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4620C8A7-A80C-6946-95A0-6516097A6F50}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ingreso" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="79">
   <si>
     <t>Alfredo</t>
   </si>
@@ -637,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D532"/>
+  <dimension ref="A1:D541"/>
   <sheetViews>
-    <sheetView topLeftCell="A513" workbookViewId="0">
-      <selection activeCell="A528" sqref="A528"/>
+    <sheetView tabSelected="1" topLeftCell="A521" workbookViewId="0">
+      <selection activeCell="B534" sqref="B534"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8098,6 +8098,132 @@
         <v>78</v>
       </c>
     </row>
+    <row r="533" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A533" s="1">
+        <v>45200</v>
+      </c>
+      <c r="B533" t="s">
+        <v>2</v>
+      </c>
+      <c r="C533">
+        <v>300</v>
+      </c>
+      <c r="D533" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="534" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A534" s="1">
+        <v>45200</v>
+      </c>
+      <c r="B534" t="s">
+        <v>9</v>
+      </c>
+      <c r="C534">
+        <v>1200</v>
+      </c>
+      <c r="D534" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="535" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A535" s="1">
+        <v>45200</v>
+      </c>
+      <c r="B535" t="s">
+        <v>11</v>
+      </c>
+      <c r="C535">
+        <v>600</v>
+      </c>
+      <c r="D535" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="536" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A536" s="1">
+        <v>45200</v>
+      </c>
+      <c r="B536" t="s">
+        <v>24</v>
+      </c>
+      <c r="C536">
+        <v>100</v>
+      </c>
+      <c r="D536" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="537" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A537" s="1">
+        <v>45200</v>
+      </c>
+      <c r="B537" t="s">
+        <v>8</v>
+      </c>
+      <c r="C537">
+        <v>100</v>
+      </c>
+      <c r="D537" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="538" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A538" s="1">
+        <v>45200</v>
+      </c>
+      <c r="B538" t="s">
+        <v>72</v>
+      </c>
+      <c r="C538">
+        <v>200</v>
+      </c>
+      <c r="D538" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="539" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A539" s="1">
+        <v>45200</v>
+      </c>
+      <c r="B539" t="s">
+        <v>31</v>
+      </c>
+      <c r="C539">
+        <v>50</v>
+      </c>
+      <c r="D539" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="540" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A540" s="1">
+        <v>45200</v>
+      </c>
+      <c r="B540" t="s">
+        <v>10</v>
+      </c>
+      <c r="C540">
+        <v>300</v>
+      </c>
+      <c r="D540" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="541" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A541" s="1">
+        <v>45200</v>
+      </c>
+      <c r="B541" t="s">
+        <v>7</v>
+      </c>
+      <c r="C541">
+        <v>1000</v>
+      </c>
+      <c r="D541" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
@@ -8109,10 +8235,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8784,6 +8910,28 @@
         <v>800</v>
       </c>
     </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>45193</v>
+      </c>
+      <c r="B61" t="s">
+        <v>46</v>
+      </c>
+      <c r="C61" s="4">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>45200</v>
+      </c>
+      <c r="B62" t="s">
+        <v>46</v>
+      </c>
+      <c r="C62" s="4">
+        <v>940</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8795,7 +8943,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Actualización al 08 de octubre 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/[5] R projects/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{10E3C71A-65FA-4015-8215-5D860CBA10CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4620C8A7-A80C-6946-95A0-6516097A6F50}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{10E3C71A-65FA-4015-8215-5D860CBA10CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13521161-7230-BE45-8BF8-B618EDBF7291}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Gastos" sheetId="2" r:id="rId2"/>
     <sheet name="Cuentas por cobrar" sheetId="6" r:id="rId3"/>
     <sheet name="Histórico de tecnicas" sheetId="7" r:id="rId4"/>
+    <sheet name="Actividad GOAT" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingreso!$A$1:$C$1</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="84">
   <si>
     <t>Alfredo</t>
   </si>
@@ -279,6 +280,21 @@
   </si>
   <si>
     <t>Préstamo</t>
+  </si>
+  <si>
+    <t>Adelanto Arbitro</t>
+  </si>
+  <si>
+    <t>Junte GOAT</t>
+  </si>
+  <si>
+    <t>Carbón</t>
+  </si>
+  <si>
+    <t>Colmado</t>
+  </si>
+  <si>
+    <t>Compra</t>
   </si>
 </sst>
 </file>
@@ -637,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D541"/>
+  <dimension ref="A1:D544"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A521" workbookViewId="0">
-      <selection activeCell="B534" sqref="B534"/>
+    <sheetView tabSelected="1" topLeftCell="A526" workbookViewId="0">
+      <selection activeCell="B549" sqref="B549"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8224,6 +8240,48 @@
         <v>34</v>
       </c>
     </row>
+    <row r="542" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A542" s="1">
+        <v>45207</v>
+      </c>
+      <c r="B542" t="s">
+        <v>37</v>
+      </c>
+      <c r="C542" s="2">
+        <v>100</v>
+      </c>
+      <c r="D542" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="543" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A543" s="1">
+        <v>45207</v>
+      </c>
+      <c r="B543" t="s">
+        <v>73</v>
+      </c>
+      <c r="C543" s="2">
+        <v>100</v>
+      </c>
+      <c r="D543" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="544" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A544" s="1">
+        <v>45207</v>
+      </c>
+      <c r="B544" t="s">
+        <v>9</v>
+      </c>
+      <c r="C544" s="2">
+        <v>-60</v>
+      </c>
+      <c r="D544" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
@@ -8235,10 +8293,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView topLeftCell="A54" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8930,6 +8988,40 @@
       </c>
       <c r="C62" s="4">
         <v>940</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>45207</v>
+      </c>
+      <c r="B63" t="s">
+        <v>46</v>
+      </c>
+      <c r="C63" s="4">
+        <f>800+260</f>
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>45207</v>
+      </c>
+      <c r="B64" t="s">
+        <v>79</v>
+      </c>
+      <c r="C64" s="4">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>45207</v>
+      </c>
+      <c r="B65" t="s">
+        <v>80</v>
+      </c>
+      <c r="C65" s="4">
+        <v>9833</v>
       </c>
     </row>
   </sheetData>
@@ -9243,4 +9335,52 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147E6DC2-7292-1F44-B969-1E00250933D7}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3">
+        <f>1668+1200+3400+1625</f>
+        <v>7893</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4">
+        <v>840</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización al 27 de octubre 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/[5] R projects/1-personales/goat/website/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Desktop/r_projects/personal/goat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{10E3C71A-65FA-4015-8215-5D860CBA10CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13521161-7230-BE45-8BF8-B618EDBF7291}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D80016-3BA6-F945-AB16-B1A81E0FFEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ingreso" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="86">
   <si>
     <t>Alfredo</t>
   </si>
@@ -295,6 +295,12 @@
   </si>
   <si>
     <t>Compra</t>
+  </si>
+  <si>
+    <t>Yandi</t>
+  </si>
+  <si>
+    <t>Agua y arbitro</t>
   </si>
 </sst>
 </file>
@@ -653,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D544"/>
+  <dimension ref="A1:D553"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A526" workbookViewId="0">
-      <selection activeCell="B549" sqref="B549"/>
+    <sheetView tabSelected="1" topLeftCell="A529" workbookViewId="0">
+      <selection activeCell="B554" sqref="B554"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8270,16 +8276,142 @@
     </row>
     <row r="544" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A544" s="1">
-        <v>45207</v>
+        <v>45214</v>
       </c>
       <c r="B544" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C544" s="2">
-        <v>-60</v>
+        <v>400</v>
       </c>
       <c r="D544" t="s">
-        <v>78</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="545" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A545" s="1">
+        <v>45214</v>
+      </c>
+      <c r="B545" t="s">
+        <v>13</v>
+      </c>
+      <c r="C545" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D545" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="546" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A546" s="1">
+        <v>45214</v>
+      </c>
+      <c r="B546" t="s">
+        <v>37</v>
+      </c>
+      <c r="C546" s="2">
+        <v>100</v>
+      </c>
+      <c r="D546" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="547" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A547" s="1">
+        <v>45214</v>
+      </c>
+      <c r="B547" t="s">
+        <v>26</v>
+      </c>
+      <c r="C547" s="2">
+        <v>50</v>
+      </c>
+      <c r="D547" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="548" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A548" s="1">
+        <v>45214</v>
+      </c>
+      <c r="B548" t="s">
+        <v>27</v>
+      </c>
+      <c r="C548" s="2">
+        <v>100</v>
+      </c>
+      <c r="D548" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="549" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A549" s="1">
+        <v>45214</v>
+      </c>
+      <c r="B549" t="s">
+        <v>28</v>
+      </c>
+      <c r="C549" s="2">
+        <v>100</v>
+      </c>
+      <c r="D549" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="550" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A550" s="1">
+        <v>45214</v>
+      </c>
+      <c r="B550" t="s">
+        <v>14</v>
+      </c>
+      <c r="C550" s="2">
+        <v>100</v>
+      </c>
+      <c r="D550" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="551" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A551" s="1">
+        <v>45214</v>
+      </c>
+      <c r="B551" t="s">
+        <v>25</v>
+      </c>
+      <c r="C551" s="2">
+        <v>100</v>
+      </c>
+      <c r="D551" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="552" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A552" s="1">
+        <v>45214</v>
+      </c>
+      <c r="B552" t="s">
+        <v>84</v>
+      </c>
+      <c r="C552" s="2">
+        <v>300</v>
+      </c>
+      <c r="D552" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="553" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A553" s="1">
+        <v>45214</v>
+      </c>
+      <c r="B553" t="s">
+        <v>1</v>
+      </c>
+      <c r="C553" s="2">
+        <v>200</v>
+      </c>
+      <c r="D553" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -8293,10 +8425,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView topLeftCell="A48" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9010,7 +9142,7 @@
         <v>79</v>
       </c>
       <c r="C64" s="4">
-        <v>400</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -9022,6 +9154,18 @@
       </c>
       <c r="C65" s="4">
         <v>9833</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>45214</v>
+      </c>
+      <c r="B66" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" s="4">
+        <f>400+230</f>
+        <v>630</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización al 04 de diciembre
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Desktop/r_projects/personal/goat/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Library/CloudStorage/OneDrive-Personal/[5] R projects/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D80016-3BA6-F945-AB16-B1A81E0FFEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1309DD37-686C-E64D-972F-FD5906E628A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="88">
   <si>
     <t>Alfredo</t>
   </si>
@@ -297,10 +297,16 @@
     <t>Compra</t>
   </si>
   <si>
-    <t>Yandi</t>
+    <t>Agua y arbitro</t>
   </si>
   <si>
-    <t>Agua y arbitro</t>
+    <t>Iverson</t>
+  </si>
+  <si>
+    <t>Yandy</t>
+  </si>
+  <si>
+    <t>Mamao</t>
   </si>
 </sst>
 </file>
@@ -659,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D553"/>
+  <dimension ref="A1:D576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A529" workbookViewId="0">
-      <selection activeCell="B554" sqref="B554"/>
+    <sheetView tabSelected="1" topLeftCell="A539" workbookViewId="0">
+      <selection activeCell="B563" sqref="B563"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8391,7 +8397,7 @@
         <v>45214</v>
       </c>
       <c r="B552" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C552" s="2">
         <v>300</v>
@@ -8411,6 +8417,328 @@
         <v>200</v>
       </c>
       <c r="D553" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="554" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A554" s="1">
+        <v>45235</v>
+      </c>
+      <c r="B554" t="s">
+        <v>3</v>
+      </c>
+      <c r="C554" s="2">
+        <v>100</v>
+      </c>
+      <c r="D554" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="555" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A555" s="1">
+        <v>45235</v>
+      </c>
+      <c r="B555" t="s">
+        <v>37</v>
+      </c>
+      <c r="C555" s="2">
+        <v>100</v>
+      </c>
+      <c r="D555" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="556" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A556" s="1">
+        <v>45235</v>
+      </c>
+      <c r="B556" t="s">
+        <v>8</v>
+      </c>
+      <c r="C556" s="2">
+        <v>100</v>
+      </c>
+      <c r="D556" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="557" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A557" s="1">
+        <v>45235</v>
+      </c>
+      <c r="B557" t="s">
+        <v>2</v>
+      </c>
+      <c r="C557" s="2">
+        <v>100</v>
+      </c>
+      <c r="D557" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="558" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A558" s="1">
+        <v>45235</v>
+      </c>
+      <c r="B558" t="s">
+        <v>25</v>
+      </c>
+      <c r="C558" s="2">
+        <v>100</v>
+      </c>
+      <c r="D558" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="559" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A559" s="1">
+        <v>45235</v>
+      </c>
+      <c r="B559" t="s">
+        <v>27</v>
+      </c>
+      <c r="C559" s="2">
+        <v>100</v>
+      </c>
+      <c r="D559" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="560" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A560" s="1">
+        <v>45242</v>
+      </c>
+      <c r="B560" t="s">
+        <v>8</v>
+      </c>
+      <c r="C560" s="2">
+        <v>100</v>
+      </c>
+      <c r="D560" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="561" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A561" s="1">
+        <v>45242</v>
+      </c>
+      <c r="B561" t="s">
+        <v>24</v>
+      </c>
+      <c r="C561" s="2">
+        <v>200</v>
+      </c>
+      <c r="D561" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="562" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A562" s="1">
+        <v>45242</v>
+      </c>
+      <c r="B562" t="s">
+        <v>28</v>
+      </c>
+      <c r="C562" s="2">
+        <v>100</v>
+      </c>
+      <c r="D562" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="563" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A563" s="1">
+        <v>45242</v>
+      </c>
+      <c r="B563" t="s">
+        <v>86</v>
+      </c>
+      <c r="C563" s="2">
+        <v>100</v>
+      </c>
+      <c r="D563" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="564" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A564" s="1">
+        <v>45242</v>
+      </c>
+      <c r="B564" t="s">
+        <v>25</v>
+      </c>
+      <c r="C564" s="2">
+        <v>100</v>
+      </c>
+      <c r="D564" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="565" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A565" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B565" t="s">
+        <v>2</v>
+      </c>
+      <c r="C565" s="2">
+        <v>150</v>
+      </c>
+      <c r="D565" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="566" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A566" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B566" t="s">
+        <v>86</v>
+      </c>
+      <c r="C566" s="2">
+        <v>100</v>
+      </c>
+      <c r="D566" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="567" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A567" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B567" t="s">
+        <v>1</v>
+      </c>
+      <c r="C567" s="2">
+        <v>200</v>
+      </c>
+      <c r="D567" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="568" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A568" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B568" t="s">
+        <v>31</v>
+      </c>
+      <c r="C568" s="2">
+        <v>100</v>
+      </c>
+      <c r="D568" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="569" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A569" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B569" t="s">
+        <v>87</v>
+      </c>
+      <c r="C569" s="2">
+        <v>100</v>
+      </c>
+      <c r="D569" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="570" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A570" s="1">
+        <v>45264</v>
+      </c>
+      <c r="B570" t="s">
+        <v>24</v>
+      </c>
+      <c r="C570" s="2">
+        <v>200</v>
+      </c>
+      <c r="D570" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="571" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A571" s="1">
+        <v>45264</v>
+      </c>
+      <c r="B571" t="s">
+        <v>21</v>
+      </c>
+      <c r="C571" s="2">
+        <v>100</v>
+      </c>
+      <c r="D571" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="572" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A572" s="1">
+        <v>45264</v>
+      </c>
+      <c r="B572" t="s">
+        <v>37</v>
+      </c>
+      <c r="C572" s="2">
+        <v>100</v>
+      </c>
+      <c r="D572" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="573" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A573" s="1">
+        <v>45264</v>
+      </c>
+      <c r="B573" t="s">
+        <v>85</v>
+      </c>
+      <c r="C573" s="2">
+        <v>10</v>
+      </c>
+      <c r="D573" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="574" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A574" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B574" t="s">
+        <v>15</v>
+      </c>
+      <c r="C574" s="2">
+        <v>500</v>
+      </c>
+      <c r="D574" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="575" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A575" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B575" t="s">
+        <v>10</v>
+      </c>
+      <c r="C575" s="2">
+        <v>300</v>
+      </c>
+      <c r="D575" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="576" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A576" s="1">
+        <v>45264</v>
+      </c>
+      <c r="B576" t="s">
+        <v>11</v>
+      </c>
+      <c r="C576" s="2">
+        <v>750</v>
+      </c>
+      <c r="D576" t="s">
         <v>34</v>
       </c>
     </row>
@@ -8425,10 +8753,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView topLeftCell="A48" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9161,11 +9489,107 @@
         <v>45214</v>
       </c>
       <c r="B66" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C66" s="4">
         <f>400+230</f>
         <v>630</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>45221</v>
+      </c>
+      <c r="B67" t="s">
+        <v>46</v>
+      </c>
+      <c r="C67" s="4">
+        <f>800+140</f>
+        <v>940</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>45228</v>
+      </c>
+      <c r="B68" t="s">
+        <v>46</v>
+      </c>
+      <c r="C68" s="4">
+        <f t="shared" ref="C68:C74" si="0">800+140</f>
+        <v>940</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>45235</v>
+      </c>
+      <c r="B69" t="s">
+        <v>46</v>
+      </c>
+      <c r="C69" s="4">
+        <f t="shared" si="0"/>
+        <v>940</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>45242</v>
+      </c>
+      <c r="B70" t="s">
+        <v>46</v>
+      </c>
+      <c r="C70" s="4">
+        <f t="shared" si="0"/>
+        <v>940</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>45249</v>
+      </c>
+      <c r="B71" t="s">
+        <v>46</v>
+      </c>
+      <c r="C71" s="4">
+        <f t="shared" si="0"/>
+        <v>940</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B72" t="s">
+        <v>46</v>
+      </c>
+      <c r="C72" s="4">
+        <f t="shared" si="0"/>
+        <v>940</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>45263</v>
+      </c>
+      <c r="B73" t="s">
+        <v>46</v>
+      </c>
+      <c r="C73" s="4">
+        <f t="shared" si="0"/>
+        <v>940</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>45270</v>
+      </c>
+      <c r="B74" t="s">
+        <v>46</v>
+      </c>
+      <c r="C74" s="4">
+        <f t="shared" si="0"/>
+        <v>940</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Registro de aportes y adecuar miembros a 2024
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Library/CloudStorage/OneDrive-Personal/[5] R projects/1-personales/goat/website/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Desktop/r_projects/personal/goat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1309DD37-686C-E64D-972F-FD5906E628A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A27A7E-4F5C-0C47-9351-7D30A4AB4BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="89">
   <si>
     <t>Alfredo</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>Mamao</t>
+  </si>
+  <si>
+    <t>Cobros</t>
   </si>
 </sst>
 </file>
@@ -665,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D576"/>
+  <dimension ref="A1:D581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A539" workbookViewId="0">
-      <selection activeCell="B563" sqref="B563"/>
+    <sheetView tabSelected="1" topLeftCell="A560" workbookViewId="0">
+      <selection activeCell="C581" sqref="C581"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8736,9 +8739,79 @@
         <v>11</v>
       </c>
       <c r="C576" s="2">
-        <v>750</v>
+        <v>350</v>
       </c>
       <c r="D576" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="577" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A577" s="1">
+        <v>45284</v>
+      </c>
+      <c r="B577" t="s">
+        <v>2</v>
+      </c>
+      <c r="C577" s="2">
+        <v>500</v>
+      </c>
+      <c r="D577" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="578" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A578" s="1">
+        <v>45284</v>
+      </c>
+      <c r="B578" t="s">
+        <v>14</v>
+      </c>
+      <c r="C578" s="2">
+        <v>100</v>
+      </c>
+      <c r="D578" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="579" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A579" s="1">
+        <v>45284</v>
+      </c>
+      <c r="B579" t="s">
+        <v>0</v>
+      </c>
+      <c r="C579" s="2">
+        <v>100</v>
+      </c>
+      <c r="D579" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="580" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A580" s="1">
+        <v>45284</v>
+      </c>
+      <c r="B580" t="s">
+        <v>24</v>
+      </c>
+      <c r="C580" s="2">
+        <v>100</v>
+      </c>
+      <c r="D580" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="581" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A581" s="1">
+        <v>45292</v>
+      </c>
+      <c r="B581" t="s">
+        <v>11</v>
+      </c>
+      <c r="C581" s="2">
+        <v>300</v>
+      </c>
+      <c r="D581" t="s">
         <v>34</v>
       </c>
     </row>
@@ -8753,10 +8826,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView topLeftCell="A48" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9592,6 +9665,17 @@
         <v>940</v>
       </c>
     </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>45284</v>
+      </c>
+      <c r="B75" t="s">
+        <v>46</v>
+      </c>
+      <c r="C75" s="4">
+        <v>1200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9600,10 +9684,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCA2D2E-DEE9-4BB9-9EC2-45DF3BC6F5C1}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9695,6 +9779,21 @@
       </c>
       <c r="D5">
         <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>45270</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6">
+        <f>500+50+100+60-100</f>
+        <v>610</v>
       </c>
     </row>
   </sheetData>
@@ -9910,7 +10009,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B1:B4"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Aportes al 6 de enero
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Desktop/r_projects/personal/goat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A27A7E-4F5C-0C47-9351-7D30A4AB4BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43C9965-B3E1-5340-85CA-66B4434C7517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="89">
   <si>
     <t>Alfredo</t>
   </si>
@@ -300,9 +300,6 @@
     <t>Agua y arbitro</t>
   </si>
   <si>
-    <t>Iverson</t>
-  </si>
-  <si>
     <t>Yandy</t>
   </si>
   <si>
@@ -310,6 +307,9 @@
   </si>
   <si>
     <t>Cobros</t>
+  </si>
+  <si>
+    <t>Se sentó en medio del juego</t>
   </si>
 </sst>
 </file>
@@ -668,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D581"/>
+  <dimension ref="A1:D588"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A560" workbookViewId="0">
-      <selection activeCell="C581" sqref="C581"/>
+    <sheetView tabSelected="1" topLeftCell="A551" workbookViewId="0">
+      <selection activeCell="D586" sqref="D586"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8400,7 +8400,7 @@
         <v>45214</v>
       </c>
       <c r="B552" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C552" s="2">
         <v>300</v>
@@ -8554,7 +8554,7 @@
         <v>45242</v>
       </c>
       <c r="B563" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C563" s="2">
         <v>100</v>
@@ -8596,7 +8596,7 @@
         <v>45256</v>
       </c>
       <c r="B566" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C566" s="2">
         <v>100</v>
@@ -8638,7 +8638,7 @@
         <v>45256</v>
       </c>
       <c r="B569" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C569" s="2">
         <v>100</v>
@@ -8694,7 +8694,7 @@
         <v>45264</v>
       </c>
       <c r="B573" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="C573" s="2">
         <v>10</v>
@@ -8813,6 +8813,95 @@
       </c>
       <c r="D581" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="582" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A582" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B582" t="s">
+        <v>20</v>
+      </c>
+      <c r="C582">
+        <v>300</v>
+      </c>
+      <c r="D582" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="583" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A583" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B583" t="s">
+        <v>31</v>
+      </c>
+      <c r="C583">
+        <v>100</v>
+      </c>
+      <c r="D583" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="584" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A584" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B584" t="s">
+        <v>86</v>
+      </c>
+      <c r="C584">
+        <v>100</v>
+      </c>
+      <c r="D584" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="585" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A585" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B585" t="s">
+        <v>16</v>
+      </c>
+      <c r="C585">
+        <v>100</v>
+      </c>
+      <c r="D585" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="586" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A586" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B586" t="s">
+        <v>9</v>
+      </c>
+      <c r="C586" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="587" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A587" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B587" t="s">
+        <v>13</v>
+      </c>
+      <c r="C587" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="588" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A588" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B588" t="s">
+        <v>10</v>
+      </c>
+      <c r="C588" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -8826,10 +8915,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
     <sheetView topLeftCell="A48" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9676,6 +9765,18 @@
         <v>1200</v>
       </c>
     </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B76" t="s">
+        <v>46</v>
+      </c>
+      <c r="C76" s="4">
+        <f>800+150</f>
+        <v>950</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9684,10 +9785,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCA2D2E-DEE9-4BB9-9EC2-45DF3BC6F5C1}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9789,11 +9890,28 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6">
         <f>500+50+100+60-100</f>
         <v>610</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>44932</v>
+      </c>
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="F7" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización al 21 de enero de 2024
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Desktop/r_projects/personal/goat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43C9965-B3E1-5340-85CA-66B4434C7517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DB7C2D-0D49-604F-B405-D4152AF655F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="89">
   <si>
     <t>Alfredo</t>
   </si>
@@ -668,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D588"/>
+  <dimension ref="A1:D611"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A551" workbookViewId="0">
-      <selection activeCell="D586" sqref="D586"/>
+    <sheetView tabSelected="1" topLeftCell="A573" workbookViewId="0">
+      <selection activeCell="C589" sqref="C589"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8881,6 +8881,9 @@
       <c r="C586" s="2">
         <v>0</v>
       </c>
+      <c r="D586" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="587" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A587" s="1">
@@ -8892,21 +8895,349 @@
       <c r="C587" s="2">
         <v>0</v>
       </c>
+      <c r="D587" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="588" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A588" s="1">
         <v>45297</v>
       </c>
       <c r="B588" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="C588" s="2">
         <v>0</v>
       </c>
+      <c r="D588" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="589" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A589" s="1">
+        <v>45305</v>
+      </c>
+      <c r="B589" t="s">
+        <v>26</v>
+      </c>
+      <c r="C589" s="2">
+        <v>0</v>
+      </c>
+      <c r="D589" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="590" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A590" s="1">
+        <v>45305</v>
+      </c>
+      <c r="B590" t="s">
+        <v>13</v>
+      </c>
+      <c r="C590" s="2">
+        <v>0</v>
+      </c>
+      <c r="D590" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="591" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A591" s="1">
+        <v>45305</v>
+      </c>
+      <c r="B591" t="s">
+        <v>20</v>
+      </c>
+      <c r="C591" s="2">
+        <v>0</v>
+      </c>
+      <c r="D591" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="592" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A592" s="1">
+        <v>45305</v>
+      </c>
+      <c r="B592" t="s">
+        <v>12</v>
+      </c>
+      <c r="C592" s="2">
+        <v>0</v>
+      </c>
+      <c r="D592" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="593" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A593" s="1">
+        <v>45305</v>
+      </c>
+      <c r="B593" t="s">
+        <v>11</v>
+      </c>
+      <c r="C593" s="2">
+        <v>0</v>
+      </c>
+      <c r="D593" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="594" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A594" s="1">
+        <v>45305</v>
+      </c>
+      <c r="B594" t="s">
+        <v>3</v>
+      </c>
+      <c r="C594" s="2">
+        <v>100</v>
+      </c>
+      <c r="D594" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="595" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A595" s="1">
+        <v>45305</v>
+      </c>
+      <c r="B595" t="s">
+        <v>10</v>
+      </c>
+      <c r="C595" s="2">
+        <v>0</v>
+      </c>
+      <c r="D595" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="596" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A596" s="1">
+        <v>45305</v>
+      </c>
+      <c r="B596" t="s">
+        <v>24</v>
+      </c>
+      <c r="C596" s="2">
+        <v>0</v>
+      </c>
+      <c r="D596" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="597" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A597" s="1">
+        <v>45305</v>
+      </c>
+      <c r="B597" t="s">
+        <v>9</v>
+      </c>
+      <c r="C597" s="2">
+        <v>0</v>
+      </c>
+      <c r="D597" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="598" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A598" s="1">
+        <v>45305</v>
+      </c>
+      <c r="B598" t="s">
+        <v>21</v>
+      </c>
+      <c r="C598" s="2">
+        <v>0</v>
+      </c>
+      <c r="D598" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="599" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A599" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B599" t="s">
+        <v>10</v>
+      </c>
+      <c r="C599" s="2">
+        <v>0</v>
+      </c>
+      <c r="D599" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="600" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A600" s="1">
+        <v>45312</v>
+      </c>
+      <c r="B600" t="s">
+        <v>23</v>
+      </c>
+      <c r="C600">
+        <v>100</v>
+      </c>
+      <c r="D600" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="601" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A601" s="1">
+        <v>45312</v>
+      </c>
+      <c r="B601" t="s">
+        <v>7</v>
+      </c>
+      <c r="C601">
+        <v>100</v>
+      </c>
+      <c r="D601" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="602" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A602" s="1">
+        <v>45312</v>
+      </c>
+      <c r="B602" t="s">
+        <v>12</v>
+      </c>
+      <c r="C602" s="2">
+        <v>0</v>
+      </c>
+      <c r="D602" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="603" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A603" s="1">
+        <v>45312</v>
+      </c>
+      <c r="B603" t="s">
+        <v>11</v>
+      </c>
+      <c r="C603" s="2">
+        <v>0</v>
+      </c>
+      <c r="D603" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="604" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A604" s="1">
+        <v>45312</v>
+      </c>
+      <c r="B604" t="s">
+        <v>3</v>
+      </c>
+      <c r="C604">
+        <v>0</v>
+      </c>
+      <c r="D604" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="605" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A605" s="1">
+        <v>45312</v>
+      </c>
+      <c r="B605" t="s">
+        <v>15</v>
+      </c>
+      <c r="C605">
+        <v>100</v>
+      </c>
+      <c r="D605" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="606" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A606" s="1">
+        <v>45312</v>
+      </c>
+      <c r="B606" t="s">
+        <v>26</v>
+      </c>
+      <c r="C606">
+        <v>0</v>
+      </c>
+      <c r="D606" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="607" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A607" s="1">
+        <v>45312</v>
+      </c>
+      <c r="B607" t="s">
+        <v>20</v>
+      </c>
+      <c r="C607">
+        <v>0</v>
+      </c>
+      <c r="D607" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="608" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A608" s="1">
+        <v>45312</v>
+      </c>
+      <c r="B608" t="s">
+        <v>13</v>
+      </c>
+      <c r="C608">
+        <v>0</v>
+      </c>
+      <c r="D608" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="609" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A609" s="1">
+        <v>45312</v>
+      </c>
+      <c r="B609" t="s">
+        <v>10</v>
+      </c>
+      <c r="C609">
+        <v>1000</v>
+      </c>
+      <c r="D609" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="610" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A610" s="1">
+        <v>45312</v>
+      </c>
+      <c r="B610" t="s">
+        <v>25</v>
+      </c>
+      <c r="C610">
+        <v>100</v>
+      </c>
+      <c r="D610" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="611" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A611" s="1">
+        <v>45312</v>
+      </c>
+      <c r="B611" t="s">
+        <v>21</v>
+      </c>
+      <c r="C611">
+        <v>0</v>
+      </c>
+      <c r="D611" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="B614:B1048576 B1:B611">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8915,10 +9246,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView topLeftCell="A48" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9775,6 +10106,17 @@
       <c r="C76" s="4">
         <f>800+150</f>
         <v>950</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>45312</v>
+      </c>
+      <c r="B77" t="s">
+        <v>62</v>
+      </c>
+      <c r="C77" s="4">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add cobro joel dic 2023
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Desktop/r_projects/personal/goat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A365939-6915-9940-9B54-FD1A087EC180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85E1C7E-75A1-B042-B324-6B3FBD26A740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="89">
   <si>
     <t>Alfredo</t>
   </si>
@@ -304,9 +304,6 @@
   </si>
   <si>
     <t>Mamao</t>
-  </si>
-  <si>
-    <t>Cobros</t>
   </si>
   <si>
     <t>Se sentó en medio del juego</t>
@@ -681,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D632"/>
+  <dimension ref="A1:D636"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A602" workbookViewId="0">
-      <selection activeCell="B632" sqref="B632"/>
+    <sheetView tabSelected="1" topLeftCell="A625" workbookViewId="0">
+      <selection activeCell="O622" sqref="O622"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9543,12 +9540,68 @@
         <v>34</v>
       </c>
     </row>
+    <row r="633" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A633" s="1">
+        <v>45270</v>
+      </c>
+      <c r="B633" t="s">
+        <v>8</v>
+      </c>
+      <c r="C633" s="2">
+        <v>400</v>
+      </c>
+      <c r="D633" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="634" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A634" s="1">
+        <v>45270</v>
+      </c>
+      <c r="B634" t="s">
+        <v>86</v>
+      </c>
+      <c r="C634" s="2">
+        <v>50</v>
+      </c>
+      <c r="D634" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="635" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A635" s="1">
+        <v>45270</v>
+      </c>
+      <c r="B635" t="s">
+        <v>25</v>
+      </c>
+      <c r="C635" s="2">
+        <v>60</v>
+      </c>
+      <c r="D635" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="636" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A636" s="1">
+        <v>45270</v>
+      </c>
+      <c r="B636" t="s">
+        <v>37</v>
+      </c>
+      <c r="C636" s="2">
+        <v>100</v>
+      </c>
+      <c r="D636" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B614:B1048576 B1:B612">
-    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9560,7 +9613,7 @@
   <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView topLeftCell="A60" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10450,10 +10503,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCA2D2E-DEE9-4BB9-9EC2-45DF3BC6F5C1}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10549,25 +10602,27 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
-        <v>45270</v>
+        <v>44932</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="F6" t="s">
         <v>87</v>
-      </c>
-      <c r="D6">
-        <f>500+50+100+60-100</f>
-        <v>610</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
-        <v>44932</v>
+        <v>45326</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
         <v>63</v>
@@ -10577,23 +10632,6 @@
       </c>
       <c r="F7" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>45326</v>
-      </c>
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8">
-        <v>100</v>
-      </c>
-      <c r="F8" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update as of 2024-02-11
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Desktop/r_projects/personal/goat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85E1C7E-75A1-B042-B324-6B3FBD26A740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6496DC7-59F5-5F41-A395-0035722C99F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ingreso" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="90">
   <si>
     <t>Alfredo</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cogió un pique y picó la pelota muy duro. </t>
+  </si>
+  <si>
+    <t>Juego Mamelles</t>
   </si>
 </sst>
 </file>
@@ -678,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D636"/>
+  <dimension ref="A1:D641"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A625" workbookViewId="0">
-      <selection activeCell="O622" sqref="O622"/>
+    <sheetView topLeftCell="A605" workbookViewId="0">
+      <selection activeCell="A638" sqref="A638:A641"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9593,6 +9596,76 @@
         <v>100</v>
       </c>
       <c r="D636" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="637" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A637" s="1">
+        <v>45333</v>
+      </c>
+      <c r="B637" t="s">
+        <v>18</v>
+      </c>
+      <c r="C637" s="2">
+        <v>100</v>
+      </c>
+      <c r="D637" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="638" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A638" s="1">
+        <v>45333</v>
+      </c>
+      <c r="B638" t="s">
+        <v>24</v>
+      </c>
+      <c r="C638" s="2">
+        <v>200</v>
+      </c>
+      <c r="D638" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="639" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A639" s="1">
+        <v>45333</v>
+      </c>
+      <c r="B639" t="s">
+        <v>8</v>
+      </c>
+      <c r="C639" s="2">
+        <v>200</v>
+      </c>
+      <c r="D639" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="640" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A640" s="1">
+        <v>45333</v>
+      </c>
+      <c r="B640" t="s">
+        <v>20</v>
+      </c>
+      <c r="C640" s="2">
+        <v>100</v>
+      </c>
+      <c r="D640" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="641" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A641" s="1">
+        <v>45333</v>
+      </c>
+      <c r="B641" t="s">
+        <v>13</v>
+      </c>
+      <c r="C641" s="2">
+        <v>200</v>
+      </c>
+      <c r="D641" t="s">
         <v>34</v>
       </c>
     </row>
@@ -9610,10 +9683,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10493,6 +10566,28 @@
       <c r="C78" s="4">
         <f>800+170</f>
         <v>970</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>45333</v>
+      </c>
+      <c r="B79" t="s">
+        <v>48</v>
+      </c>
+      <c r="C79" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>45332</v>
+      </c>
+      <c r="B80" t="s">
+        <v>89</v>
+      </c>
+      <c r="C80" s="4">
+        <v>700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update finanza y fotos orlando robert
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Desktop/r_projects/personal/goat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6496DC7-59F5-5F41-A395-0035722C99F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF264C15-C9E0-EE4D-A410-55B6F25A9FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ingreso" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="90">
   <si>
     <t>Alfredo</t>
   </si>
@@ -681,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D641"/>
+  <dimension ref="A1:D648"/>
   <sheetViews>
-    <sheetView topLeftCell="A605" workbookViewId="0">
-      <selection activeCell="A638" sqref="A638:A641"/>
+    <sheetView tabSelected="1" topLeftCell="A623" workbookViewId="0">
+      <selection activeCell="B648" sqref="B648"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9666,6 +9666,104 @@
         <v>200</v>
       </c>
       <c r="D641" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="642" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A642" s="1">
+        <v>45340</v>
+      </c>
+      <c r="B642" t="s">
+        <v>25</v>
+      </c>
+      <c r="C642">
+        <v>100</v>
+      </c>
+      <c r="D642" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="643" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A643" s="1">
+        <v>45340</v>
+      </c>
+      <c r="B643" t="s">
+        <v>8</v>
+      </c>
+      <c r="C643">
+        <v>100</v>
+      </c>
+      <c r="D643" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="644" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A644" s="1">
+        <v>45340</v>
+      </c>
+      <c r="B644" t="s">
+        <v>27</v>
+      </c>
+      <c r="C644">
+        <v>200</v>
+      </c>
+      <c r="D644" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="645" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A645" s="1">
+        <v>45340</v>
+      </c>
+      <c r="B645" t="s">
+        <v>2</v>
+      </c>
+      <c r="C645">
+        <v>200</v>
+      </c>
+      <c r="D645" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="646" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A646" s="1">
+        <v>45340</v>
+      </c>
+      <c r="B646" t="s">
+        <v>20</v>
+      </c>
+      <c r="C646">
+        <v>100</v>
+      </c>
+      <c r="D646" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="647" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A647" s="1">
+        <v>45340</v>
+      </c>
+      <c r="B647" t="s">
+        <v>12</v>
+      </c>
+      <c r="C647">
+        <v>400</v>
+      </c>
+      <c r="D647" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="648" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A648" s="1">
+        <v>45334</v>
+      </c>
+      <c r="B648" t="s">
+        <v>19</v>
+      </c>
+      <c r="C648" s="2">
+        <v>300</v>
+      </c>
+      <c r="D648" t="s">
         <v>34</v>
       </c>
     </row>
@@ -9683,9 +9781,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A60" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
@@ -10588,6 +10686,18 @@
       </c>
       <c r="C80" s="4">
         <v>700</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>45340</v>
+      </c>
+      <c r="B81" t="s">
+        <v>74</v>
+      </c>
+      <c r="C81" s="4">
+        <f>150+800</f>
+        <v>950</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update as of 2024-02-24
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Desktop/r_projects/personal/goat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF264C15-C9E0-EE4D-A410-55B6F25A9FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28451B46-AC58-E94E-A581-FAC6CC2FF12D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="91">
   <si>
     <t>Alfredo</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>Juego Mamelles</t>
+  </si>
+  <si>
+    <t>Le dijo "Mamagüevo" a los que no entraban a rebotar</t>
   </si>
 </sst>
 </file>
@@ -681,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D648"/>
+  <dimension ref="A1:D662"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A623" workbookViewId="0">
-      <selection activeCell="B648" sqref="B648"/>
+    <sheetView tabSelected="1" topLeftCell="A637" workbookViewId="0">
+      <selection activeCell="C655" sqref="C655"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9764,6 +9767,202 @@
         <v>300</v>
       </c>
       <c r="D648" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="649" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A649" s="1">
+        <v>45347</v>
+      </c>
+      <c r="B649" t="s">
+        <v>24</v>
+      </c>
+      <c r="C649">
+        <v>200</v>
+      </c>
+      <c r="D649" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="650" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A650" s="1">
+        <v>45347</v>
+      </c>
+      <c r="B650" t="s">
+        <v>14</v>
+      </c>
+      <c r="C650">
+        <v>100</v>
+      </c>
+      <c r="D650" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="651" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A651" s="1">
+        <v>45347</v>
+      </c>
+      <c r="B651" t="s">
+        <v>6</v>
+      </c>
+      <c r="C651">
+        <v>100</v>
+      </c>
+      <c r="D651" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="652" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A652" s="1">
+        <v>45347</v>
+      </c>
+      <c r="B652" t="s">
+        <v>21</v>
+      </c>
+      <c r="C652">
+        <v>145</v>
+      </c>
+      <c r="D652" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="653" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A653" s="1">
+        <v>45347</v>
+      </c>
+      <c r="B653" t="s">
+        <v>18</v>
+      </c>
+      <c r="C653">
+        <v>100</v>
+      </c>
+      <c r="D653" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="654" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A654" s="1">
+        <v>45347</v>
+      </c>
+      <c r="B654" t="s">
+        <v>10</v>
+      </c>
+      <c r="C654">
+        <v>100</v>
+      </c>
+      <c r="D654" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="655" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A655" s="1">
+        <v>45347</v>
+      </c>
+      <c r="B655" t="s">
+        <v>8</v>
+      </c>
+      <c r="C655">
+        <v>100</v>
+      </c>
+      <c r="D655" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="656" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A656" s="1">
+        <v>45347</v>
+      </c>
+      <c r="B656" t="s">
+        <v>0</v>
+      </c>
+      <c r="C656">
+        <v>100</v>
+      </c>
+      <c r="D656" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="657" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A657" s="1">
+        <v>45347</v>
+      </c>
+      <c r="B657" t="s">
+        <v>13</v>
+      </c>
+      <c r="C657">
+        <v>0</v>
+      </c>
+      <c r="D657" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="658" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A658" s="1">
+        <v>45347</v>
+      </c>
+      <c r="B658" t="s">
+        <v>25</v>
+      </c>
+      <c r="C658">
+        <v>0</v>
+      </c>
+      <c r="D658" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="659" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A659" s="1">
+        <v>45347</v>
+      </c>
+      <c r="B659" t="s">
+        <v>11</v>
+      </c>
+      <c r="C659">
+        <v>0</v>
+      </c>
+      <c r="D659" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="660" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A660" s="1">
+        <v>45347</v>
+      </c>
+      <c r="B660" t="s">
+        <v>7</v>
+      </c>
+      <c r="C660">
+        <v>0</v>
+      </c>
+      <c r="D660" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="661" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A661" s="1">
+        <v>45347</v>
+      </c>
+      <c r="B661" t="s">
+        <v>9</v>
+      </c>
+      <c r="C661" s="2">
+        <v>0</v>
+      </c>
+      <c r="D661" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="662" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A662" s="1">
+        <v>45347</v>
+      </c>
+      <c r="B662" t="s">
+        <v>20</v>
+      </c>
+      <c r="C662" s="2">
+        <v>0</v>
+      </c>
+      <c r="D662" t="s">
         <v>34</v>
       </c>
     </row>
@@ -9781,10 +9980,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView topLeftCell="A56" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82:C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10700,6 +10899,18 @@
         <v>950</v>
       </c>
     </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>45347</v>
+      </c>
+      <c r="B82" t="s">
+        <v>74</v>
+      </c>
+      <c r="C82" s="4">
+        <f>150+800</f>
+        <v>950</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10708,10 +10919,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCA2D2E-DEE9-4BB9-9EC2-45DF3BC6F5C1}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10837,6 +11048,23 @@
       </c>
       <c r="F7" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>45347</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="F8" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update as of 2024-03-10
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Desktop/r_projects/personal/goat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28451B46-AC58-E94E-A581-FAC6CC2FF12D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FE32CD-25F4-CC40-B433-4F38A4F0FA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Actividad GOAT" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingreso!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingreso!$A$1:$D$677</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="91">
   <si>
     <t>Alfredo</t>
   </si>
@@ -276,9 +276,6 @@
     <t>Gatorade</t>
   </si>
   <si>
-    <t>Invitado</t>
-  </si>
-  <si>
     <t>Préstamo</t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>Le dijo "Mamagüevo" a los que no entraban a rebotar</t>
+  </si>
+  <si>
+    <t>Le dijo "Canalla" al arbitro. (Con razón)</t>
   </si>
 </sst>
 </file>
@@ -684,10 +684,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D662"/>
+  <dimension ref="A1:D677"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A637" workbookViewId="0">
-      <selection activeCell="C655" sqref="C655"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A651" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C677" sqref="C677"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7904,7 +7905,7 @@
         <v>-100</v>
       </c>
       <c r="D515" t="s">
-        <v>77</v>
+        <v>34</v>
       </c>
     </row>
     <row r="516" spans="1:4" x14ac:dyDescent="0.2">
@@ -8142,7 +8143,7 @@
         <v>-150</v>
       </c>
       <c r="D532" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.2">
@@ -8416,7 +8417,7 @@
         <v>45214</v>
       </c>
       <c r="B552" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C552" s="2">
         <v>300</v>
@@ -8570,7 +8571,7 @@
         <v>45242</v>
       </c>
       <c r="B563" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C563" s="2">
         <v>100</v>
@@ -8612,7 +8613,7 @@
         <v>45256</v>
       </c>
       <c r="B566" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C566" s="2">
         <v>100</v>
@@ -8654,7 +8655,7 @@
         <v>45256</v>
       </c>
       <c r="B569" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C569" s="2">
         <v>100</v>
@@ -8864,7 +8865,7 @@
         <v>45297</v>
       </c>
       <c r="B584" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C584">
         <v>100</v>
@@ -9298,7 +9299,7 @@
         <v>45326</v>
       </c>
       <c r="B615" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C615">
         <v>200</v>
@@ -9565,7 +9566,7 @@
         <v>45270</v>
       </c>
       <c r="B634" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C634" s="2">
         <v>50</v>
@@ -9966,7 +9967,218 @@
         <v>34</v>
       </c>
     </row>
+    <row r="663" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A663" s="1">
+        <v>45354</v>
+      </c>
+      <c r="B663" t="s">
+        <v>3</v>
+      </c>
+      <c r="C663">
+        <v>500</v>
+      </c>
+      <c r="D663" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="664" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A664" s="1">
+        <v>45354</v>
+      </c>
+      <c r="B664" t="s">
+        <v>6</v>
+      </c>
+      <c r="C664">
+        <v>100</v>
+      </c>
+      <c r="D664" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="665" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A665" s="1">
+        <v>45354</v>
+      </c>
+      <c r="B665" t="s">
+        <v>26</v>
+      </c>
+      <c r="C665">
+        <v>50</v>
+      </c>
+      <c r="D665" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="666" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A666" s="1">
+        <v>45354</v>
+      </c>
+      <c r="B666" t="s">
+        <v>16</v>
+      </c>
+      <c r="C666">
+        <v>-200</v>
+      </c>
+      <c r="D666" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="667" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A667" s="1">
+        <v>45354</v>
+      </c>
+      <c r="B667" t="s">
+        <v>24</v>
+      </c>
+      <c r="C667">
+        <v>200</v>
+      </c>
+      <c r="D667" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="668" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A668" s="1">
+        <v>45354</v>
+      </c>
+      <c r="B668" t="s">
+        <v>14</v>
+      </c>
+      <c r="C668">
+        <v>100</v>
+      </c>
+      <c r="D668" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="669" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A669" s="1">
+        <v>45354</v>
+      </c>
+      <c r="B669" t="s">
+        <v>25</v>
+      </c>
+      <c r="C669">
+        <v>100</v>
+      </c>
+      <c r="D669" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="670" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A670" s="1">
+        <v>45354</v>
+      </c>
+      <c r="B670" t="s">
+        <v>8</v>
+      </c>
+      <c r="C670">
+        <v>300</v>
+      </c>
+      <c r="D670" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="671" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A671" s="1">
+        <v>45354</v>
+      </c>
+      <c r="B671" t="s">
+        <v>2</v>
+      </c>
+      <c r="C671">
+        <v>100</v>
+      </c>
+      <c r="D671" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="672" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A672" s="1">
+        <v>45361</v>
+      </c>
+      <c r="B672" t="s">
+        <v>8</v>
+      </c>
+      <c r="C672" s="2">
+        <v>200</v>
+      </c>
+      <c r="D672" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="673" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A673" s="1">
+        <v>45361</v>
+      </c>
+      <c r="B673" t="s">
+        <v>0</v>
+      </c>
+      <c r="C673" s="2">
+        <v>200</v>
+      </c>
+      <c r="D673" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="674" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A674" s="1">
+        <v>45361</v>
+      </c>
+      <c r="B674" t="s">
+        <v>18</v>
+      </c>
+      <c r="C674" s="2">
+        <v>100</v>
+      </c>
+      <c r="D674" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="675" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A675" s="1">
+        <v>45361</v>
+      </c>
+      <c r="B675" t="s">
+        <v>15</v>
+      </c>
+      <c r="C675" s="2">
+        <v>500</v>
+      </c>
+      <c r="D675" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="676" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A676" s="1">
+        <v>45361</v>
+      </c>
+      <c r="B676" t="s">
+        <v>12</v>
+      </c>
+      <c r="C676" s="2">
+        <v>100</v>
+      </c>
+      <c r="D676" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="677" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A677" s="1">
+        <v>45361</v>
+      </c>
+      <c r="B677" t="s">
+        <v>11</v>
+      </c>
+      <c r="C677" s="2">
+        <v>100</v>
+      </c>
+      <c r="D677" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:D677" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
@@ -9980,10 +10192,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82:C82"/>
+    <sheetView topLeftCell="A59" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10694,7 +10906,7 @@
         <v>45207</v>
       </c>
       <c r="B64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C64" s="4">
         <v>1200</v>
@@ -10705,7 +10917,7 @@
         <v>45207</v>
       </c>
       <c r="B65" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C65" s="4">
         <v>9833</v>
@@ -10716,7 +10928,7 @@
         <v>45214</v>
       </c>
       <c r="B66" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C66" s="4">
         <f>400+230</f>
@@ -10881,7 +11093,7 @@
         <v>45332</v>
       </c>
       <c r="B80" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C80" s="4">
         <v>700</v>
@@ -10909,6 +11121,29 @@
       <c r="C82" s="4">
         <f>150+800</f>
         <v>950</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>45354</v>
+      </c>
+      <c r="B83" t="s">
+        <v>74</v>
+      </c>
+      <c r="C83" s="4">
+        <f>1200</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>44995</v>
+      </c>
+      <c r="B84" t="s">
+        <v>74</v>
+      </c>
+      <c r="C84" s="4">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -10919,10 +11154,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCA2D2E-DEE9-4BB9-9EC2-45DF3BC6F5C1}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11021,7 +11256,7 @@
         <v>44932</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
         <v>63</v>
@@ -11030,7 +11265,7 @@
         <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -11047,24 +11282,7 @@
         <v>100</v>
       </c>
       <c r="F7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>45347</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8">
-        <v>100</v>
-      </c>
-      <c r="F8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -11074,15 +11292,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE771D5-AE0E-9C4B-B862-1B8092D29603}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -11268,6 +11487,46 @@
       </c>
       <c r="F10" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>45347</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11">
+        <v>100</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>45361</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -11287,7 +11546,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1">
         <v>220</v>
@@ -11295,7 +11554,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2">
         <v>230</v>
@@ -11303,7 +11562,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3">
         <f>1668+1200+3400+1625</f>

</xml_diff>

<commit_message>
Update as of 2024-03-17
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Desktop/r_projects/personal/goat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FE32CD-25F4-CC40-B433-4F38A4F0FA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAFE76D-D126-8E4A-9348-3C16861F078E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Actividad GOAT" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingreso!$A$1:$D$677</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingreso!$A$1:$D$676</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="92">
   <si>
     <t>Alfredo</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>Le dijo "Canalla" al arbitro. (Con razón)</t>
+  </si>
+  <si>
+    <t>Hizo un pique con el mmg de carlos y le amagó un trompón</t>
   </si>
 </sst>
 </file>
@@ -684,11 +687,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D677"/>
+  <dimension ref="A1:D684"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A651" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C677" sqref="C677"/>
+      <pane ySplit="1" topLeftCell="A659" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A685" sqref="A685"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10014,10 +10017,10 @@
         <v>45354</v>
       </c>
       <c r="B666" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C666">
-        <v>-200</v>
+        <v>200</v>
       </c>
       <c r="D666" t="s">
         <v>34</v>
@@ -10028,10 +10031,10 @@
         <v>45354</v>
       </c>
       <c r="B667" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C667">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D667" t="s">
         <v>34</v>
@@ -10042,7 +10045,7 @@
         <v>45354</v>
       </c>
       <c r="B668" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C668">
         <v>100</v>
@@ -10056,10 +10059,10 @@
         <v>45354</v>
       </c>
       <c r="B669" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C669">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D669" t="s">
         <v>34</v>
@@ -10070,10 +10073,10 @@
         <v>45354</v>
       </c>
       <c r="B670" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C670">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D670" t="s">
         <v>34</v>
@@ -10081,13 +10084,13 @@
     </row>
     <row r="671" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A671" s="1">
-        <v>45354</v>
+        <v>45361</v>
       </c>
       <c r="B671" t="s">
-        <v>2</v>
-      </c>
-      <c r="C671">
-        <v>100</v>
+        <v>8</v>
+      </c>
+      <c r="C671" s="2">
+        <v>200</v>
       </c>
       <c r="D671" t="s">
         <v>34</v>
@@ -10098,7 +10101,7 @@
         <v>45361</v>
       </c>
       <c r="B672" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C672" s="2">
         <v>200</v>
@@ -10112,10 +10115,10 @@
         <v>45361</v>
       </c>
       <c r="B673" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C673" s="2">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D673" t="s">
         <v>34</v>
@@ -10126,10 +10129,10 @@
         <v>45361</v>
       </c>
       <c r="B674" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C674" s="2">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D674" t="s">
         <v>34</v>
@@ -10140,13 +10143,13 @@
         <v>45361</v>
       </c>
       <c r="B675" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C675" s="2">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="D675" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="676" spans="1:4" x14ac:dyDescent="0.2">
@@ -10154,7 +10157,7 @@
         <v>45361</v>
       </c>
       <c r="B676" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C676" s="2">
         <v>100</v>
@@ -10165,7 +10168,7 @@
     </row>
     <row r="677" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A677" s="1">
-        <v>45361</v>
+        <v>45368</v>
       </c>
       <c r="B677" t="s">
         <v>11</v>
@@ -10177,8 +10180,106 @@
         <v>38</v>
       </c>
     </row>
+    <row r="678" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A678" s="1">
+        <v>45368</v>
+      </c>
+      <c r="B678" t="s">
+        <v>13</v>
+      </c>
+      <c r="C678" s="2">
+        <v>100</v>
+      </c>
+      <c r="D678" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="679" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A679" s="1">
+        <v>45368</v>
+      </c>
+      <c r="B679" t="s">
+        <v>13</v>
+      </c>
+      <c r="C679" s="2">
+        <v>900</v>
+      </c>
+      <c r="D679" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="680" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A680" s="1">
+        <v>45368</v>
+      </c>
+      <c r="B680" t="s">
+        <v>8</v>
+      </c>
+      <c r="C680" s="2">
+        <v>400</v>
+      </c>
+      <c r="D680" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="681" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A681" s="1">
+        <v>45368</v>
+      </c>
+      <c r="B681" t="s">
+        <v>16</v>
+      </c>
+      <c r="C681" s="2">
+        <v>300</v>
+      </c>
+      <c r="D681" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="682" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A682" s="1">
+        <v>45368</v>
+      </c>
+      <c r="B682" t="s">
+        <v>18</v>
+      </c>
+      <c r="C682" s="2">
+        <v>100</v>
+      </c>
+      <c r="D682" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="683" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A683" s="1">
+        <v>45368</v>
+      </c>
+      <c r="B683" t="s">
+        <v>12</v>
+      </c>
+      <c r="C683" s="2">
+        <v>100</v>
+      </c>
+      <c r="D683" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="684" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A684" s="1">
+        <v>45368</v>
+      </c>
+      <c r="B684" t="s">
+        <v>11</v>
+      </c>
+      <c r="C684" s="2">
+        <v>300</v>
+      </c>
+      <c r="D684" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D677" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D676" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
@@ -10192,10 +10293,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
     <sheetView topLeftCell="A59" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11137,13 +11238,25 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
-        <v>44995</v>
+        <v>45361</v>
       </c>
       <c r="B84" t="s">
         <v>74</v>
       </c>
       <c r="C84" s="4">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>45368</v>
+      </c>
+      <c r="B85" t="s">
+        <v>74</v>
+      </c>
+      <c r="C85" s="4">
+        <f>900+140</f>
+        <v>1040</v>
       </c>
     </row>
   </sheetData>
@@ -11154,10 +11267,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCA2D2E-DEE9-4BB9-9EC2-45DF3BC6F5C1}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11205,10 +11318,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <v>45067</v>
+        <v>45109</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>63</v>
@@ -11217,12 +11330,12 @@
         <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <v>45109</v>
+        <v>45151</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -11233,16 +11346,13 @@
       <c r="D4">
         <v>100</v>
       </c>
-      <c r="F4" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>45151</v>
+        <v>44932</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
         <v>63</v>
@@ -11250,13 +11360,16 @@
       <c r="D5">
         <v>100</v>
       </c>
+      <c r="F5" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
-        <v>44932</v>
+        <v>45326</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
         <v>63</v>
@@ -11265,23 +11378,6 @@
         <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>45326</v>
-      </c>
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7">
-        <v>100</v>
-      </c>
-      <c r="F7" t="s">
         <v>87</v>
       </c>
     </row>
@@ -11292,10 +11388,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE771D5-AE0E-9C4B-B862-1B8092D29603}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11497,7 +11593,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="D11">
         <v>100</v>
@@ -11517,7 +11613,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="D12">
         <v>100</v>
@@ -11527,6 +11623,46 @@
       </c>
       <c r="F12" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>45368</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>45067</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14">
+        <v>100</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update as of 2024-04-29
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Trabajo laptop\_personal\goat_website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8563E11E-FF8D-4730-81A0-6DDBB6BF3074}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5C9DA9-1FD4-4806-9B34-A0D6EE2B5F9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="21015" windowHeight="17505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1563" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="93">
   <si>
     <t>Alfredo</t>
   </si>
@@ -679,11 +679,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D703"/>
+  <dimension ref="A1:D711"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A686" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G694" sqref="G694"/>
+      <pane ySplit="1" topLeftCell="A700" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C714" sqref="C714"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10535,6 +10535,118 @@
         <v>100</v>
       </c>
       <c r="D703" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="704" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A704" s="1">
+        <v>45411</v>
+      </c>
+      <c r="B704" t="s">
+        <v>21</v>
+      </c>
+      <c r="C704" s="2">
+        <v>100</v>
+      </c>
+      <c r="D704" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="705" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A705" s="1">
+        <v>45411</v>
+      </c>
+      <c r="B705" t="s">
+        <v>3</v>
+      </c>
+      <c r="C705" s="2">
+        <v>200</v>
+      </c>
+      <c r="D705" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="706" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A706" s="1">
+        <v>45411</v>
+      </c>
+      <c r="B706" t="s">
+        <v>2</v>
+      </c>
+      <c r="C706" s="2">
+        <v>900</v>
+      </c>
+      <c r="D706" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="707" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A707" s="1">
+        <v>45411</v>
+      </c>
+      <c r="B707" t="s">
+        <v>6</v>
+      </c>
+      <c r="C707" s="2">
+        <v>100</v>
+      </c>
+      <c r="D707" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="708" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A708" s="1">
+        <v>45411</v>
+      </c>
+      <c r="B708" t="s">
+        <v>8</v>
+      </c>
+      <c r="C708" s="2">
+        <v>100</v>
+      </c>
+      <c r="D708" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="709" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A709" s="1">
+        <v>45411</v>
+      </c>
+      <c r="B709" t="s">
+        <v>7</v>
+      </c>
+      <c r="C709" s="2">
+        <v>50</v>
+      </c>
+      <c r="D709" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="710" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A710" s="1">
+        <v>45411</v>
+      </c>
+      <c r="B710" t="s">
+        <v>13</v>
+      </c>
+      <c r="C710" s="2">
+        <v>200</v>
+      </c>
+      <c r="D710" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="711" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A711" s="1">
+        <v>45411</v>
+      </c>
+      <c r="B711" t="s">
+        <v>19</v>
+      </c>
+      <c r="C711" s="2">
+        <v>500</v>
+      </c>
+      <c r="D711" t="s">
         <v>34</v>
       </c>
     </row>
@@ -10553,9 +10665,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A79" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
@@ -11564,6 +11676,17 @@
       </c>
       <c r="C89" s="4">
         <v>5080</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>45411</v>
+      </c>
+      <c r="B90" t="s">
+        <v>74</v>
+      </c>
+      <c r="C90" s="4">
+        <v>960</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update as of 2024-05-26
</commit_message>
<xml_diff>
--- a/data/aportes.xlsx
+++ b/data/aportes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Trabajo laptop\_personal\goat_website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5C9DA9-1FD4-4806-9B34-A0D6EE2B5F9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7243B2AF-903A-4611-AC94-D7D4B1F3FF5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="21015" windowHeight="17505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1600" uniqueCount="93">
   <si>
     <t>Alfredo</t>
   </si>
@@ -679,11 +679,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D711"/>
+  <dimension ref="A1:D720"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A700" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C714" sqref="C714"/>
+      <pane ySplit="1" topLeftCell="A705" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A720" sqref="A720"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10647,6 +10647,132 @@
         <v>500</v>
       </c>
       <c r="D711" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="712" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A712" s="1">
+        <v>45417</v>
+      </c>
+      <c r="B712" t="s">
+        <v>23</v>
+      </c>
+      <c r="C712" s="2">
+        <v>100</v>
+      </c>
+      <c r="D712" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="713" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A713" s="1">
+        <v>45417</v>
+      </c>
+      <c r="B713" t="s">
+        <v>1</v>
+      </c>
+      <c r="C713" s="2">
+        <v>100</v>
+      </c>
+      <c r="D713" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="714" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A714" s="1">
+        <v>45438</v>
+      </c>
+      <c r="B714" t="s">
+        <v>8</v>
+      </c>
+      <c r="C714" s="2">
+        <v>300</v>
+      </c>
+      <c r="D714" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="715" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A715" s="1">
+        <v>45438</v>
+      </c>
+      <c r="B715" t="s">
+        <v>24</v>
+      </c>
+      <c r="C715" s="2">
+        <v>100</v>
+      </c>
+      <c r="D715" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="716" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A716" s="1">
+        <v>45438</v>
+      </c>
+      <c r="B716" t="s">
+        <v>21</v>
+      </c>
+      <c r="C716" s="2">
+        <v>80</v>
+      </c>
+      <c r="D716" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="717" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A717" s="1">
+        <v>45438</v>
+      </c>
+      <c r="B717" t="s">
+        <v>20</v>
+      </c>
+      <c r="C717" s="2">
+        <v>300</v>
+      </c>
+      <c r="D717" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="718" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A718" s="1">
+        <v>45438</v>
+      </c>
+      <c r="B718" t="s">
+        <v>16</v>
+      </c>
+      <c r="C718" s="2">
+        <v>200</v>
+      </c>
+      <c r="D718" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="719" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A719" s="1">
+        <v>45438</v>
+      </c>
+      <c r="B719" t="s">
+        <v>11</v>
+      </c>
+      <c r="C719" s="2">
+        <v>300</v>
+      </c>
+      <c r="D719" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="720" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A720" s="1">
+        <v>45438</v>
+      </c>
+      <c r="B720" t="s">
+        <v>1</v>
+      </c>
+      <c r="C720" s="2">
+        <v>100</v>
+      </c>
+      <c r="D720" t="s">
         <v>34</v>
       </c>
     </row>
@@ -10665,10 +10791,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE6B05F-97B9-4791-8A51-7994BA510F1D}">
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView topLeftCell="A82" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11687,6 +11813,28 @@
       </c>
       <c r="C90" s="4">
         <v>960</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>45417</v>
+      </c>
+      <c r="B91" t="s">
+        <v>74</v>
+      </c>
+      <c r="C91" s="4">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>45438</v>
+      </c>
+      <c r="B92" t="s">
+        <v>62</v>
+      </c>
+      <c r="C92" s="4">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -11820,7 +11968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE771D5-AE0E-9C4B-B862-1B8092D29603}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>